<commit_message>
fix target 11.c without UNSD code and indicator
</commit_message>
<xml_diff>
--- a/SDG_Target_Indicator_UNSD_2023.xlsx
+++ b/SDG_Target_Indicator_UNSD_2023.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G249"/>
+  <dimension ref="A1:G250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6208,38 +6208,30 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Responsible Consumption and Production</t>
+          <t>Sustainable Cities and Communities</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>12.1</t>
+          <t>11.c</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Implement the 10‑Year Framework of Programmes on Sustainable Consumption and Production Patterns, all countries taking action, with developed countries taking the lead, taking into account the development and capabilities of developing countries</t>
-        </is>
-      </c>
-      <c r="E157" t="inlineStr">
-        <is>
-          <t>12.1.1</t>
-        </is>
-      </c>
-      <c r="F157" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Number of countries developing, adopting or implementing policy instruments aimed at supporting the shift to sustainable consumption and production</t>
-        </is>
-      </c>
-      <c r="G157" t="inlineStr">
-        <is>
-          <t>C120101</t>
-        </is>
+          <t xml:space="preserve"> Support least developed countries, including through financial and technical assistance, in building sustainable and resilient buildings utilizing local materials</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>0</v>
+      </c>
+      <c r="F157" t="inlineStr"/>
+      <c r="G157" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -6255,27 +6247,27 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>12.2</t>
+          <t>12.1</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2030, achieve the sustainable management and efficient use of natural resources</t>
+          <t xml:space="preserve"> Implement the 10‑Year Framework of Programmes on Sustainable Consumption and Production Patterns, all countries taking action, with developed countries taking the lead, taking into account the development and capabilities of developing countries</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>12.2.1</t>
+          <t>12.1.1</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Material footprint, material footprint per capita, and material footprint per GDP</t>
+          <t xml:space="preserve"> Number of countries developing, adopting or implementing policy instruments aimed at supporting the shift to sustainable consumption and production</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>C200202</t>
+          <t>C120101</t>
         </is>
       </c>
     </row>
@@ -6302,17 +6294,17 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>12.2.2</t>
+          <t>12.2.1</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Domestic material consumption, domestic material consumption per capita, and domestic material consumption per GDP</t>
+          <t xml:space="preserve"> Material footprint, material footprint per capita, and material footprint per GDP</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>C200203</t>
+          <t>C200202</t>
         </is>
       </c>
     </row>
@@ -6329,27 +6321,27 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>12.3</t>
+          <t>12.2</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2030, halve per capita global food waste at the retail and consumer levels and reduce food losses along production and supply chains, including post-harvest losses</t>
+          <t xml:space="preserve"> By 2030, achieve the sustainable management and efficient use of natural resources</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>12.3.1</t>
+          <t>12.2.2</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (a) Food loss index and (b) food waste index</t>
+          <t xml:space="preserve"> Domestic material consumption, domestic material consumption per capita, and domestic material consumption per GDP</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>C120301</t>
+          <t>C200203</t>
         </is>
       </c>
     </row>
@@ -6366,27 +6358,27 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>12.4</t>
+          <t>12.3</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2020, achieve the environmentally sound management of chemicals and all wastes throughout their life cycle, in accordance with agreed international frameworks, and significantly reduce their release to air, water and soil in order to minimize their adverse impacts on human health and the environment</t>
+          <t xml:space="preserve"> By 2030, halve per capita global food waste at the retail and consumer levels and reduce food losses along production and supply chains, including post-harvest losses</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>12.4.1</t>
+          <t>12.3.1</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of parties to international multilateral environmental agreements on hazardous waste, and other chemicals that meet their commitments and obligations in transmitting information as required by each relevant agreement</t>
+          <t xml:space="preserve"> (a) Food loss index and (b) food waste index</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>C120401</t>
+          <t>C120301</t>
         </is>
       </c>
     </row>
@@ -6413,17 +6405,17 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>12.4.2</t>
+          <t>12.4.1</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (a) Hazardous waste generated per capita; and (b) proportion of hazardous waste treated, by type of treatment</t>
+          <t xml:space="preserve"> Number of parties to international multilateral environmental agreements on hazardous waste, and other chemicals that meet their commitments and obligations in transmitting information as required by each relevant agreement</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>C120402</t>
+          <t>C120401</t>
         </is>
       </c>
     </row>
@@ -6440,27 +6432,27 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>12.5</t>
+          <t>12.4</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2030, substantially reduce waste generation through prevention, reduction, recycling and reuse</t>
+          <t xml:space="preserve"> By 2020, achieve the environmentally sound management of chemicals and all wastes throughout their life cycle, in accordance with agreed international frameworks, and significantly reduce their release to air, water and soil in order to minimize their adverse impacts on human health and the environment</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>12.5.1</t>
+          <t>12.4.2</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t xml:space="preserve"> National recycling rate, tons of material recycled</t>
+          <t xml:space="preserve"> (a) Hazardous waste generated per capita; and (b) proportion of hazardous waste treated, by type of treatment</t>
         </is>
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>C120501</t>
+          <t>C120402</t>
         </is>
       </c>
     </row>
@@ -6477,27 +6469,27 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>12.6</t>
+          <t>12.5</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Encourage companies, especially large and transnational companies, to adopt sustainable practices and to integrate sustainability information into their reporting cycle</t>
+          <t xml:space="preserve"> By 2030, substantially reduce waste generation through prevention, reduction, recycling and reuse</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>12.6.1</t>
+          <t>12.5.1</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of companies publishing sustainability reports</t>
+          <t xml:space="preserve"> National recycling rate, tons of material recycled</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>C120601</t>
+          <t>C120501</t>
         </is>
       </c>
     </row>
@@ -6514,27 +6506,27 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>12.7</t>
+          <t>12.6</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Promote public procurement practices that are sustainable, in accordance with national policies and priorities</t>
+          <t xml:space="preserve"> Encourage companies, especially large and transnational companies, to adopt sustainable practices and to integrate sustainability information into their reporting cycle</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>12.7.1</t>
+          <t>12.6.1</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries implementing sustainable public procurement policies and action plans</t>
+          <t xml:space="preserve"> Number of companies publishing sustainability reports</t>
         </is>
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>C120702</t>
+          <t>C120601</t>
         </is>
       </c>
     </row>
@@ -6551,27 +6543,27 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>12.8</t>
+          <t>12.7</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2030, ensure that people everywhere have the relevant information and awareness for sustainable development and lifestyles in harmony with nature</t>
+          <t xml:space="preserve"> Promote public procurement practices that are sustainable, in accordance with national policies and priorities</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>12.8.1</t>
+          <t>12.7.1</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Extent to which (i) global citizenship education and (ii) education for sustainable development are mainstreamed in (a) national education policies; (b) curricula; (c) teacher education; and (d) student assessment</t>
+          <t xml:space="preserve"> Number of countries implementing sustainable public procurement policies and action plans</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>C200306</t>
+          <t>C120702</t>
         </is>
       </c>
     </row>
@@ -6588,27 +6580,27 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>12.a</t>
+          <t>12.8</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Support developing countries to strengthen their scientific and technological capacity to move towards more sustainable patterns of consumption and production</t>
+          <t xml:space="preserve"> By 2030, ensure that people everywhere have the relevant information and awareness for sustainable development and lifestyles in harmony with nature</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>12.a.1</t>
+          <t>12.8.1</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Installed renewable energy-generating capacity in developing countries (in watts per capita)</t>
+          <t xml:space="preserve"> Extent to which (i) global citizenship education and (ii) education for sustainable development are mainstreamed in (a) national education policies; (b) curricula; (c) teacher education; and (d) student assessment</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>C200208</t>
+          <t>C200306</t>
         </is>
       </c>
     </row>
@@ -6625,27 +6617,27 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>12.b</t>
+          <t>12.a</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Develop and implement tools to monitor sustainable development impacts for sustainable tourism that creates jobs and promotes local culture and products</t>
+          <t xml:space="preserve"> Support developing countries to strengthen their scientific and technological capacity to move towards more sustainable patterns of consumption and production</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>12.b.1</t>
+          <t>12.a.1</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Implementation of standard accounting tools to monitor the economic and environmental aspects of tourism sustainability</t>
+          <t xml:space="preserve"> Installed renewable energy-generating capacity in developing countries (in watts per capita)</t>
         </is>
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>C120b02</t>
+          <t>C200208</t>
         </is>
       </c>
     </row>
@@ -6662,64 +6654,64 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>12.c</t>
+          <t>12.b</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Rationalize inefficient fossil-fuel subsidies that encourage wasteful consumption by removing market distortions, in accordance with national circumstances, including by restructuring taxation and phasing out those harmful subsidies, where they exist, to reflect their environmental impacts, taking fully into account the specific needs and conditions of developing countries and minimizing the possible adverse impacts on their development in a manner that protects the poor and the affected communities</t>
+          <t xml:space="preserve"> Develop and implement tools to monitor sustainable development impacts for sustainable tourism that creates jobs and promotes local culture and products</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>12.c.1</t>
+          <t>12.b.1</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Amount of fossil-fuel subsidies (production and consumption) per unit of GDP</t>
+          <t xml:space="preserve"> Implementation of standard accounting tools to monitor the economic and environmental aspects of tourism sustainability</t>
         </is>
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>C120c01</t>
+          <t>C120b02</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Climate Action</t>
+          <t>Responsible Consumption and Production</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>13.1</t>
+          <t>12.c</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Strengthen resilience and adaptive capacity to climate-related hazards and natural disasters in all countries</t>
+          <t xml:space="preserve"> Rationalize inefficient fossil-fuel subsidies that encourage wasteful consumption by removing market distortions, in accordance with national circumstances, including by restructuring taxation and phasing out those harmful subsidies, where they exist, to reflect their environmental impacts, taking fully into account the specific needs and conditions of developing countries and minimizing the possible adverse impacts on their development in a manner that protects the poor and the affected communities</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>13.1.1</t>
+          <t>12.c.1</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of deaths, missing persons and directly affected persons attributed to disasters per 100,000 population</t>
+          <t xml:space="preserve"> Amount of fossil-fuel subsidies (production and consumption) per unit of GDP</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>C200303</t>
+          <t>C120c01</t>
         </is>
       </c>
     </row>
@@ -6746,17 +6738,17 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>13.1.2</t>
+          <t>13.1.1</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries that adopt and implement national disaster risk reduction strategies in line with the Sendai Framework for Disaster Risk Reduction 2015–2030</t>
+          <t xml:space="preserve"> Number of deaths, missing persons and directly affected persons attributed to disasters per 100,000 population</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>C200304</t>
+          <t>C200303</t>
         </is>
       </c>
     </row>
@@ -6783,17 +6775,17 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>13.1.3</t>
+          <t>13.1.2</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of local governments that adopt and implement local disaster risk reduction strategies in line with national disaster risk reduction strategies</t>
+          <t xml:space="preserve"> Number of countries that adopt and implement national disaster risk reduction strategies in line with the Sendai Framework for Disaster Risk Reduction 2015–2030</t>
         </is>
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>C200305</t>
+          <t>C200304</t>
         </is>
       </c>
     </row>
@@ -6810,27 +6802,27 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>13.1</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Integrate climate change measures into national policies, strategies and planning</t>
+          <t xml:space="preserve"> Strengthen resilience and adaptive capacity to climate-related hazards and natural disasters in all countries</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>13.2.1</t>
+          <t>13.1.3</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries with nationally determined contributions, long-term strategies, national adaptation plans and adaptation communications, as reported to the secretariat of the United Nations Framework Convention on Climate Change</t>
+          <t xml:space="preserve"> Proportion of local governments that adopt and implement local disaster risk reduction strategies in line with national disaster risk reduction strategies</t>
         </is>
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>C130203</t>
+          <t>C200305</t>
         </is>
       </c>
     </row>
@@ -6857,17 +6849,17 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>13.2.2</t>
+          <t>13.2.1</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Total greenhouse gas emissions per year</t>
+          <t xml:space="preserve"> Number of countries with nationally determined contributions, long-term strategies, national adaptation plans and adaptation communications, as reported to the secretariat of the United Nations Framework Convention on Climate Change</t>
         </is>
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>C130202</t>
+          <t>C130203</t>
         </is>
       </c>
     </row>
@@ -6884,27 +6876,27 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>13.3</t>
+          <t>13.2</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Improve education, awareness-raising and human and institutional capacity on climate change mitigation, adaptation, impact reduction and early warning</t>
+          <t xml:space="preserve"> Integrate climate change measures into national policies, strategies and planning</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>13.3.1</t>
+          <t>13.2.2</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Extent to which (i) global citizenship education and (ii) education for sustainable development are mainstreamed in (a) national education policies; (b) curricula; (c) teacher education; and (d) student assessment</t>
+          <t xml:space="preserve"> Total greenhouse gas emissions per year</t>
         </is>
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>C200306</t>
+          <t>C130202</t>
         </is>
       </c>
     </row>
@@ -6921,27 +6913,27 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>13.a</t>
+          <t>13.3</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Implement the commitment undertaken by developed-country parties to the United Nations Framework Convention on Climate Change to a goal of mobilizing jointly $100 billion annually by 2020 from all sources to address the needs of developing countries in the context of meaningful mitigation actions and transparency on implementation and fully operationalize the Green Climate Fund through its capitalization as soon as possible</t>
+          <t xml:space="preserve"> Improve education, awareness-raising and human and institutional capacity on climate change mitigation, adaptation, impact reduction and early warning</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>13.a.1</t>
+          <t>13.3.1</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Amounts provided and mobilized in United States dollars per year in relation to the continued existing collective mobilization goal of the $100 billion commitment through to 2025</t>
+          <t xml:space="preserve"> Extent to which (i) global citizenship education and (ii) education for sustainable development are mainstreamed in (a) national education policies; (b) curricula; (c) teacher education; and (d) student assessment</t>
         </is>
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>C130a02</t>
+          <t>C200306</t>
         </is>
       </c>
     </row>
@@ -6958,64 +6950,64 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>13.b</t>
+          <t>13.a</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Promote mechanisms for raising capacity for effective climate change-related planning and management in least developed countries and small island developing States, including focusing on women, youth and local and marginalized communities</t>
+          <t xml:space="preserve"> Implement the commitment undertaken by developed-country parties to the United Nations Framework Convention on Climate Change to a goal of mobilizing jointly $100 billion annually by 2020 from all sources to address the needs of developing countries in the context of meaningful mitigation actions and transparency on implementation and fully operationalize the Green Climate Fund through its capitalization as soon as possible</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>13.b.1</t>
+          <t>13.a.1</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of least developed countries and small island developing States with nationally determined contributions, long-term strategies, national adaptation plans and adaptation communications, as reported to the secretariat of the United Nations Framework Convention on Climate Change</t>
+          <t xml:space="preserve"> Amounts provided and mobilized in United States dollars per year in relation to the continued existing collective mobilization goal of the $100 billion commitment through to 2025</t>
         </is>
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>C130b02</t>
+          <t>C130a02</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Life Below Water</t>
+          <t>Climate Action</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>14.1</t>
+          <t>13.b</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2025, prevent and significantly reduce marine pollution of all kinds, in particular from land-based activities, including marine debris and nutrient pollution</t>
+          <t xml:space="preserve"> Promote mechanisms for raising capacity for effective climate change-related planning and management in least developed countries and small island developing States, including focusing on women, youth and local and marginalized communities</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>14.1.1</t>
+          <t>13.b.1</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (a) Index of coastal eutrophication; and (b) plastic debris density</t>
+          <t xml:space="preserve"> Number of least developed countries and small island developing States with nationally determined contributions, long-term strategies, national adaptation plans and adaptation communications, as reported to the secretariat of the United Nations Framework Convention on Climate Change</t>
         </is>
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>C140101</t>
+          <t>C130b02</t>
         </is>
       </c>
     </row>
@@ -7032,27 +7024,27 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>14.2</t>
+          <t>14.1</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2020, sustainably manage and protect marine and coastal ecosystems to avoid significant adverse impacts, including by strengthening their resilience, and take action for their restoration in order to achieve healthy and productive oceans</t>
+          <t xml:space="preserve"> By 2025, prevent and significantly reduce marine pollution of all kinds, in particular from land-based activities, including marine debris and nutrient pollution</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>14.2.1</t>
+          <t>14.1.1</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries using ecosystem-based approaches to managing marine areas</t>
+          <t xml:space="preserve"> (a) Index of coastal eutrophication; and (b) plastic debris density</t>
         </is>
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>C140201</t>
+          <t>C140101</t>
         </is>
       </c>
     </row>
@@ -7069,27 +7061,27 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>14.3</t>
+          <t>14.2</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Minimize and address the impacts of ocean acidification, including through enhanced scientific cooperation at all levels</t>
+          <t xml:space="preserve"> By 2020, sustainably manage and protect marine and coastal ecosystems to avoid significant adverse impacts, including by strengthening their resilience, and take action for their restoration in order to achieve healthy and productive oceans</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>14.3.1</t>
+          <t>14.2.1</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Average marine acidity (pH) measured at agreed suite of representative sampling stations</t>
+          <t xml:space="preserve"> Number of countries using ecosystem-based approaches to managing marine areas</t>
         </is>
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>C140301</t>
+          <t>C140201</t>
         </is>
       </c>
     </row>
@@ -7106,27 +7098,27 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>14.4</t>
+          <t>14.3</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2020, effectively regulate harvesting and end overfishing, illegal, unreported and unregulated fishing and destructive fishing practices and implement science-based management plans, in order to restore fish stocks in the shortest time feasible, at least to levels that can produce maximum sustainable yield as determined by their biological characteristics</t>
+          <t xml:space="preserve"> Minimize and address the impacts of ocean acidification, including through enhanced scientific cooperation at all levels</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>14.4.1</t>
+          <t>14.3.1</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of fish stocks within biologically sustainable levels</t>
+          <t xml:space="preserve"> Average marine acidity (pH) measured at agreed suite of representative sampling stations</t>
         </is>
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>C140401</t>
+          <t>C140301</t>
         </is>
       </c>
     </row>
@@ -7143,27 +7135,27 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>14.5</t>
+          <t>14.4</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2020, conserve at least 10 per cent of coastal and marine areas, consistent with national and international law and based on the best available scientific information</t>
+          <t xml:space="preserve"> By 2020, effectively regulate harvesting and end overfishing, illegal, unreported and unregulated fishing and destructive fishing practices and implement science-based management plans, in order to restore fish stocks in the shortest time feasible, at least to levels that can produce maximum sustainable yield as determined by their biological characteristics</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>14.5.1</t>
+          <t>14.4.1</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Coverage of protected areas in relation to marine areas</t>
+          <t xml:space="preserve"> Proportion of fish stocks within biologically sustainable levels</t>
         </is>
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>C140501</t>
+          <t>C140401</t>
         </is>
       </c>
     </row>
@@ -7180,27 +7172,27 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>14.6</t>
+          <t>14.5</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2020, prohibit certain forms of fisheries subsidies which contribute to overcapacity and overfishing, eliminate subsidies that contribute to illegal, unreported and unregulated fishing and refrain from introducing new such subsidies, recognizing that appropriate and effective special and differential treatment for developing and least developed countries should be an integral part of the World Trade Organization fisheries subsidies negotiation4</t>
+          <t xml:space="preserve"> By 2020, conserve at least 10 per cent of coastal and marine areas, consistent with national and international law and based on the best available scientific information</t>
         </is>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>14.6.1</t>
+          <t>14.5.1</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Degree of implementation of international instruments aiming to combat illegal, unreported and unregulated fishing</t>
+          <t xml:space="preserve"> Coverage of protected areas in relation to marine areas</t>
         </is>
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>C140601</t>
+          <t>C140501</t>
         </is>
       </c>
     </row>
@@ -7217,27 +7209,27 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>14.7</t>
+          <t>14.6</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2030, increase the economic benefits to small island developing States and least developed countries from the sustainable use of marine resources, including through sustainable management of fisheries, aquaculture and tourism</t>
+          <t xml:space="preserve"> By 2020, prohibit certain forms of fisheries subsidies which contribute to overcapacity and overfishing, eliminate subsidies that contribute to illegal, unreported and unregulated fishing and refrain from introducing new such subsidies, recognizing that appropriate and effective special and differential treatment for developing and least developed countries should be an integral part of the World Trade Organization fisheries subsidies negotiation4</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>14.7.1</t>
+          <t>14.6.1</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Sustainable fisheries as a proportion of GDP in small island developing States, least developed countries and all countries</t>
+          <t xml:space="preserve"> Degree of implementation of international instruments aiming to combat illegal, unreported and unregulated fishing</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>C140701</t>
+          <t>C140601</t>
         </is>
       </c>
     </row>
@@ -7254,27 +7246,27 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>14.a</t>
+          <t>14.7</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Increase scientific knowledge, develop research capacity and transfer marine technology, taking into account the Intergovernmental Oceanographic Commission Criteria and Guidelines on the Transfer of Marine Technology, in order to improve ocean health and to enhance the contribution of marine biodiversity to the development of developing countries, in particular small island developing States and least developed countries</t>
+          <t xml:space="preserve"> By 2030, increase the economic benefits to small island developing States and least developed countries from the sustainable use of marine resources, including through sustainable management of fisheries, aquaculture and tourism</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>14.a.1</t>
+          <t>14.7.1</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of total research budget allocated to research in the field of marine technology</t>
+          <t xml:space="preserve"> Sustainable fisheries as a proportion of GDP in small island developing States, least developed countries and all countries</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>C140a01</t>
+          <t>C140701</t>
         </is>
       </c>
     </row>
@@ -7291,27 +7283,27 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>14.b</t>
+          <t>14.a</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Provide access for small-scale artisanal fishers to marine resources and markets</t>
+          <t xml:space="preserve"> Increase scientific knowledge, develop research capacity and transfer marine technology, taking into account the Intergovernmental Oceanographic Commission Criteria and Guidelines on the Transfer of Marine Technology, in order to improve ocean health and to enhance the contribution of marine biodiversity to the development of developing countries, in particular small island developing States and least developed countries</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>14.b.1</t>
+          <t>14.a.1</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Degree of application of a legal/regulatory/ policy/institutional framework which recognizes and protects access rights for small-scale fisheries</t>
+          <t xml:space="preserve"> Proportion of total research budget allocated to research in the field of marine technology</t>
         </is>
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>C140b01</t>
+          <t>C140a01</t>
         </is>
       </c>
     </row>
@@ -7328,64 +7320,64 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>14.c</t>
+          <t>14.b</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Enhance the conservation and sustainable use of oceans and their resources by implementing international law as reflected in the United Nations Convention on the Law of the Sea, which provides the legal framework for the conservation and sustainable use of oceans and their resources, as recalled in paragraph 158 of “The future we want”</t>
+          <t xml:space="preserve"> Provide access for small-scale artisanal fishers to marine resources and markets</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>14.c.1</t>
+          <t>14.b.1</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries making progress in ratifying, accepting and implementing through legal, policy and institutional frameworks, ocean-related instruments that implement international law, as reflected in the United Nations Convention on the Law of the Sea, for the conservation and sustainable use of the oceans and their resources</t>
+          <t xml:space="preserve"> Degree of application of a legal/regulatory/ policy/institutional framework which recognizes and protects access rights for small-scale fisheries</t>
         </is>
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>C140c01</t>
+          <t>C140b01</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Life on Land</t>
+          <t>Life Below Water</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>15.1</t>
+          <t>14.c</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2020, ensure the conservation, restoration and sustainable use of terrestrial and inland freshwater ecosystems and their services, in particular forests, wetlands, mountains and drylands, in line with obligations under international agreements</t>
+          <t xml:space="preserve"> Enhance the conservation and sustainable use of oceans and their resources by implementing international law as reflected in the United Nations Convention on the Law of the Sea, which provides the legal framework for the conservation and sustainable use of oceans and their resources, as recalled in paragraph 158 of “The future we want”</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>15.1.1</t>
+          <t>14.c.1</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Forest area as a proportion of total land area</t>
+          <t xml:space="preserve"> Number of countries making progress in ratifying, accepting and implementing through legal, policy and institutional frameworks, ocean-related instruments that implement international law, as reflected in the United Nations Convention on the Law of the Sea, for the conservation and sustainable use of the oceans and their resources</t>
         </is>
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>C150101</t>
+          <t>C140c01</t>
         </is>
       </c>
     </row>
@@ -7412,17 +7404,17 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>15.1.2</t>
+          <t>15.1.1</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of important sites for terrestrial and freshwater biodiversity that are covered by protected areas, by ecosystem type</t>
+          <t xml:space="preserve"> Forest area as a proportion of total land area</t>
         </is>
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>C150102</t>
+          <t>C150101</t>
         </is>
       </c>
     </row>
@@ -7439,27 +7431,27 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>15.2</t>
+          <t>15.1</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2020, promote the implementation of sustainable management of all types of forests, halt deforestation, restore degraded forests and substantially increase afforestation and reforestation globally</t>
+          <t xml:space="preserve"> By 2020, ensure the conservation, restoration and sustainable use of terrestrial and inland freshwater ecosystems and their services, in particular forests, wetlands, mountains and drylands, in line with obligations under international agreements</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>15.2.1</t>
+          <t>15.1.2</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Progress towards sustainable forest management</t>
+          <t xml:space="preserve"> Proportion of important sites for terrestrial and freshwater biodiversity that are covered by protected areas, by ecosystem type</t>
         </is>
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>C150201</t>
+          <t>C150102</t>
         </is>
       </c>
     </row>
@@ -7476,27 +7468,27 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>15.3</t>
+          <t>15.2</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2030, combat desertification, restore degraded land and soil, including land affected by desertification, drought and floods, and strive to achieve a land degradation-neutral world</t>
+          <t xml:space="preserve"> By 2020, promote the implementation of sustainable management of all types of forests, halt deforestation, restore degraded forests and substantially increase afforestation and reforestation globally</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>15.3.1</t>
+          <t>15.2.1</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of land that is degraded over total land area</t>
+          <t xml:space="preserve"> Progress towards sustainable forest management</t>
         </is>
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>C150301</t>
+          <t>C150201</t>
         </is>
       </c>
     </row>
@@ -7513,27 +7505,27 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>15.4</t>
+          <t>15.3</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2030, ensure the conservation of mountain ecosystems, including their biodiversity, in order to enhance their capacity to provide benefits that are essential for sustainable development</t>
+          <t xml:space="preserve"> By 2030, combat desertification, restore degraded land and soil, including land affected by desertification, drought and floods, and strive to achieve a land degradation-neutral world</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>15.4.1</t>
+          <t>15.3.1</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Coverage by protected areas of important sites for mountain biodiversity</t>
+          <t xml:space="preserve"> Proportion of land that is degraded over total land area</t>
         </is>
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>C150401</t>
+          <t>C150301</t>
         </is>
       </c>
     </row>
@@ -7560,17 +7552,17 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>15.4.2</t>
+          <t>15.4.1</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (a) Mountain Green Cover Index and (b) proportion of degraded mountain land</t>
+          <t xml:space="preserve"> Coverage by protected areas of important sites for mountain biodiversity</t>
         </is>
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>C150402</t>
+          <t>C150401</t>
         </is>
       </c>
     </row>
@@ -7587,27 +7579,27 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>15.5</t>
+          <t>15.4</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Take urgent and significant action to reduce the degradation of natural habitats, halt the loss of biodiversity and, by 2020, protect and prevent the extinction of threatened species</t>
+          <t xml:space="preserve"> By 2030, ensure the conservation of mountain ecosystems, including their biodiversity, in order to enhance their capacity to provide benefits that are essential for sustainable development</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>15.5.1</t>
+          <t>15.4.2</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Red List Index</t>
+          <t xml:space="preserve"> (a) Mountain Green Cover Index and (b) proportion of degraded mountain land</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>C150501</t>
+          <t>C150402</t>
         </is>
       </c>
     </row>
@@ -7624,27 +7616,27 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>15.6</t>
+          <t>15.5</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Promote fair and equitable sharing of the benefits arising from the utilization of genetic resources and promote appropriate access to such resources, as internationally agreed</t>
+          <t xml:space="preserve"> Take urgent and significant action to reduce the degradation of natural habitats, halt the loss of biodiversity and, by 2020, protect and prevent the extinction of threatened species</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>15.6.1</t>
+          <t>15.5.1</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries that have adopted legislative, administrative and policy frameworks to ensure fair and equitable sharing of benefits</t>
+          <t xml:space="preserve"> Red List Index</t>
         </is>
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>C150601</t>
+          <t>C150501</t>
         </is>
       </c>
     </row>
@@ -7661,27 +7653,27 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>15.7</t>
+          <t>15.6</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Take urgent action to end poaching and trafficking of protected species of flora and fauna and address both demand and supply of illegal wildlife products</t>
+          <t xml:space="preserve"> Promote fair and equitable sharing of the benefits arising from the utilization of genetic resources and promote appropriate access to such resources, as internationally agreed</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>15.7.1</t>
+          <t>15.6.1</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of traded wildlife that was poached or illicitly trafficked</t>
+          <t xml:space="preserve"> Number of countries that have adopted legislative, administrative and policy frameworks to ensure fair and equitable sharing of benefits</t>
         </is>
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>C200206</t>
+          <t>C150601</t>
         </is>
       </c>
     </row>
@@ -7698,27 +7690,27 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>15.8</t>
+          <t>15.7</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2020, introduce measures to prevent the introduction and significantly reduce the impact of invasive alien species on land and water ecosystems and control or eradicate the priority species</t>
+          <t xml:space="preserve"> Take urgent action to end poaching and trafficking of protected species of flora and fauna and address both demand and supply of illegal wildlife products</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>15.8.1</t>
+          <t>15.7.1</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of countries adopting relevant national legislation and adequately resourcing the prevention or control of invasive alien species</t>
+          <t xml:space="preserve"> Proportion of traded wildlife that was poached or illicitly trafficked</t>
         </is>
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>C150801</t>
+          <t>C200206</t>
         </is>
       </c>
     </row>
@@ -7735,27 +7727,27 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>15.9</t>
+          <t>15.8</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2020, integrate ecosystem and biodiversity values into national and local planning, development processes, poverty reduction strategies and accounts</t>
+          <t xml:space="preserve"> By 2020, introduce measures to prevent the introduction and significantly reduce the impact of invasive alien species on land and water ecosystems and control or eradicate the priority species</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>15.9.1</t>
+          <t>15.8.1</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (a) Number of countries that have established national targets in accordance with or similar to Aichi Biodiversity Target 2 of the Strategic Plan for Biodiversity 2011–2020 in their national biodiversity strategy and action plans and the progress reported towards these targets; and (b) integration of biodiversity into national accounting and reporting systems, defined as implementation of the System of Environmental-Economic Accounting</t>
+          <t xml:space="preserve"> Proportion of countries adopting relevant national legislation and adequately resourcing the prevention or control of invasive alien species</t>
         </is>
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>C150902</t>
+          <t>C150801</t>
         </is>
       </c>
     </row>
@@ -7772,27 +7764,27 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>15.a</t>
+          <t>15.9</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mobilize and significantly increase financial resources from all sources to conserve and sustainably use biodiversity and ecosystems</t>
+          <t xml:space="preserve"> By 2020, integrate ecosystem and biodiversity values into national and local planning, development processes, poverty reduction strategies and accounts</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>15.a.1</t>
+          <t>15.9.1</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (a) Official development assistance on conservation and sustainable use of biodiversity; and (b) revenue generated and finance mobilized from biodiversity-relevant economic instruments</t>
+          <t xml:space="preserve"> (a) Number of countries that have established national targets in accordance with or similar to Aichi Biodiversity Target 2 of the Strategic Plan for Biodiversity 2011–2020 in their national biodiversity strategy and action plans and the progress reported towards these targets; and (b) integration of biodiversity into national accounting and reporting systems, defined as implementation of the System of Environmental-Economic Accounting</t>
         </is>
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>C200210</t>
+          <t>C150902</t>
         </is>
       </c>
     </row>
@@ -7809,17 +7801,17 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>15.b</t>
+          <t>15.a</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mobilize significant resources from all sources and at all levels to finance sustainable forest management and provide adequate incentives to developing countries to advance such management, including for conservation and reforestation</t>
+          <t xml:space="preserve"> Mobilize and significantly increase financial resources from all sources to conserve and sustainably use biodiversity and ecosystems</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>15.b.1</t>
+          <t>15.a.1</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -7846,64 +7838,64 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>15.c</t>
+          <t>15.b</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Enhance global support for efforts to combat poaching and trafficking of protected species, including by increasing the capacity of local communities to pursue sustainable livelihood opportunities</t>
+          <t xml:space="preserve"> Mobilize significant resources from all sources and at all levels to finance sustainable forest management and provide adequate incentives to developing countries to advance such management, including for conservation and reforestation</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>15.c.1</t>
+          <t>15.b.1</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of traded wildlife that was poached or illicitly trafficked</t>
+          <t xml:space="preserve"> (a) Official development assistance on conservation and sustainable use of biodiversity; and (b) revenue generated and finance mobilized from biodiversity-relevant economic instruments</t>
         </is>
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>C200206</t>
+          <t>C200210</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>15</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Peace, Justice, and Strong Institutions</t>
+          <t>Life on Land</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>16.1</t>
+          <t>15.c</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Significantly reduce all forms of violence and related death rates everywhere</t>
+          <t xml:space="preserve"> Enhance global support for efforts to combat poaching and trafficking of protected species, including by increasing the capacity of local communities to pursue sustainable livelihood opportunities</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>16.1.1</t>
+          <t>15.c.1</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of victims of intentional homicide per 100,000 population, by sex and age</t>
+          <t xml:space="preserve"> Proportion of traded wildlife that was poached or illicitly trafficked</t>
         </is>
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>C160101</t>
+          <t>C200206</t>
         </is>
       </c>
     </row>
@@ -7930,17 +7922,17 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>16.1.2</t>
+          <t>16.1.1</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Conflict-related deaths per 100,000 population, by sex, age and cause</t>
+          <t xml:space="preserve"> Number of victims of intentional homicide per 100,000 population, by sex and age</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>C160102</t>
+          <t>C160101</t>
         </is>
       </c>
     </row>
@@ -7967,17 +7959,17 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>16.1.3</t>
+          <t>16.1.2</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of population subjected to (a) physical violence, (b) psychological violence and (c) sexual violence in the previous 12 months</t>
+          <t xml:space="preserve"> Conflict-related deaths per 100,000 population, by sex, age and cause</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>C160103</t>
+          <t>C160102</t>
         </is>
       </c>
     </row>
@@ -8004,17 +7996,17 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>16.1.4</t>
+          <t>16.1.3</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of population that feel safe walking alone around the area they live after dark</t>
+          <t xml:space="preserve"> Proportion of population subjected to (a) physical violence, (b) psychological violence and (c) sexual violence in the previous 12 months</t>
         </is>
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>C160105</t>
+          <t>C160103</t>
         </is>
       </c>
     </row>
@@ -8031,27 +8023,27 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>16.1</t>
         </is>
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t xml:space="preserve"> End abuse, exploitation, trafficking and all forms of violence against and torture of children</t>
+          <t xml:space="preserve"> Significantly reduce all forms of violence and related death rates everywhere</t>
         </is>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>16.2.1</t>
+          <t>16.1.4</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of children aged 1–17 years who experienced any physical punishment and/or psychological aggression by caregivers in the past month</t>
+          <t xml:space="preserve"> Proportion of population that feel safe walking alone around the area they live after dark</t>
         </is>
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>C160201</t>
+          <t>C160105</t>
         </is>
       </c>
     </row>
@@ -8078,17 +8070,17 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>16.2.2</t>
+          <t>16.2.1</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of victims of human trafficking per 100,000 population, by sex, age and form of exploitation</t>
+          <t xml:space="preserve"> Proportion of children aged 1–17 years who experienced any physical punishment and/or psychological aggression by caregivers in the past month</t>
         </is>
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>C160202</t>
+          <t>C160201</t>
         </is>
       </c>
     </row>
@@ -8115,17 +8107,17 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>16.2.3</t>
+          <t>16.2.2</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of young women and men aged 18–29 years who experienced sexual violence by age 18</t>
+          <t xml:space="preserve"> Number of victims of human trafficking per 100,000 population, by sex, age and form of exploitation</t>
         </is>
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>C160203</t>
+          <t>C160202</t>
         </is>
       </c>
     </row>
@@ -8142,27 +8134,27 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>16.3</t>
+          <t>16.2</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Promote the rule of law at the national and international levels and ensure equal access to justice for all</t>
+          <t xml:space="preserve"> End abuse, exploitation, trafficking and all forms of violence against and torture of children</t>
         </is>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>16.3.1</t>
+          <t>16.2.3</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of victims of violence in the previous 12 months who reported their victimization to competent authorities or other officially recognized conflict resolution mechanisms</t>
+          <t xml:space="preserve"> Proportion of young women and men aged 18–29 years who experienced sexual violence by age 18</t>
         </is>
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>C160301</t>
+          <t>C160203</t>
         </is>
       </c>
     </row>
@@ -8189,17 +8181,17 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>16.3.2</t>
+          <t>16.3.1</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Unsentenced detainees as a proportion of overall prison population</t>
+          <t xml:space="preserve"> Proportion of victims of violence in the previous 12 months who reported their victimization to competent authorities or other officially recognized conflict resolution mechanisms</t>
         </is>
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>C160302</t>
+          <t>C160301</t>
         </is>
       </c>
     </row>
@@ -8226,17 +8218,17 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>16.3.3</t>
+          <t>16.3.2</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of the population who have experienced a dispute in the past two years and who accessed a formal or informal dispute resolution mechanism, by type of mechanism</t>
+          <t xml:space="preserve"> Unsentenced detainees as a proportion of overall prison population</t>
         </is>
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>C160303</t>
+          <t>C160302</t>
         </is>
       </c>
     </row>
@@ -8253,27 +8245,27 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>16.4</t>
+          <t>16.3</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2030, significantly reduce illicit financial and arms flows, strengthen the recovery and return of stolen assets and combat all forms of organized crime</t>
+          <t xml:space="preserve"> Promote the rule of law at the national and international levels and ensure equal access to justice for all</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>16.4.1</t>
+          <t>16.3.3</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Total value of inward and outward illicit financial flows (in current United States dollars)</t>
+          <t xml:space="preserve"> Proportion of the population who have experienced a dispute in the past two years and who accessed a formal or informal dispute resolution mechanism, by type of mechanism</t>
         </is>
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>C160401</t>
+          <t>C160303</t>
         </is>
       </c>
     </row>
@@ -8300,17 +8292,17 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>16.4.2</t>
+          <t>16.4.1</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of seized, found or surrendered arms whose illicit origin or context has been traced or established by a competent authority in line with international instruments</t>
+          <t xml:space="preserve"> Total value of inward and outward illicit financial flows (in current United States dollars)</t>
         </is>
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>C160402</t>
+          <t>C160401</t>
         </is>
       </c>
     </row>
@@ -8327,27 +8319,27 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>16.5</t>
+          <t>16.4</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Substantially reduce corruption and bribery in all their forms</t>
+          <t xml:space="preserve"> By 2030, significantly reduce illicit financial and arms flows, strengthen the recovery and return of stolen assets and combat all forms of organized crime</t>
         </is>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>16.5.1</t>
+          <t>16.4.2</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of persons who had at least one contact with a public official and who paid a bribe to a public official, or were asked for a bribe by those public officials, during the previous 12 months</t>
+          <t xml:space="preserve"> Proportion of seized, found or surrendered arms whose illicit origin or context has been traced or established by a competent authority in line with international instruments</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>C160501</t>
+          <t>C160402</t>
         </is>
       </c>
     </row>
@@ -8374,17 +8366,17 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>16.5.2</t>
+          <t>16.5.1</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of businesses that had at least one contact with a public official and that paid a bribe to a public official, or were asked for a bribe by those public officials during the previous 12 months</t>
+          <t xml:space="preserve"> Proportion of persons who had at least one contact with a public official and who paid a bribe to a public official, or were asked for a bribe by those public officials, during the previous 12 months</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>C160502</t>
+          <t>C160501</t>
         </is>
       </c>
     </row>
@@ -8401,27 +8393,27 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>16.5</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Develop effective, accountable and transparent institutions at all levels</t>
+          <t xml:space="preserve"> Substantially reduce corruption and bribery in all their forms</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>16.6.1</t>
+          <t>16.5.2</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Primary government expenditures as a proportion of original approved budget, by sector (or by budget codes or similar)</t>
+          <t xml:space="preserve"> Proportion of businesses that had at least one contact with a public official and that paid a bribe to a public official, or were asked for a bribe by those public officials during the previous 12 months</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>C160601</t>
+          <t>C160502</t>
         </is>
       </c>
     </row>
@@ -8448,17 +8440,17 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>16.6.2</t>
+          <t>16.6.1</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of population satisfied with their last experience of public services</t>
+          <t xml:space="preserve"> Primary government expenditures as a proportion of original approved budget, by sector (or by budget codes or similar)</t>
         </is>
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>C160602</t>
+          <t>C160601</t>
         </is>
       </c>
     </row>
@@ -8475,27 +8467,27 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>16.7</t>
+          <t>16.6</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ensure responsive, inclusive, participatory and representative decision-making at all levels</t>
+          <t xml:space="preserve"> Develop effective, accountable and transparent institutions at all levels</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>16.7.1</t>
+          <t>16.6.2</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportions of positions in national and local institutions, including (a) the legislatures; (b) the public service; and (c) the judiciary, compared to national distributions, by sex, age, persons with disabilities and population groups</t>
+          <t xml:space="preserve"> Proportion of population satisfied with their last experience of public services</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>C160701</t>
+          <t>C160602</t>
         </is>
       </c>
     </row>
@@ -8522,17 +8514,17 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>16.7.2</t>
+          <t>16.7.1</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of population who believe decision-making is inclusive and responsive, by sex, age, disability and population group</t>
+          <t xml:space="preserve"> Proportions of positions in national and local institutions, including (a) the legislatures; (b) the public service; and (c) the judiciary, compared to national distributions, by sex, age, persons with disabilities and population groups</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>C160702</t>
+          <t>C160701</t>
         </is>
       </c>
     </row>
@@ -8549,27 +8541,27 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>16.8</t>
+          <t>16.7</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Broaden and strengthen the participation of developing countries in the institutions of global governance</t>
+          <t xml:space="preserve"> Ensure responsive, inclusive, participatory and representative decision-making at all levels</t>
         </is>
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>16.8.1</t>
+          <t>16.7.2</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of members and voting rights of developing countries in international organizations</t>
+          <t xml:space="preserve"> Proportion of population who believe decision-making is inclusive and responsive, by sex, age, disability and population group</t>
         </is>
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>C200205</t>
+          <t>C160702</t>
         </is>
       </c>
     </row>
@@ -8586,27 +8578,27 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>16.9</t>
+          <t>16.8</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2030, provide legal identity for all, including birth registration</t>
+          <t xml:space="preserve"> Broaden and strengthen the participation of developing countries in the institutions of global governance</t>
         </is>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>16.9.1</t>
+          <t>16.8.1</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of children under 5 years of age whose births have been registered with a civil authority, by age</t>
+          <t xml:space="preserve"> Proportion of members and voting rights of developing countries in international organizations</t>
         </is>
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>C160901</t>
+          <t>C200205</t>
         </is>
       </c>
     </row>
@@ -8623,27 +8615,27 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>16.10</t>
+          <t>16.9</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ensure public access to information and protect fundamental freedoms, in accordance with national legislation and international agreements</t>
+          <t xml:space="preserve"> By 2030, provide legal identity for all, including birth registration</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>16.10.1</t>
+          <t>16.9.1</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of verified cases of killing, kidnapping, enforced disappearance, arbitrary detention and torture of journalists, associated media personnel, trade unionists and human rights advocates in the previous 12 months</t>
+          <t xml:space="preserve"> Proportion of children under 5 years of age whose births have been registered with a civil authority, by age</t>
         </is>
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>C161001</t>
+          <t>C160901</t>
         </is>
       </c>
     </row>
@@ -8670,17 +8662,17 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>16.10.2</t>
+          <t>16.10.1</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries that adopt and implement constitutional, statutory and/or policy guarantees for public access to information</t>
+          <t xml:space="preserve"> Number of verified cases of killing, kidnapping, enforced disappearance, arbitrary detention and torture of journalists, associated media personnel, trade unionists and human rights advocates in the previous 12 months</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>C161002</t>
+          <t>C161001</t>
         </is>
       </c>
     </row>
@@ -8697,27 +8689,27 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>16.a</t>
+          <t>16.10</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Strengthen relevant national institutions, including through international cooperation, for building capacity at all levels, in particular in developing countries, to prevent violence and combat terrorism and crime</t>
+          <t xml:space="preserve"> Ensure public access to information and protect fundamental freedoms, in accordance with national legislation and international agreements</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>16.a.1</t>
+          <t>16.10.2</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Existence of independent national human rights institutions in compliance with the Paris Principles</t>
+          <t xml:space="preserve"> Number of countries that adopt and implement constitutional, statutory and/or policy guarantees for public access to information</t>
         </is>
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>C160a01</t>
+          <t>C161002</t>
         </is>
       </c>
     </row>
@@ -8734,64 +8726,64 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>16.b</t>
+          <t>16.a</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Promote and enforce non-discriminatory laws and policies for sustainable development</t>
+          <t xml:space="preserve"> Strengthen relevant national institutions, including through international cooperation, for building capacity at all levels, in particular in developing countries, to prevent violence and combat terrorism and crime</t>
         </is>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>16.b.1</t>
+          <t>16.a.1</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of population reporting having personally felt discriminated against or harassed in the previous 12 months on the basis of a ground of discrimination prohibited under international human rights law</t>
+          <t xml:space="preserve"> Existence of independent national human rights institutions in compliance with the Paris Principles</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>C200204</t>
+          <t>C160a01</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>16</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Partnerships for the Goals</t>
+          <t>Peace, Justice, and Strong Institutions</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>17.1</t>
+          <t>16.b</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Strengthen domestic resource mobilization, including through international support to developing countries, to improve domestic capacity for tax and other revenue collection</t>
+          <t xml:space="preserve"> Promote and enforce non-discriminatory laws and policies for sustainable development</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>17.1.1</t>
+          <t>16.b.1</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Total government revenue as a proportion of GDP, by source</t>
+          <t xml:space="preserve"> Proportion of population reporting having personally felt discriminated against or harassed in the previous 12 months on the basis of a ground of discrimination prohibited under international human rights law</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>C170101</t>
+          <t>C200204</t>
         </is>
       </c>
     </row>
@@ -8818,17 +8810,17 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>17.1.2</t>
+          <t>17.1.1</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of domestic budget funded by domestic taxes</t>
+          <t xml:space="preserve"> Total government revenue as a proportion of GDP, by source</t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>C170102</t>
+          <t>C170101</t>
         </is>
       </c>
     </row>
@@ -8845,27 +8837,27 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>17.2</t>
+          <t>17.1</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Developed countries to implement fully their official development assistance commitments, including the commitment by many developed countries to achieve the target of 0.7 per cent of gross national income for official development assistance (ODA/GNI) to developing countries and 0.15 to 0.20 per cent of ODA/GNI to least developed countries; ODA providers are encouraged to consider setting a target to provide at least 0.20 per cent of ODA/GNI to least developed countries</t>
+          <t xml:space="preserve"> Strengthen domestic resource mobilization, including through international support to developing countries, to improve domestic capacity for tax and other revenue collection</t>
         </is>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>17.2.1</t>
+          <t>17.1.2</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Net official development assistance, total and to least developed countries, as a proportion of the Organization for Economic Cooperation and Development (OECD) Development Assistance Committee donors’ gross national income (GNI)</t>
+          <t xml:space="preserve"> Proportion of domestic budget funded by domestic taxes</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>C170201</t>
+          <t>C170102</t>
         </is>
       </c>
     </row>
@@ -8882,27 +8874,27 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>17.3</t>
+          <t>17.2</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mobilize additional financial resources for developing countries from multiple sources</t>
+          <t xml:space="preserve"> Developed countries to implement fully their official development assistance commitments, including the commitment by many developed countries to achieve the target of 0.7 per cent of gross national income for official development assistance (ODA/GNI) to developing countries and 0.15 to 0.20 per cent of ODA/GNI to least developed countries; ODA providers are encouraged to consider setting a target to provide at least 0.20 per cent of ODA/GNI to least developed countries</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>17.3.1</t>
+          <t>17.2.1</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Additional financial resources mobilized for developing countries from multiple sources</t>
+          <t xml:space="preserve"> Net official development assistance, total and to least developed countries, as a proportion of the Organization for Economic Cooperation and Development (OECD) Development Assistance Committee donors’ gross national income (GNI)</t>
         </is>
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>C170304</t>
+          <t>C170201</t>
         </is>
       </c>
     </row>
@@ -8929,17 +8921,17 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>17.3.2</t>
+          <t>17.3.1</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Volume of remittances (in United States dollars) as a proportion of total GDP</t>
+          <t xml:space="preserve"> Additional financial resources mobilized for developing countries from multiple sources</t>
         </is>
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>C170302</t>
+          <t>C170304</t>
         </is>
       </c>
     </row>
@@ -8956,27 +8948,27 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>17.4</t>
+          <t>17.3</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Assist developing countries in attaining long-term debt sustainability through coordinated policies aimed at fostering debt financing, debt relief and debt restructuring, as appropriate, and address the external debt of highly indebted poor countries to reduce debt distress</t>
+          <t xml:space="preserve"> Mobilize additional financial resources for developing countries from multiple sources</t>
         </is>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>17.4.1</t>
+          <t>17.3.2</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Debt service as a proportion of exports of goods and services</t>
+          <t xml:space="preserve"> Volume of remittances (in United States dollars) as a proportion of total GDP</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>C170401</t>
+          <t>C170302</t>
         </is>
       </c>
     </row>
@@ -8993,27 +8985,27 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>17.5</t>
+          <t>17.4</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Adopt and implement investment promotion regimes for least developed countries</t>
+          <t xml:space="preserve"> Assist developing countries in attaining long-term debt sustainability through coordinated policies aimed at fostering debt financing, debt relief and debt restructuring, as appropriate, and address the external debt of highly indebted poor countries to reduce debt distress</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>17.5.1</t>
+          <t>17.4.1</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries that adopt and implement investment promotion regimes for developing countries, including the least developed countries</t>
+          <t xml:space="preserve"> Debt service as a proportion of exports of goods and services</t>
         </is>
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>C170502</t>
+          <t>C170401</t>
         </is>
       </c>
     </row>
@@ -9030,27 +9022,27 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>17.6</t>
+          <t>17.5</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Enhance North-South, South-South and triangular regional and international cooperation on and access to science, technology and innovation and enhance knowledge-sharing on mutually agreed terms, including through improved coordination among existing mechanisms, in particular at the United Nations level, and through a global technology facilitation mechanism</t>
+          <t xml:space="preserve"> Adopt and implement investment promotion regimes for least developed countries</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>17.6.1</t>
+          <t>17.5.1</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fixed Internet broadband subscriptions per 100 inhabitants, by speed5</t>
+          <t xml:space="preserve"> Number of countries that adopt and implement investment promotion regimes for developing countries, including the least developed countries</t>
         </is>
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>C170602</t>
+          <t>C170502</t>
         </is>
       </c>
     </row>
@@ -9067,27 +9059,27 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>17.7</t>
+          <t>17.6</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Promote the development, transfer, dissemination and diffusion of environmentally sound technologies to developing countries on favourable terms, including on concessional and preferential terms, as mutually agreed</t>
+          <t xml:space="preserve"> Enhance North-South, South-South and triangular regional and international cooperation on and access to science, technology and innovation and enhance knowledge-sharing on mutually agreed terms, including through improved coordination among existing mechanisms, in particular at the United Nations level, and through a global technology facilitation mechanism</t>
         </is>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>17.7.1</t>
+          <t>17.6.1</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Total amount of funding for developing countries to promote the development, transfer, dissemination and diffusion of environmentally sound technologies</t>
+          <t xml:space="preserve"> Fixed Internet broadband subscriptions per 100 inhabitants, by speed5</t>
         </is>
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>C170701</t>
+          <t>C170602</t>
         </is>
       </c>
     </row>
@@ -9104,27 +9096,27 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>17.8</t>
+          <t>17.7</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fully operationalize the technology bank and science, technology and innovation capacity-building mechanism for least developed countries by 2017 and enhance the use of enabling technology, in particular information and communications technology</t>
+          <t xml:space="preserve"> Promote the development, transfer, dissemination and diffusion of environmentally sound technologies to developing countries on favourable terms, including on concessional and preferential terms, as mutually agreed</t>
         </is>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>17.8.1</t>
+          <t>17.7.1</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Proportion of individuals using the Internet</t>
+          <t xml:space="preserve"> Total amount of funding for developing countries to promote the development, transfer, dissemination and diffusion of environmentally sound technologies</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>C170801</t>
+          <t>C170701</t>
         </is>
       </c>
     </row>
@@ -9141,27 +9133,27 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>17.9</t>
+          <t>17.8</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Enhance international support for implementing effective and targeted capacity-building in developing countries to support national plans to implement all the Sustainable Development Goals, including through North-South, South-South and triangular cooperation</t>
+          <t xml:space="preserve"> Fully operationalize the technology bank and science, technology and innovation capacity-building mechanism for least developed countries by 2017 and enhance the use of enabling technology, in particular information and communications technology</t>
         </is>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>17.9.1</t>
+          <t>17.8.1</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dollar value of financial and technical assistance (including through North-South, South‑South and triangular cooperation) committed to developing countries</t>
+          <t xml:space="preserve"> Proportion of individuals using the Internet</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>C170901</t>
+          <t>C170801</t>
         </is>
       </c>
     </row>
@@ -9178,27 +9170,27 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>17.10</t>
+          <t>17.9</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Promote a universal, rules-based, open, non‑discriminatory and equitable multilateral trading system under the World Trade Organization, including through the conclusion of negotiations under its Doha Development Agenda</t>
+          <t xml:space="preserve"> Enhance international support for implementing effective and targeted capacity-building in developing countries to support national plans to implement all the Sustainable Development Goals, including through North-South, South-South and triangular cooperation</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>17.10.1</t>
+          <t>17.9.1</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Worldwide weighted tariff-average</t>
+          <t xml:space="preserve"> Dollar value of financial and technical assistance (including through North-South, South‑South and triangular cooperation) committed to developing countries</t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>C171001</t>
+          <t>C170901</t>
         </is>
       </c>
     </row>
@@ -9215,27 +9207,27 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>17.11</t>
+          <t>17.10</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Significantly increase the exports of developing countries, in particular with a view to doubling the least developed countries’ share of global exports by 2020</t>
+          <t xml:space="preserve"> Promote a universal, rules-based, open, non‑discriminatory and equitable multilateral trading system under the World Trade Organization, including through the conclusion of negotiations under its Doha Development Agenda</t>
         </is>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>17.11.1</t>
+          <t>17.10.1</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Developing countries’ and least developed countries’ share of global exports</t>
+          <t xml:space="preserve"> Worldwide weighted tariff-average</t>
         </is>
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>C171101</t>
+          <t>C171001</t>
         </is>
       </c>
     </row>
@@ -9252,27 +9244,27 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>17.12</t>
+          <t>17.11</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Realize timely implementation of duty-free and quota-free market access on a lasting basis for all least developed countries, consistent with World Trade Organization decisions, including by ensuring that preferential rules of origin applicable to imports from least developed countries are transparent and simple, and contribute to facilitating market access</t>
+          <t xml:space="preserve"> Significantly increase the exports of developing countries, in particular with a view to doubling the least developed countries’ share of global exports by 2020</t>
         </is>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>17.12.1</t>
+          <t>17.11.1</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Weighted average tariffs faced by developing countries, least developed countries and small island developing States</t>
+          <t xml:space="preserve"> Developing countries’ and least developed countries’ share of global exports</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>C171201</t>
+          <t>C171101</t>
         </is>
       </c>
     </row>
@@ -9289,27 +9281,27 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>17.13</t>
+          <t>17.12</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Enhance global macroeconomic stability, including through policy coordination and policy coherence</t>
+          <t xml:space="preserve"> Realize timely implementation of duty-free and quota-free market access on a lasting basis for all least developed countries, consistent with World Trade Organization decisions, including by ensuring that preferential rules of origin applicable to imports from least developed countries are transparent and simple, and contribute to facilitating market access</t>
         </is>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>17.13.1</t>
+          <t>17.12.1</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Macroeconomic Dashboard</t>
+          <t xml:space="preserve"> Weighted average tariffs faced by developing countries, least developed countries and small island developing States</t>
         </is>
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>C171301</t>
+          <t>C171201</t>
         </is>
       </c>
     </row>
@@ -9326,27 +9318,27 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>17.14</t>
+          <t>17.13</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Enhance policy coherence for sustainable development</t>
+          <t xml:space="preserve"> Enhance global macroeconomic stability, including through policy coordination and policy coherence</t>
         </is>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>17.14.1</t>
+          <t>17.13.1</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries with mechanisms in place to enhance policy coherence of sustainable development</t>
+          <t xml:space="preserve"> Macroeconomic Dashboard</t>
         </is>
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>C171401</t>
+          <t>C171301</t>
         </is>
       </c>
     </row>
@@ -9363,27 +9355,27 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>17.15</t>
+          <t>17.14</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Respect each country’s policy space and leadership to establish and implement policies for poverty eradication and sustainable development</t>
+          <t xml:space="preserve"> Enhance policy coherence for sustainable development</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>17.15.1</t>
+          <t>17.14.1</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Extent of use of country-owned results frameworks and planning tools by providers of development cooperation</t>
+          <t xml:space="preserve"> Number of countries with mechanisms in place to enhance policy coherence of sustainable development</t>
         </is>
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>C171501</t>
+          <t>C171401</t>
         </is>
       </c>
     </row>
@@ -9400,27 +9392,27 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>17.16</t>
+          <t>17.15</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Enhance the Global Partnership for Sustainable Development, complemented by multi-stakeholder partnerships that mobilize and share knowledge, expertise, technology and financial resources, to support the achievement of the Sustainable Development Goals in all countries, in particular developing countries</t>
+          <t xml:space="preserve"> Respect each country’s policy space and leadership to establish and implement policies for poverty eradication and sustainable development</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>17.16.1</t>
+          <t>17.15.1</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries reporting progress in multi-stakeholder development effectiveness monitoring frameworks that support the achievement of the sustainable development goals</t>
+          <t xml:space="preserve"> Extent of use of country-owned results frameworks and planning tools by providers of development cooperation</t>
         </is>
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>C171601</t>
+          <t>C171501</t>
         </is>
       </c>
     </row>
@@ -9437,27 +9429,27 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>17.17</t>
+          <t>17.16</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Encourage and promote effective public, public-private and civil society partnerships, building on the experience and resourcing strategies of partnerships</t>
+          <t xml:space="preserve"> Enhance the Global Partnership for Sustainable Development, complemented by multi-stakeholder partnerships that mobilize and share knowledge, expertise, technology and financial resources, to support the achievement of the Sustainable Development Goals in all countries, in particular developing countries</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>17.17.1</t>
+          <t>17.16.1</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Amount in United States dollars committed to public-private partnerships for infrastructure</t>
+          <t xml:space="preserve"> Number of countries reporting progress in multi-stakeholder development effectiveness monitoring frameworks that support the achievement of the sustainable development goals</t>
         </is>
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>C171702</t>
+          <t>C171601</t>
         </is>
       </c>
     </row>
@@ -9474,27 +9466,27 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>17.18</t>
+          <t>17.17</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2020, enhance capacity-building support to developing countries, including for least developed countries and small island developing States, to increase significantly the availability of high-quality, timely and reliable data disaggregated by income, gender, age, race, ethnicity, migratory status, disability, geographic location and other characteristics relevant in national contexts</t>
+          <t xml:space="preserve"> Encourage and promote effective public, public-private and civil society partnerships, building on the experience and resourcing strategies of partnerships</t>
         </is>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>17.18.1</t>
+          <t>17.17.1</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Statistical capacity indicator for Sustainable Development Goal monitoring</t>
+          <t xml:space="preserve"> Amount in United States dollars committed to public-private partnerships for infrastructure</t>
         </is>
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>C171804</t>
+          <t>C171702</t>
         </is>
       </c>
     </row>
@@ -9521,17 +9513,17 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>17.18.2</t>
+          <t>17.18.1</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries that have national statistical legislation that complies with the Fundamental Principles of Official Statistics</t>
+          <t xml:space="preserve"> Statistical capacity indicator for Sustainable Development Goal monitoring</t>
         </is>
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>C171802</t>
+          <t>C171804</t>
         </is>
       </c>
     </row>
@@ -9558,17 +9550,17 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>17.18.3</t>
+          <t>17.18.2</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Number of countries with a national statistical plan that is fully funded and under implementation, by source of funding</t>
+          <t xml:space="preserve"> Number of countries that have national statistical legislation that complies with the Fundamental Principles of Official Statistics</t>
         </is>
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>C171803</t>
+          <t>C171802</t>
         </is>
       </c>
     </row>
@@ -9585,27 +9577,27 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>17.19</t>
+          <t>17.18</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t xml:space="preserve"> By 2030, build on existing initiatives to develop measurements of progress on sustainable development that complement gross domestic product, and support statistical capacity-building in developing countries</t>
+          <t xml:space="preserve"> By 2020, enhance capacity-building support to developing countries, including for least developed countries and small island developing States, to increase significantly the availability of high-quality, timely and reliable data disaggregated by income, gender, age, race, ethnicity, migratory status, disability, geographic location and other characteristics relevant in national contexts</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>17.19.1</t>
+          <t>17.18.3</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Dollar value of all resources made available to strengthen statistical capacity in developing countries</t>
+          <t xml:space="preserve"> Number of countries with a national statistical plan that is fully funded and under implementation, by source of funding</t>
         </is>
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>C171901</t>
+          <t>C171803</t>
         </is>
       </c>
     </row>
@@ -9632,15 +9624,52 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
+          <t>17.19.1</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Dollar value of all resources made available to strengthen statistical capacity in developing countries</t>
+        </is>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>C171901</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Partnerships for the Goals</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>17.19</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> By 2030, build on existing initiatives to develop measurements of progress on sustainable development that complement gross domestic product, and support statistical capacity-building in developing countries</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
           <t>17.19.2</t>
         </is>
       </c>
-      <c r="F249" t="inlineStr">
+      <c r="F250" t="inlineStr">
         <is>
           <t xml:space="preserve"> Proportion of countries that (a) have conducted at least one population and housing census in the last 10 years; and (b) have achieved 100 per cent birth registration and 80 per cent death registration</t>
         </is>
       </c>
-      <c r="G249" t="inlineStr">
+      <c r="G250" t="inlineStr">
         <is>
           <t>C171902</t>
         </is>

</xml_diff>

<commit_message>
add JRC SGD target keywords
</commit_message>
<xml_diff>
--- a/SDG_Target_Indicator_UNSD_2023.xlsx
+++ b/SDG_Target_Indicator_UNSD_2023.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G250"/>
+  <dimension ref="A1:H250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>UNSDIndicatorCodes</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>JRCKeywords</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -506,6 +511,11 @@
           <t>C010101</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>['international poverty line', ' extreme poverty', ' abject poverty', ' absolute poverty', 'destitution', 'penury', 'severe deprivation', 'help people suffering from food and material deprivation', 'extremely poor', 'incidence of poverty', 'Households in poverty']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -543,6 +553,11 @@
           <t>C010201</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>['severely materially deprived people', 'low work intensity', 'national poverty line', 'social exclusion', 'income poverty', 'combatting child poverty', 'children out of poverty', 'addressing child poverty', 'at risk of poverty', 'fight child poverty', 'poverty rate', 'living in poverty', 'poor households', 'multidimensional poverty', 'basic needs']</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -580,6 +595,11 @@
           <t>C010202</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>['severely materially deprived people', 'low work intensity', 'national poverty line', 'social exclusion', 'income poverty', 'combatting child poverty', 'children out of poverty', 'addressing child poverty', 'at risk of poverty', 'fight child poverty', 'poverty rate', 'living in poverty', 'poor households', 'multidimensional poverty', 'basic needs']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -617,6 +637,11 @@
           <t>C010301</t>
         </is>
       </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>['social risk', 'social protection', 'rights of persons with disabilities', 'rights of unemployed persons', 'rights of older persons', 'rights of pregnant women', 'rights of work-injury victims', 'rights of the poor', 'rights of the vulnerable', 'hiring subsidies', 'social security', 'child benefits', 'maternity benefits', 'support for unemployment', 'support for people without a job', 'benefits for persons with disabilities', 'benefits for victims of work injuries', 'benefits for older persons', 'family benefits', 'maternity protection', 'unemployment support', 'employment injury benefits', 'sickness benefits', 'disability pensions', 'old-age pensions', 'social welfare benefits', 'social spending', 'social services', 'social expenditure']</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -654,6 +679,11 @@
           <t>C010401</t>
         </is>
       </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>['tenure rights', 'equal rights to economic resources', 'control over land', 'access to inheritance', 'rights to land', '\naccess to property', 'access to natural resources', 'access to new technology', 'access to financial services', 'access to microfinance', 'access to services', 'property rights', 'access to basic goods', 'basic goods for all', 'access to basic services', 'delivery of essential services', 'provide essential basic services', 'land tenancy right']</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -691,6 +721,11 @@
           <t>C010402</t>
         </is>
       </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>['tenure rights', 'equal rights to economic resources', 'control over land', 'access to inheritance', 'rights to land', '\naccess to property', 'access to natural resources', 'access to new technology', 'access to financial services', 'access to microfinance', 'access to services', 'property rights', 'access to basic goods', 'basic goods for all', 'access to basic services', 'delivery of essential services', 'provide essential basic services', 'land tenancy right']</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -728,6 +763,11 @@
           <t>C200303</t>
         </is>
       </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>['disaster risk reduction', 'vulnerability in disaster', 'affected by extreme events', 'resilience of the poor', 'reduce vulnerability', 'resilience to disaster', 'disaster resilience', 'vulnerable people', 'protect livelihoods', 'build resilience to future shocks', 'build resilience to shocks', 'vulnerability to climate event', 'vulnerability to climate extreme event', 'vulnerability to economic shock', 'vulnerability to natural disaster', 'resilience to catastrophic events', 'vulnerability to catastrophic events', 'economic loss attributed to disasters', 'economic loss due to disasters', 'strengthen economic resilience', 'strengthen social resilience', 'preventing disaster risk', 'vulnerable groups', 'vulnerable social groups', ' vulnerable to external shocks', 'vulnerable individuals', 'vulnerable sections of the population', 'vulnerable population', 'vulnerable communities', 'resilience within communities', 'weakest population', 'vulnerability to earthquakes', 'resilience to earthquakes', 'earthquake risk', 'earthquakes resilience', 'plagues risk reduction', 'vulnerability to plagues', 'resilience to plagues', 'plagues resilience', 'preventing plagues risk', 'sandstorms risk reduction', 'vulnerability to sandstorms', 'resilience to sandstorms', 'sandstorms resilience', 'preventing sandstorms risk', 'vulnerability to extreme climate event']</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -765,6 +805,11 @@
           <t>C200211</t>
         </is>
       </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>['disaster risk reduction', 'vulnerability in disaster', 'affected by extreme events', 'resilience of the poor', 'reduce vulnerability', 'resilience to disaster', 'disaster resilience', 'vulnerable people', 'protect livelihoods', 'build resilience to future shocks', 'build resilience to shocks', 'vulnerability to climate event', 'vulnerability to climate extreme event', 'vulnerability to economic shock', 'vulnerability to natural disaster', 'resilience to catastrophic events', 'vulnerability to catastrophic events', 'economic loss attributed to disasters', 'economic loss due to disasters', 'strengthen economic resilience', 'strengthen social resilience', 'preventing disaster risk', 'vulnerable groups', 'vulnerable social groups', ' vulnerable to external shocks', 'vulnerable individuals', 'vulnerable sections of the population', 'vulnerable population', 'vulnerable communities', 'resilience within communities', 'weakest population', 'vulnerability to earthquakes', 'resilience to earthquakes', 'earthquake risk', 'earthquakes resilience', 'plagues risk reduction', 'vulnerability to plagues', 'resilience to plagues', 'plagues resilience', 'preventing plagues risk', 'sandstorms risk reduction', 'vulnerability to sandstorms', 'resilience to sandstorms', 'sandstorms resilience', 'preventing sandstorms risk', 'vulnerability to extreme climate event']</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -802,6 +847,11 @@
           <t>C200304</t>
         </is>
       </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>['disaster risk reduction', 'vulnerability in disaster', 'affected by extreme events', 'resilience of the poor', 'reduce vulnerability', 'resilience to disaster', 'disaster resilience', 'vulnerable people', 'protect livelihoods', 'build resilience to future shocks', 'build resilience to shocks', 'vulnerability to climate event', 'vulnerability to climate extreme event', 'vulnerability to economic shock', 'vulnerability to natural disaster', 'resilience to catastrophic events', 'vulnerability to catastrophic events', 'economic loss attributed to disasters', 'economic loss due to disasters', 'strengthen economic resilience', 'strengthen social resilience', 'preventing disaster risk', 'vulnerable groups', 'vulnerable social groups', ' vulnerable to external shocks', 'vulnerable individuals', 'vulnerable sections of the population', 'vulnerable population', 'vulnerable communities', 'resilience within communities', 'weakest population', 'vulnerability to earthquakes', 'resilience to earthquakes', 'earthquake risk', 'earthquakes resilience', 'plagues risk reduction', 'vulnerability to plagues', 'resilience to plagues', 'plagues resilience', 'preventing plagues risk', 'sandstorms risk reduction', 'vulnerability to sandstorms', 'resilience to sandstorms', 'sandstorms resilience', 'preventing sandstorms risk', 'vulnerability to extreme climate event']</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -839,6 +889,11 @@
           <t>C200305</t>
         </is>
       </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>['disaster risk reduction', 'vulnerability in disaster', 'affected by extreme events', 'resilience of the poor', 'reduce vulnerability', 'resilience to disaster', 'disaster resilience', 'vulnerable people', 'protect livelihoods', 'build resilience to future shocks', 'build resilience to shocks', 'vulnerability to climate event', 'vulnerability to climate extreme event', 'vulnerability to economic shock', 'vulnerability to natural disaster', 'resilience to catastrophic events', 'vulnerability to catastrophic events', 'economic loss attributed to disasters', 'economic loss due to disasters', 'strengthen economic resilience', 'strengthen social resilience', 'preventing disaster risk', 'vulnerable groups', 'vulnerable social groups', ' vulnerable to external shocks', 'vulnerable individuals', 'vulnerable sections of the population', 'vulnerable population', 'vulnerable communities', 'resilience within communities', 'weakest population', 'vulnerability to earthquakes', 'resilience to earthquakes', 'earthquake risk', 'earthquakes resilience', 'plagues risk reduction', 'vulnerability to plagues', 'resilience to plagues', 'plagues resilience', 'preventing plagues risk', 'sandstorms risk reduction', 'vulnerability to sandstorms', 'resilience to sandstorms', 'sandstorms resilience', 'preventing sandstorms risk', 'vulnerability to extreme climate event']</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -876,6 +931,11 @@
           <t>C010a04</t>
         </is>
       </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>['poverty reduction programmes', 'means for developing countries', 'reduce poverty in developing countries', 'reduce poverty LDCs', 'donors that focus on poverty reduction', 'development assistance for poverty reduction']</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -913,6 +973,11 @@
           <t>C010a02</t>
         </is>
       </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>['poverty reduction programmes', 'means for developing countries', 'reduce poverty in developing countries', 'reduce poverty LDCs', 'donors that focus on poverty reduction', 'development assistance for poverty reduction']</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -950,6 +1015,11 @@
           <t>C010b02</t>
         </is>
       </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>['pro-poor policy framework', 'poverty eradication actions', 'poverty reduction strategies', 'investments in poverty eradication', 'development strategies for poverty', 'Pro-poor public social spending', 'Pro-poor spending', 'Pro-poor investment', 'poor-oriented']</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -987,6 +1057,11 @@
           <t>C020101</t>
         </is>
       </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>['sufficient food', 'undernourishment', 'end hunger', 'necessary nourishment', 'access to food', 'food access', 'food insecurity', 'food for all', ' food for the poor', ' food for people in vulnerable situations', 'food for vulnerable people', 'safe food', 'wholesome food', 'food safety', 'safety of food', 'food nutritional value', 'food security', 'zero hunger', 'acute hunger', 'people affected by hunger', 'starvation', 'acute undernutrition', 'famine', ' food needs', 'extreme hunger', 'food shortage', 'nutritious and affordable food']</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1024,6 +1099,11 @@
           <t>C020102</t>
         </is>
       </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>['sufficient food', 'undernourishment', 'end hunger', 'necessary nourishment', 'access to food', 'food access', 'food insecurity', 'food for all', ' food for the poor', ' food for people in vulnerable situations', 'food for vulnerable people', 'safe food', 'wholesome food', 'food safety', 'safety of food', 'food nutritional value', 'food security', 'zero hunger', 'acute hunger', 'people affected by hunger', 'starvation', 'acute undernutrition', 'famine', ' food needs', 'extreme hunger', 'food shortage', 'nutritious and affordable food']</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1061,6 +1141,11 @@
           <t>C020201</t>
         </is>
       </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>['child growth standards', 'obesity rate', 'nutritional needs', 'nutritious food', 'stunting', 'malnutrition', 'malnourishment', 'obesity prevalence', 'childhood obesity', 'childhood nutrition', 'child nutrition', 'Prevalence of anaemia', 'wasting in children', 'children affected by wasting', 'underweight children', 'healthy and nutritious diets', 'healthy and sustainable diets', 'nutrition security']</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1098,6 +1183,11 @@
           <t>C020202</t>
         </is>
       </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>['child growth standards', 'obesity rate', 'nutritional needs', 'nutritious food', 'stunting', 'malnutrition', 'malnourishment', 'obesity prevalence', 'childhood obesity', 'childhood nutrition', 'child nutrition', 'Prevalence of anaemia', 'wasting in children', 'children affected by wasting', 'underweight children', 'healthy and nutritious diets', 'healthy and sustainable diets', 'nutrition security']</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1135,6 +1225,11 @@
           <t>C020203</t>
         </is>
       </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>['child growth standards', 'obesity rate', 'nutritional needs', 'nutritious food', 'stunting', 'malnutrition', 'malnourishment', 'obesity prevalence', 'childhood obesity', 'childhood nutrition', 'child nutrition', 'Prevalence of anaemia', 'wasting in children', 'children affected by wasting', 'underweight children', 'healthy and nutritious diets', 'healthy and sustainable diets', 'nutrition security']</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1172,6 +1267,11 @@
           <t>C020301</t>
         </is>
       </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>['small scale food producers', 'farm employment', 'family farmers', 'agricultural productivity', 'support pastoralists', 'Agricultural Fund for Rural Development', 'help farmers', 'support farmers', 'smallholder farmers ability', 'small scale farmers', 'improves rural livelihoods', 'sustainably managing agricultural soils', 'decent living for farmers', 'decent living for fishermen', 'agricultural products', 'agricultural producers', 'agricultural output', 'agri-business', 'agro-processing', 'agricultural value chains', 'small farmers', 'productive land uses', 'increase livestock', 'improve pastoral transhumance', 'support pastoral farming', 'cotton production', 'maize production', 'crops production', 'yield production']</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1209,6 +1309,11 @@
           <t>C020302</t>
         </is>
       </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>['small scale food producers', 'farm employment', 'family farmers', 'agricultural productivity', 'support pastoralists', 'Agricultural Fund for Rural Development', 'help farmers', 'support farmers', 'smallholder farmers ability', 'small scale farmers', 'improves rural livelihoods', 'sustainably managing agricultural soils', 'decent living for farmers', 'decent living for fishermen', 'agricultural products', 'agricultural producers', 'agricultural output', 'agri-business', 'agro-processing', 'agricultural value chains', 'small farmers', 'productive land uses', 'increase livestock', 'improve pastoral transhumance', 'support pastoral farming', 'cotton production', 'maize production', 'crops production', 'yield production']</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1246,6 +1351,11 @@
           <t>C020401</t>
         </is>
       </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>['sustainable food production systems', 'resilient agricultural practices', 'sustainable agriculture', 'soil quality', 'organic farming', 'make the agricultural system more resilient to climate change', 'environmentally-friendly food system', 'sustainable food supply chains', 'sustainable agri-food systems', 'risk of non-sustainable agriculture', 'eco-agricultural models', 'sustainable livelihoods Initiative', 'climate-friendly agriculture', 'environment-friendly agriculture', 'reduce the footprint of food production', 'agro-ecology', 'agroecology', 'sustainable food system', 'sustainable farming', 'farm to fork', 'climate-smart agriculture', 'resource efficient food production', 'agri-food production']</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1283,6 +1393,11 @@
           <t>C020501</t>
         </is>
       </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>['animal genetic resources', 'cultivated plants', 'seed banks', 'GMO', 'domesticated animals', 'plant banks', 'plant genetic resources', ' genetic diversity of seeds', 'plant gene banks', 'livestock gene banks', 'breeds classified as being at risk of extinction', 'breeds at risk of extinction', 'silvopastoral and agroforestry production modes', 'genetic diversity in agriculture', 'genetic diversity of agricultural crops', 'agricultural area under high-diversity landscape']</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1320,6 +1435,11 @@
           <t>C020503</t>
         </is>
       </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>['animal genetic resources', 'cultivated plants', 'seed banks', 'GMO', 'domesticated animals', 'plant banks', 'plant genetic resources', ' genetic diversity of seeds', 'plant gene banks', 'livestock gene banks', 'breeds classified as being at risk of extinction', 'breeds at risk of extinction', 'silvopastoral and agroforestry production modes', 'genetic diversity in agriculture', 'genetic diversity of agricultural crops', 'agricultural area under high-diversity landscape']</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1357,6 +1477,11 @@
           <t>C020a01</t>
         </is>
       </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>['agricultural investment', 'agriculture orientation index', ' agricultural research', 'finance agriculture', 'stimulate research and development within the agri-food industry', 'research in the agri-food industry', 'stimulate development within the agri-food industry', 'research within the agri-food industry', 'investment in agriculture', 'agricultural cooperation']</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1394,6 +1519,11 @@
           <t>C020a02</t>
         </is>
       </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>['agricultural investment', 'agriculture orientation index', ' agricultural research', 'finance agriculture', 'stimulate research and development within the agri-food industry', 'research in the agri-food industry', 'stimulate development within the agri-food industry', 'research within the agri-food industry', 'investment in agriculture', 'agricultural cooperation']</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1431,6 +1561,11 @@
           <t>C020b02</t>
         </is>
       </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>['agricultural export subsidies', 'world agricultural markets', 'agricultural exports', 'agricultural market', 'agricultural trade', 'agricultural goods market', 'food imports']</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1468,6 +1603,11 @@
           <t>C020c01</t>
         </is>
       </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>['food price volatility', 'food price anomalies', 'food commodity markets', 'food reserves', 'food price changes', 'changes food price', 'volatility food price', 'volatility prices of food', 'anomalies food price', 'anomalies prices of food', 'food mispricing']</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1505,6 +1645,11 @@
           <t>C030101</t>
         </is>
       </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>['maternal mortality', ' death in pregnancy', 'death in childbirth', 'maternal deaths', 'deaths which occur during pregnancy', 'obstetric deaths', 'death occurring in childbirth', 'pregnancy related deaths', 'pregnancy deaths', 'deaths related to pregnancy', 'deaths related to childbirth', 'MMR', 'MMRate', 'maternal health', 'childbirth assisted']</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1542,6 +1687,11 @@
           <t>C030102</t>
         </is>
       </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>['maternal mortality', ' death in pregnancy', 'death in childbirth', 'maternal deaths', 'deaths which occur during pregnancy', 'obstetric deaths', 'death occurring in childbirth', 'pregnancy related deaths', 'pregnancy deaths', 'deaths related to pregnancy', 'deaths related to childbirth', 'MMR', 'MMRate', 'maternal health', 'childbirth assisted']</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1579,6 +1729,11 @@
           <t>C030201</t>
         </is>
       </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>['child mortality', 'neonatal mortality', 'infant mortality', 'children mortality', 'U5MR', 'Mortality rates among young children', 'Mortality rates among children', 'Mortality rates of children', 'under-5 mortality', 'NMR', 'mortality of children', 'stunting in children']</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1616,6 +1771,11 @@
           <t>C030202</t>
         </is>
       </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>['child mortality', 'neonatal mortality', 'infant mortality', 'children mortality', 'U5MR', 'Mortality rates among young children', 'Mortality rates among children', 'Mortality rates of children', 'under-5 mortality', 'NMR', 'mortality of children', 'stunting in children']</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1653,6 +1813,11 @@
           <t>C030301</t>
         </is>
       </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>['hepatitis', 'malaria', 'neglected tropical diseases', 'communicable diseases', 'water-borne diseases', 'AIDS', 'end epidemics', 'HIV', 'tuberculosis', 'cope with epidemic', 'combat pandemic', 'combat epidemic', 'combat COVID-19', 'stem COVID transmission', 'infectious diseases']</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1690,6 +1855,11 @@
           <t>C030302</t>
         </is>
       </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>['hepatitis', 'malaria', 'neglected tropical diseases', 'communicable diseases', 'water-borne diseases', 'AIDS', 'end epidemics', 'HIV', 'tuberculosis', 'cope with epidemic', 'combat pandemic', 'combat epidemic', 'combat COVID-19', 'stem COVID transmission', 'infectious diseases']</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1727,6 +1897,11 @@
           <t>C030303</t>
         </is>
       </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>['hepatitis', 'malaria', 'neglected tropical diseases', 'communicable diseases', 'water-borne diseases', 'AIDS', 'end epidemics', 'HIV', 'tuberculosis', 'cope with epidemic', 'combat pandemic', 'combat epidemic', 'combat COVID-19', 'stem COVID transmission', 'infectious diseases']</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1764,6 +1939,11 @@
           <t>C030304</t>
         </is>
       </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>['hepatitis', 'malaria', 'neglected tropical diseases', 'communicable diseases', 'water-borne diseases', 'AIDS', 'end epidemics', 'HIV', 'tuberculosis', 'cope with epidemic', 'combat pandemic', 'combat epidemic', 'combat COVID-19', 'stem COVID transmission', 'infectious diseases']</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1801,6 +1981,11 @@
           <t>C030305</t>
         </is>
       </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>['hepatitis', 'malaria', 'neglected tropical diseases', 'communicable diseases', 'water-borne diseases', 'AIDS', 'end epidemics', 'HIV', 'tuberculosis', 'cope with epidemic', 'combat pandemic', 'combat epidemic', 'combat COVID-19', 'stem COVID transmission', 'infectious diseases']</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1838,6 +2023,11 @@
           <t>C030401</t>
         </is>
       </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>['premature mortality', 'suicide mortality rate', 'mental health', 'chronic respiratory disease', 'cardiovascular disease', 'diabetes', 'fight cancer', 'improving cancer control', 'improving cancer care', 'cancer incidence', 'non-communicable diseases', 'ncd', 'carcinogens', 'suicide deaths', 'promote mental health', 'mental illness']</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1875,6 +2065,11 @@
           <t>C030402</t>
         </is>
       </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>['premature mortality', 'suicide mortality rate', 'mental health', 'chronic respiratory disease', 'cardiovascular disease', 'diabetes', 'fight cancer', 'improving cancer control', 'improving cancer care', 'cancer incidence', 'non-communicable diseases', 'ncd', 'carcinogens', 'suicide deaths', 'promote mental health', 'mental illness']</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1912,6 +2107,11 @@
           <t>C030501</t>
         </is>
       </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>['drug abuse', 'alcohol per capita consumption', 'substance abuse', 'cocaine', ' alcohol consumption', 'cannabis', 'illegal substances', 'drug addiction', 'use of alcohol', 'use of drugs', 'alcohol abuse', 'substance use disorders', 'alcohol consumed', 'alcohol exposure', 'drug exposure']</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1949,6 +2149,11 @@
           <t>C030502</t>
         </is>
       </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>['drug abuse', 'alcohol per capita consumption', 'substance abuse', 'cocaine', ' alcohol consumption', 'cannabis', 'illegal substances', 'drug addiction', 'use of alcohol', 'use of drugs', 'alcohol abuse', 'substance use disorders', 'alcohol consumed', 'alcohol exposure', 'drug exposure']</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1986,6 +2191,11 @@
           <t>C030601</t>
         </is>
       </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>['road traffic injuries', 'road traffic fatality', 'injuries from road traffic crashes', 'injuries from road traffic accidents', 'injuries from road accidents', 'injuries from traffic accident', 'injuries from accidents road', 'injuries from accident traffic', 'deaths from road traffic crashes', 'deaths from road traffic accidents', 'deaths from road accidents', 'deaths from traffic accident', 'deaths from accidents road', 'deaths from accident traffic']</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2023,6 +2233,11 @@
           <t>C030701</t>
         </is>
       </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>['reproductive health', 'family planning', 'sexual health', 'sexual education', 'sexual information', 'adolescent birth', 'reproductive education', 'reproductive information', 'access to contraceptive', 'access to means to prevent pregnancy', 'use of means to prevent pregnancy', 'preventing unintended pregnancies', 'reproductive services', 'adolescent pregnancies', 'Adolescent childbearing', 'safe abortions', 'reproductive rights', 'contraception']</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2060,6 +2275,11 @@
           <t>C030702</t>
         </is>
       </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>['reproductive health', 'family planning', 'sexual health', 'sexual education', 'sexual information', 'adolescent birth', 'reproductive education', 'reproductive information', 'access to contraceptive', 'access to means to prevent pregnancy', 'use of means to prevent pregnancy', 'preventing unintended pregnancies', 'reproductive services', 'adolescent pregnancies', 'Adolescent childbearing', 'safe abortions', 'reproductive rights', 'contraception']</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2097,6 +2317,11 @@
           <t>C030801</t>
         </is>
       </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>['affordable essential medicines', 'essential health services', 'care services', 'access to medicines', 'health coverage', 'health service', 'medicine access', 'health protection', 'protect public health', 'support to health care systems', 'health security', 'inclusive health systems', 'efficient health systems', 'reinforce health care systems', 'resilience of health systems', 'access to healthcare', 'access to health care', 'access to the most basic of rights like healthcare', 'universal healthcare', 'affordable vaccines', 'access to vaccines', 'vaccine access', 'UHC', 'health insurance', 'care costs', 'access to care', 'quality care', 'medical care', 'care provision', 'Household health expenditure', 'inclusive health policy', 'inclusive health']</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2134,6 +2359,11 @@
           <t>C030802</t>
         </is>
       </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>['affordable essential medicines', 'essential health services', 'care services', 'access to medicines', 'health coverage', 'health service', 'medicine access', 'health protection', 'protect public health', 'support to health care systems', 'health security', 'inclusive health systems', 'efficient health systems', 'reinforce health care systems', 'resilience of health systems', 'access to healthcare', 'access to health care', 'access to the most basic of rights like healthcare', 'universal healthcare', 'affordable vaccines', 'access to vaccines', 'vaccine access', 'UHC', 'health insurance', 'care costs', 'access to care', 'quality care', 'medical care', 'care provision', 'Household health expenditure', 'inclusive health policy', 'inclusive health']</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2171,6 +2401,11 @@
           <t>C030901</t>
         </is>
       </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>['respiratory disease', 'health effects of soil pollution', 'health impacts of soil pollution', 'effects of unsafe water', 'harmful effects of chemicals', 'deaths related to hazardous chemical', 'unintentional poisoning', 'deaths related to unsafe water', ' deaths related to unsafe sanitation', 'illnesses from pollution', 'illnesses from contamination', ' mortality attributed to unsafe water', 'mortality attributed to sanitation', 'mortality for lack of hygiene', 'health effects of air pollution', 'health impacts of air pollution', 'deaths related to air pollution', 'deaths from hazardous chemicals', 'deaths from air pollution', 'deaths from water pollution', 'deaths from water contamination', 'deaths from soil pollution', 'deaths from soil contamination', 'illness related to air pollution', 'illness from hazardous chemicals', 'illness from air pollution', 'illness from water pollution', 'illness from water contamination', 'illness from soil pollution', 'illness from soil contamination', 'health effects of water contamination', 'health impacts of water contamination', 'Mortality rate attributed to air pollution', 'Mortality rate for air pollution', 'Mortality for air pollution', 'Mortality attributed to air pollution', 'deaths from hazardous air pollution', 'illness from hazardous air pollution', 'deaths associated with air pollution', 'illness associated with air pollution', 'deaths associated with hazardous chemicals', 'illness associated with hazardous chemicals', 'deaths associated with water contamination', 'illness associated with water contamination', 'deaths associated with soil contamination', 'illness associated with soil contamination', 'air pollution associated diseases', 'water contamination associated diseases', 'soil contamination associated diseases', 'soil pollution associated diseases', 'water pollution associated diseases', 'deaths from unsafe water', 'deaths from unsafe sanitation', 'deaths from lack of hygiene', 'Deaths attributable to unsafe water', 'Deaths attributable to unsafe sanitation', 'Deaths attributable to unsafe hygiene', 'Environmental health']</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2208,6 +2443,11 @@
           <t>C030902</t>
         </is>
       </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>['respiratory disease', 'health effects of soil pollution', 'health impacts of soil pollution', 'effects of unsafe water', 'harmful effects of chemicals', 'deaths related to hazardous chemical', 'unintentional poisoning', 'deaths related to unsafe water', ' deaths related to unsafe sanitation', 'illnesses from pollution', 'illnesses from contamination', ' mortality attributed to unsafe water', 'mortality attributed to sanitation', 'mortality for lack of hygiene', 'health effects of air pollution', 'health impacts of air pollution', 'deaths related to air pollution', 'deaths from hazardous chemicals', 'deaths from air pollution', 'deaths from water pollution', 'deaths from water contamination', 'deaths from soil pollution', 'deaths from soil contamination', 'illness related to air pollution', 'illness from hazardous chemicals', 'illness from air pollution', 'illness from water pollution', 'illness from water contamination', 'illness from soil pollution', 'illness from soil contamination', 'health effects of water contamination', 'health impacts of water contamination', 'Mortality rate attributed to air pollution', 'Mortality rate for air pollution', 'Mortality for air pollution', 'Mortality attributed to air pollution', 'deaths from hazardous air pollution', 'illness from hazardous air pollution', 'deaths associated with air pollution', 'illness associated with air pollution', 'deaths associated with hazardous chemicals', 'illness associated with hazardous chemicals', 'deaths associated with water contamination', 'illness associated with water contamination', 'deaths associated with soil contamination', 'illness associated with soil contamination', 'air pollution associated diseases', 'water contamination associated diseases', 'soil contamination associated diseases', 'soil pollution associated diseases', 'water pollution associated diseases', 'deaths from unsafe water', 'deaths from unsafe sanitation', 'deaths from lack of hygiene', 'Deaths attributable to unsafe water', 'Deaths attributable to unsafe sanitation', 'Deaths attributable to unsafe hygiene', 'Environmental health']</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2245,6 +2485,11 @@
           <t>C030903</t>
         </is>
       </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>['respiratory disease', 'health effects of soil pollution', 'health impacts of soil pollution', 'effects of unsafe water', 'harmful effects of chemicals', 'deaths related to hazardous chemical', 'unintentional poisoning', 'deaths related to unsafe water', ' deaths related to unsafe sanitation', 'illnesses from pollution', 'illnesses from contamination', ' mortality attributed to unsafe water', 'mortality attributed to sanitation', 'mortality for lack of hygiene', 'health effects of air pollution', 'health impacts of air pollution', 'deaths related to air pollution', 'deaths from hazardous chemicals', 'deaths from air pollution', 'deaths from water pollution', 'deaths from water contamination', 'deaths from soil pollution', 'deaths from soil contamination', 'illness related to air pollution', 'illness from hazardous chemicals', 'illness from air pollution', 'illness from water pollution', 'illness from water contamination', 'illness from soil pollution', 'illness from soil contamination', 'health effects of water contamination', 'health impacts of water contamination', 'Mortality rate attributed to air pollution', 'Mortality rate for air pollution', 'Mortality for air pollution', 'Mortality attributed to air pollution', 'deaths from hazardous air pollution', 'illness from hazardous air pollution', 'deaths associated with air pollution', 'illness associated with air pollution', 'deaths associated with hazardous chemicals', 'illness associated with hazardous chemicals', 'deaths associated with water contamination', 'illness associated with water contamination', 'deaths associated with soil contamination', 'illness associated with soil contamination', 'air pollution associated diseases', 'water contamination associated diseases', 'soil contamination associated diseases', 'soil pollution associated diseases', 'water pollution associated diseases', 'deaths from unsafe water', 'deaths from unsafe sanitation', 'deaths from lack of hygiene', 'Deaths attributable to unsafe water', 'Deaths attributable to unsafe sanitation', 'Deaths attributable to unsafe hygiene', 'Environmental health']</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2282,6 +2527,11 @@
           <t>C030a01</t>
         </is>
       </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>['tobacco control', 'decrease smoking prevalence', 'reduce tobacco use', 'reduce cigarette consumption', 'lower tobacco use', 'lower cigarette consumption']</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2319,6 +2569,11 @@
           <t>C030b01</t>
         </is>
       </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>['vaccination research', 'vaccine development', 'basic health research', 'aid to health', 'official development assistance for medical research', 'european medicines agency', 'support for health and climate-related research', 'support for health research', 'innovative protective measures, virology, vaccines', 'research and development of vaccines and medicines', 'research of vaccines', 'research of medicines', 'development of vaccines', 'development of medicines', 'medicines for developing countries', 'vaccines for developing countries', 'official development assistance for health', 'official development assistance for basic health', 'pharmaceutical research', 'development of pharmaceutical products', 'research for pharmaceutical', 'EMA']</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2356,6 +2611,11 @@
           <t>C030b02</t>
         </is>
       </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>['vaccination research', 'vaccine development', 'basic health research', 'aid to health', 'official development assistance for medical research', 'european medicines agency', 'support for health and climate-related research', 'support for health research', 'innovative protective measures, virology, vaccines', 'research and development of vaccines and medicines', 'research of vaccines', 'research of medicines', 'development of vaccines', 'development of medicines', 'medicines for developing countries', 'vaccines for developing countries', 'official development assistance for health', 'official development assistance for basic health', 'pharmaceutical research', 'development of pharmaceutical products', 'research for pharmaceutical', 'EMA']</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2393,6 +2653,11 @@
           <t>C030b03</t>
         </is>
       </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>['vaccination research', 'vaccine development', 'basic health research', 'aid to health', 'official development assistance for medical research', 'european medicines agency', 'support for health and climate-related research', 'support for health research', 'innovative protective measures, virology, vaccines', 'research and development of vaccines and medicines', 'research of vaccines', 'research of medicines', 'development of vaccines', 'development of medicines', 'medicines for developing countries', 'vaccines for developing countries', 'official development assistance for health', 'official development assistance for basic health', 'pharmaceutical research', 'development of pharmaceutical products', 'research for pharmaceutical', 'EMA']</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2430,6 +2695,11 @@
           <t>C030c01</t>
         </is>
       </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>['increase health financing in developing countries', 'increase health workforce in developing countries']</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2467,6 +2737,11 @@
           <t>C030d01</t>
         </is>
       </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>['international health regulations', 'health emergency', 'public health capacity', 'health inequities', 'health system', 'national health risks', 'health risk management', 'health risk reduction', 'health risk warning', 'health risk assessment', 'public health', 'safety risk to human health', 'elimination of a risk to health', 'avoidance of a risk to health', 'health surveillance', 'health risk', 'reduction of disease risk', 'reduces a risk factor in the development of a human disease', 'risks to human health', 'impact on human health', ' effects on human health', 'react to future health crises', 'react to health crises', 'prepare for future health crises', 'health crisis prevention', 'manage health crisis', 'risk communication framework', 'disease prevention', 'health system resilience']</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2504,6 +2779,11 @@
           <t>C030d02</t>
         </is>
       </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>['international health regulations', 'health emergency', 'public health capacity', 'health inequities', 'health system', 'national health risks', 'health risk management', 'health risk reduction', 'health risk warning', 'health risk assessment', 'public health', 'safety risk to human health', 'elimination of a risk to health', 'avoidance of a risk to health', 'health surveillance', 'health risk', 'reduction of disease risk', 'reduces a risk factor in the development of a human disease', 'risks to human health', 'impact on human health', ' effects on human health', 'react to future health crises', 'react to health crises', 'prepare for future health crises', 'health crisis prevention', 'manage health crisis', 'risk communication framework', 'disease prevention', 'health system resilience']</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2541,6 +2821,11 @@
           <t>C040101</t>
         </is>
       </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>['primary completion rate', 'primary school completion rate', 'free primary education', 'free secondary education', 'minimum proficiency level', 'effective learning outcomes', 'compulsory education', 'prevent early school leaving', 'free primary school', 'children out of school', 'out-of-school children', 'progress in primary school enrolment', 'Completion rate primary education', 'Completion rate lower secondary education', 'Completion rate upper secondary education', 'Completion rate secondary education', 'completion rate of education', 'early school leavers', 'out-of-school', 'learning conditions']</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2578,6 +2863,11 @@
           <t>C040102</t>
         </is>
       </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>['primary completion rate', 'primary school completion rate', 'free primary education', 'free secondary education', 'minimum proficiency level', 'effective learning outcomes', 'compulsory education', 'prevent early school leaving', 'free primary school', 'children out of school', 'out-of-school children', 'progress in primary school enrolment', 'Completion rate primary education', 'Completion rate lower secondary education', 'Completion rate upper secondary education', 'Completion rate secondary education', 'completion rate of education', 'early school leavers', 'out-of-school', 'learning conditions']</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2615,6 +2905,11 @@
           <t>C040201</t>
         </is>
       </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>['learning services for children', 'childhood development', 'pre primary education', 'early childhood education', 'children development', 'learning process for children', 'nursery education', 'family-day care', 'pre-primary provision', 'compulsory school starting age', 'early childhood learning', 'ensure that all children have access to basic services like health and education', 'children early learning', 'Early childhood and primary education', 'support children’s early cognitive development', 'support children’s cognitive development', 'support children’s early development', 'early childhood development', 'children developmentally on track', 'completion rate for upper-secondary education']</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2652,6 +2947,11 @@
           <t>C040202</t>
         </is>
       </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>['learning services for children', 'childhood development', 'pre primary education', 'early childhood education', 'children development', 'learning process for children', 'nursery education', 'family-day care', 'pre-primary provision', 'compulsory school starting age', 'early childhood learning', 'ensure that all children have access to basic services like health and education', 'children early learning', 'Early childhood and primary education', 'support children’s early cognitive development', 'support children’s cognitive development', 'support children’s early development', 'early childhood development', 'children developmentally on track', 'completion rate for upper-secondary education']</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2689,6 +2989,11 @@
           <t>C040301</t>
         </is>
       </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>['tertiary education', 'adult participation in learning', 'participation in formal education', 'participation in non-formal education', 'participation in training', 'access to universities', 'adult education', 'adult formal education', 'adult training', 'Lifelong training', 'lifelong education', 'lifelong learning']</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2726,6 +3031,11 @@
           <t>C040401</t>
         </is>
       </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>['technical skills', 'vocational skills', 'skills for employment', 'digital skills', 'ICT skills', 'technology skills', 'skill training', 'vocational training', ' vocational education', 'upgrading of skills', 'skills adjusted to labour market', 'reskilling', 'upskilling', 'skills for job', 'skills for labour market', 'digital literacy', 'up-skilling', 'TVET', 'skills development', 'skilled labour', 'quality skills', 'human capital development', 'new skills', 'E-learning', 'labour market demand']</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2763,6 +3073,11 @@
           <t>C040501</t>
         </is>
       </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>['equal access to education', 'quality education and training for disadvantaged groups', 'education for indigenous', 'education for all', 'education for disadvantaged', 'education for vulnerable', 'gender equality in education', 'education for persons with disabilities', 'parity of education', 'education socially inclusive', 'training socially inclusive', 'inclusive education', 'educational inequalities', 'education is inclusive', 'equal access to high-quality education', 'parity in primary education', 'parity in secondary education', 'parity in tertiary education', 'parity in university', 'inequalities in education', 'disparity in education', 'gender discrepancy in education', 'gender discrepancy in terms of education', 'education for gender equality', 'remove barriers to education', 'inclusive schools', 'right to education', 'discrimination in education', 'right to common education']</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2800,6 +3115,11 @@
           <t>C040601</t>
         </is>
       </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>['numeracy', 'language proficiency', 'underachievement in reading', 'reading skills', 'reading proficiency', 'math proficiency', 'mathematical proficiency', 'math skills', 'mathematical skills', 'underachiever in mathematics', 'proficiency standards in reading', 'proficiency standards in mathematics', 'reduce illiterate', 'proficiency in reading', 'proficiency in math', 'functionally literate', 'increase literacy']</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2837,6 +3157,11 @@
           <t>C200306</t>
         </is>
       </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>['global citizenship education', 'sustainable development skills', 'human rights education', 'sustainable development in teacher education', 'sustainable development in national education', 'culture of peace', 'respect of cultural diversity', 'sustainable development in curricula', 'sustainability education', 'sustainability learning', 'education sustainability', 'learning sustainability', 'competences for sustainable development', 'education for sustainable development', 'skills for sustainable development', 'training on sustainable development', 'teach sustainable development', 'teacher of sustainable development', 'education for sustainable lifestyle', 'skills for sustainable lifestyle', 'training on sustainable lifestyle', 'teach sustainable lifestyle', 'teacher of sustainable lifestyle', 'learn sustainable development', 'learn sustainable lifestyle', 'education for human rights', 'training on human rights', 'teach human rights', 'teacher of human rights', 'learn human rights', 'education for peace', 'education for global citizenship', 'teach global citizenship', 'learn global citizenship', 'culture of sustainable development', 'culture of sustainable lifestyle', 'awareness of sustainable lifestyle', 'education for environmental sustainability', 'inclusive teaching', 'inclusive training course for teaching staff']</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2874,6 +3199,11 @@
           <t>C040a01</t>
         </is>
       </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>['education facilities', 'safe learning environment', 'inclusive learning environment', 'effective learning environment', 'sanitation in school', 'electricity in school', 'internet in school', 'drinking water in school', 'schools offering basic services', 'schools with basic resources', 'schools with drinking water', 'schools with electricity', 'schools with computers', 'schools with Internet', 'schools with sanitation', 'schools with access to electricity', 'schools with access to Internet', 'school with basic handwashing facilities', 'school with handwashing facilities', ' handwashing facilities in school', 'internet for teaching', 'internet accessible by pupils', 'students can access to internet', 'internet access students', 'internet for students', 'computer for teaching', 'computer for learning', 'computer in school', 'Accessible learning materials', 'access in schools to key basic services', 'access in schools to basic services', 'access in schools to facilities']</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2911,6 +3241,11 @@
           <t>C040b01</t>
         </is>
       </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>['scholarship', 'improve access to higher education', 'increase access to higher education', 'financial aid awards for individual students', 'financial aid for students', 'financial contributions to trainees', 'financial contributions to study', 'financial contributions for students', 'economic aid for students', 'economic aid to study', 'grants to students', 'grant for studying', 'grant for learning', 'official development assistance for studying', 'official development assistance for learning', 'official development assistance for school', 'official development assistance for education', 'ODA for education', 'ODA for school', 'Erasmus']</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2948,6 +3283,11 @@
           <t>C040c01</t>
         </is>
       </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>['qualified teacher', 'skilled teacher', 'teacher education', 'teacher training', 'development of teaching staff', 'train teachers', 'educate teachers', 'adequate teacher', 'well-trained teachers', 'well-trained to teach', 'training for teaching', 'teachers with the minimum required qualifications']</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2985,6 +3325,11 @@
           <t>C050101</t>
         </is>
       </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>['woman discrimination', 'gender discrimination', 'women discrimination', 'discrimination for women', 'discrimination for woman', 'discrimination for girls', 'discrimination faced by girls', 'discrimination faced by women', 'discrimination faced by woman', 'girls are deprived', 'women are deprived', 'woman  deprived', 'women discriminated', 'woman discriminated', 'girls discriminated', 'discriminated women', 'discriminated woman', 'discriminated girls', 'discrimination on the basis of sex', 'discrimination by sex', 'discrimination on the basis of gender', 'discrimination by gender', 'equal treatment women']</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3022,6 +3367,11 @@
           <t>C050201</t>
         </is>
       </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>['gender violence', 'violence against woman', 'violence against girls', 'gender-based violence', 'marital violence', 'violence within marriage', 'dowry-related death', 'sexual harassment', 'rape victim', 'intimate partner violence', 'rape women', 'women rape', 'violence against women', 'abuse women', 'women abuse', 'abuse woman', 'woman abuse', 'rape woman', 'woman rape', 'protect women from violence', 'protect woman from violence', 'marital rape', 'women sexually assaulted', 'woman sexually assaulted', 'domestic violence']</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3059,6 +3409,11 @@
           <t>C050202</t>
         </is>
       </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>['gender violence', 'violence against woman', 'violence against girls', 'gender-based violence', 'marital violence', 'violence within marriage', 'dowry-related death', 'sexual harassment', 'rape victim', 'intimate partner violence', 'rape women', 'women rape', 'violence against women', 'abuse women', 'women abuse', 'abuse woman', 'woman abuse', 'rape woman', 'woman rape', 'protect women from violence', 'protect woman from violence', 'marital rape', 'women sexually assaulted', 'woman sexually assaulted', 'domestic violence']</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3096,6 +3451,11 @@
           <t>C050301</t>
         </is>
       </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>['forced marriage', 'fgm', 'female genital mutilation', 'child marriage', 'forced into early marriage', 'genital cutting', 'marrying in childhood', 'Marriage before the age of']</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3133,6 +3493,11 @@
           <t>C050302</t>
         </is>
       </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>['forced marriage', 'fgm', 'female genital mutilation', 'child marriage', 'forced into early marriage', 'genital cutting', 'marrying in childhood', 'Marriage before the age of']</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3170,6 +3535,11 @@
           <t>C050401</t>
         </is>
       </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>['unpaid domestic work', 'unpaid care', 'shared household responsibility', 'sharing family responsibility', 'responsibility shared household', 'Unpaid domestic services']</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3207,6 +3577,11 @@
           <t>C050501</t>
         </is>
       </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>['women in leading positions', 'women in managerial positions', 'women in management positions', 'women in parliament', 'women in top position', 'female CEO', 'female boss', 'women in government', 'women leading', 'leading women', 'women are serving in parliament', 'women in positions of leadership', 'women leadership', 'women’s representation in policy', 'women’s representation politics', 'woman in leading positions', 'woman in managerial positions', 'woman in management positions', 'woman in parliament', 'woman in top position', 'woman in government', 'woman leading', 'leading woman', 'woman serving in parliament', 'woman in positions of leadership', 'woman leadership', 'woman’s representation in the political', 'woman’s representation in policy', 'women in political leadership', 'woman in political leadership', 'woman in political offices', 'women in political offices', 'seats held by women', 'positions held by women', 'females employed in decision-making', 'females employed in management roles', 'women who are employed in decision-making', 'women employed in management roles', 'woman employed in decision-making', 'woman employed in management roles', 'women in decision-making', 'women in management roles', 'woman in decision-making', 'woman in management roles', 'gender balance on company boards', 'female-led households']</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3244,6 +3619,11 @@
           <t>C050502</t>
         </is>
       </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>['women in leading positions', 'women in managerial positions', 'women in management positions', 'women in parliament', 'women in top position', 'female CEO', 'female boss', 'women in government', 'women leading', 'leading women', 'women are serving in parliament', 'women in positions of leadership', 'women leadership', 'women’s representation in policy', 'women’s representation politics', 'woman in leading positions', 'woman in managerial positions', 'woman in management positions', 'woman in parliament', 'woman in top position', 'woman in government', 'woman leading', 'leading woman', 'woman serving in parliament', 'woman in positions of leadership', 'woman leadership', 'woman’s representation in the political', 'woman’s representation in policy', 'women in political leadership', 'woman in political leadership', 'woman in political offices', 'women in political offices', 'seats held by women', 'positions held by women', 'females employed in decision-making', 'females employed in management roles', 'women who are employed in decision-making', 'women employed in management roles', 'woman employed in decision-making', 'woman employed in management roles', 'women in decision-making', 'women in management roles', 'woman in decision-making', 'woman in management roles', 'gender balance on company boards', 'female-led households']</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3281,6 +3661,11 @@
           <t>C050601</t>
         </is>
       </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>['reproductive rights', 'sex education', 'freedom for women in sexual relations', 'freedom for woman in sexual relations']</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3318,6 +3703,11 @@
           <t>C050602</t>
         </is>
       </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>['reproductive rights', 'sex education', 'freedom for women in sexual relations', 'freedom for woman in sexual relations']</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3355,6 +3745,11 @@
           <t>C050a01</t>
         </is>
       </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>['land rights for women', 'women owned business', 'womens right to land', 'womens property rights', 'female property ownership', 'womens property', 'female land ownership', 'women land ownership', 'gender discrimination in land ownership', 'land rights for woman', 'woman owned business', 'womans right to land', 'womans property rights', 'womens land', 'woman land ownership', 'inheritance rights for woman', 'inheritance rights for women', 'women inheritance rights', 'woman inheritance rights', 'give women equal rights land', 'give women equal rights property', 'gender balance on ownership over agricultural land', 'gender balance on tenure rights over agricultural land', 'gender balance over agricultural land', 'woman owning land', 'women owning land', 'women equal rights to land']</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3392,6 +3787,11 @@
           <t>C050a02</t>
         </is>
       </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>['land rights for women', 'women owned business', 'womens right to land', 'womens property rights', 'female property ownership', 'womens property', 'female land ownership', 'women land ownership', 'gender discrimination in land ownership', 'land rights for woman', 'woman owned business', 'womans right to land', 'womans property rights', 'womens land', 'woman land ownership', 'inheritance rights for woman', 'inheritance rights for women', 'women inheritance rights', 'woman inheritance rights', 'give women equal rights land', 'give women equal rights property', 'gender balance on ownership over agricultural land', 'gender balance on tenure rights over agricultural land', 'gender balance over agricultural land', 'woman owning land', 'women owning land', 'women equal rights to land']</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3429,6 +3829,11 @@
           <t>C050b01</t>
         </is>
       </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>['women in technology', 'women in tech', 'gender and technology', 'technology and women', 'female tech leader', 'women techmakers', 'ict women', 'women ict', 'gender ict', 'ict gender', 'woman in technology', 'woman in tech', 'technology and woman', 'woman techmakers', 'ict woman', 'woman ict', 'mobile phone for women', 'mobile phone for girls', 'women with mobile phones', 'girls with mobile phones']</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3466,6 +3871,11 @@
           <t>C050c01</t>
         </is>
       </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>['gender laws', 'gender-neutral legislation', 'gender-sensitive legislation', 'gender-relevant legislation', 'gender legislation', 'public allocations for gender equality', 'laws gender', 'equality in law for women', 'women business and the law', 'women and law', 'gender equality law', 'gender equality legislation', 'law gender equality', 'equality in law for woman', 'discriminatory laws for women', 'discriminatory laws for woman', 'legislation on domestic violence', 'laws protecting women', 'address the way laws impact the decisions women take', 'give women and men equal legal rights', 'give men and women equal legal rights', 'gender approach in legislation', 'gender approach in policy', 'integrate gender in legislation', 'integrate gender in policy', 'gender mainstreaming', 'mainstreaming gender', 'gender sensitive legislation', 'gender sensitive policy', 'gender sensitive budget', 'gender budgeting']</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3503,6 +3913,11 @@
           <t>C060101</t>
         </is>
       </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>['safe drinking water', 'drinking water access', 'affordable drinking water', 'access to drinking water', 'dwindling drinking water', 'water insecurity', 'drinking water stress', 'freshwater resources', 'drinking water services', 'improved drinking water source', 'basins where water use exceeds recharge', 'availability of water', 'recurring water shortages', 'safely-managed drinking water', 'shortfall in freshwater resources', 'water crisis', 'Drinking water supply']</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3540,6 +3955,11 @@
           <t>C060201</t>
         </is>
       </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>['equitable sanitation', 'washing facility', 'access to sanitation', 'equitable hygiene', 'cleaning facilities', 'open defecation', 'sanitation service', 'ensure sanitation', 'hand hygiene', 'handwashing', 'WASH services', 'basic water, sanitation and hygiene facilities', 'basic water services', 'safely managed sanitation facilities', 'access to toilets', 'access to latrines', 'inadequate sanitation', 'lack of access to sanitised water', 'adequately disposed excreta', 'adequately treated excreta', 'safe sanitation', 'sanitary facilities', 'urban sanitation', 'sanitation infrastructure', 'sanitary conditions', 'adequate sanitation']</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3577,6 +3997,11 @@
           <t>C060303</t>
         </is>
       </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>['water quality', 'wastewater treatment', 'waste water treatment', ' waste water management', 'untreated waste water', 'untreated wastewater', 'water pollution', 'nitrate in rivers', 'phosphate in rivers', 'reclaimed water', 'recycled water', 'pollution of surface water', 'pollution of water', 'pollution of groundwater', 'pollution of the aquatic environment', 'safeguard zones for surface and groundwater', 'clean water', 'lack of running water', 'untreated water', 'wastewater discharged into rivers without pollution removal', 'wastewater discharged into sea without pollution removal', 'wastewater management', 'degradation of water resources', 'water treatment projects', 'water treatment plant', 'recycling of treated water']</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3614,6 +4039,11 @@
           <t>C060302</t>
         </is>
       </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>['water quality', 'wastewater treatment', 'waste water treatment', ' waste water management', 'untreated waste water', 'untreated wastewater', 'water pollution', 'nitrate in rivers', 'phosphate in rivers', 'reclaimed water', 'recycled water', 'pollution of surface water', 'pollution of water', 'pollution of groundwater', 'pollution of the aquatic environment', 'safeguard zones for surface and groundwater', 'clean water', 'lack of running water', 'untreated water', 'wastewater discharged into rivers without pollution removal', 'wastewater discharged into sea without pollution removal', 'wastewater management', 'degradation of water resources', 'water treatment projects', 'water treatment plant', 'recycling of treated water']</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3651,6 +4081,11 @@
           <t>C060401</t>
         </is>
       </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>['water exploitation index', 'water-use efficiency', 'sustainable water', 'efficient water', 'water stress', 'freshwater withdrawal', 'available freshwater', ' water scarcity', 'scarce water', 'water resource efficiency', 'water-saving technologies', 'water saving techniques', 'Water efficiency']</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3688,6 +4123,11 @@
           <t>C060402</t>
         </is>
       </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>['water exploitation index', 'water-use efficiency', 'sustainable water', 'efficient water', 'water stress', 'freshwater withdrawal', 'available freshwater', ' water scarcity', 'scarce water', 'water resource efficiency', 'water-saving technologies', 'water saving techniques', 'Water efficiency']</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3725,6 +4165,11 @@
           <t>C060501</t>
         </is>
       </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>['water resource management', 'integrated water resource', 'transboundary basin', 'water cooperation', 'water management', 'sustainable management of water', 'watershed management', 'reliable irrigation', 'equitable use of water', 'water catchment area']</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3762,6 +4207,11 @@
           <t>C060502</t>
         </is>
       </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>['water resource management', 'integrated water resource', 'transboundary basin', 'water cooperation', 'water management', 'sustainable management of water', 'watershed management', 'reliable irrigation', 'equitable use of water', 'water catchment area']</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3799,6 +4249,11 @@
           <t>C060601</t>
         </is>
       </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>['protect wetlands', 'wetland protection', 'river protection', 'protect rivers', 'water basin protection', 'water-related ecosystem', 'protect water resource', 'restore water', 'draining wetland', 'natural wetlands lost', 'restore wetlands', 'restore freshwater ecosystems', 'restore river', 'river restored', 'restore floodplains', 'floodplains restored']</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3836,6 +4291,11 @@
           <t>C060a01</t>
         </is>
       </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>['water oda', 'water-related oda', 'water-related official development assistance', 'sanitation-related oda', ' sanitation-related official development assistance', 'water programmes in developing countries', 'sanitation in developing countries', 'water harvesting in developing countries', ' water efficiency in developing countries', 'official development assistance for water projects']</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3873,6 +4333,11 @@
           <t>C060b01</t>
         </is>
       </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>['local communities in water', 'community water management', 'community water system', 'community sanitation', 'community-led sanitation', 'community-led water', 'local water management', 'local water strategy', 'local water policy', 'managing local water', 'local management of water']</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3910,6 +4375,11 @@
           <t>C070101</t>
         </is>
       </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>['energy access', 'electricity access', 'access to energy', 'access to electricity', 'modern energy', 'access to affordable, reliable and modern energy', 'energy for all', 'energy-poor country', 'stand-alone energy services', 'energy security', 'affordable energy', 'widely available energy', 'increase electrification', 'access to clean cooking fuels', 'limited electricity', 'reliable electricity', 'unreliable electricity', 'access to power', 'uninterrupted energy', 'scarce energy resources', 'energy supply needs to be secure and affordable', 'energy supply secure and affordable', 'energy supply affordable', 'keep home adequately warm', 'reduce energy poverty', 'electricity grids', 'mini-grids', 'micropower plants', 'energy wood', 'charcoal reduction', 'electricity generation', 'power plants', 'clean cooking', 'modern cooking systems']</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3947,6 +4417,11 @@
           <t>C070102</t>
         </is>
       </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>['energy access', 'electricity access', 'access to energy', 'access to electricity', 'modern energy', 'access to affordable, reliable and modern energy', 'energy for all', 'energy-poor country', 'stand-alone energy services', 'energy security', 'affordable energy', 'widely available energy', 'increase electrification', 'access to clean cooking fuels', 'limited electricity', 'reliable electricity', 'unreliable electricity', 'access to power', 'uninterrupted energy', 'scarce energy resources', 'energy supply needs to be secure and affordable', 'energy supply secure and affordable', 'energy supply affordable', 'keep home adequately warm', 'reduce energy poverty', 'electricity grids', 'mini-grids', 'micropower plants', 'energy wood', 'charcoal reduction', 'electricity generation', 'power plants', 'clean cooking', 'modern cooking systems']</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3984,6 +4459,11 @@
           <t>C070201</t>
         </is>
       </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>['clean energy', 'renewable energy', 'energy mix', 'green energy', 'access to clean fuels', 'clean hydrogen', 'hydropower', 'hydraulic energy', 'wind energy', 'solar energy', 'hydroenergy production', 'eco-friendly energy', 'thermal power', 'solar power', 'unhealthy fuels', 'polluting fuels', 'power generated through renewable sources', 'solar panels', 'new solar systems', 'renewable power capacity', 'wind turbines', 'decarbonise energy', 'renewable energy generation', 'share of renewables', 'off-grid renewable', 'renewable energy sources', 'hydroelectric', 'wind power']</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4021,6 +4501,11 @@
           <t>C070301</t>
         </is>
       </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>['energy productivity', 'energy efficiency', 'energy consumption', 'energy intensity', 'inefficient energy solutions', 'energy potential', 'energy saving', 'energy efficient production modes', 'energy efficient technologies', 'energy efficient buildings', 'efficient energy solutions']</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4058,6 +4543,11 @@
           <t>C070a01</t>
         </is>
       </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>['clean energy research', 'clean energy technology', 'international cooperation for energy', 'financing energy', 'financing clean energy', 'renewable energy in developing countries', 'energy efficiency in developing countries', 'investment in energy in developing countries', 'hybrid systems in developing countries', 'energy preparedness', 'clean energy investments', 'development of the energy sector', 'investments in electricity generation', ' investments in electricity transmission', 'renewable energy investment projects', 'energy access partnership']</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4095,6 +4585,11 @@
           <t>C200208</t>
         </is>
       </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>['sustainable energy in developing countries', 'sustainable energy in LDCs', 'Investments in energy efficiency in developing countries', 'clean energy in developing countries', 'developing countries clean energy', 'developing countries sustainable energy', 'energy services in developing countries', 'electricity access in developing countries', 'electricity in developing countries', 'energy independence developing countries', 'energy independence third world', 'sustainable local energy developing countries', 'clean energy sovereignty third world', 'clean energy sovereignty developing countries', 'clean energy sovereignty developing nations', 'clean energy sovereignty ldc', 'clean energy sovereignty least developed', 'sustainable local energy third world', 'sustainable local energy developing nations', 'sustainable local energy ldc', 'sustainable local energy least developed countries']</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4132,6 +4627,11 @@
           <t>C080101</t>
         </is>
       </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>['economic growth', 'economic development', 'gdp growth', 'growth rate of real gdp', 'growth rate of gdp', 'gross domestic product growth', 'gross added value', 'growth and jobs', 'inclusive growth', 'sustainable growth', 'productive sectors growth']</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4169,6 +4669,11 @@
           <t>C080201</t>
         </is>
       </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>['economic productivity', 'technological innovation', 'innovation union', 'technological progress', 'innovation and growth', 'competitiveness and innovation', 'innovation and competitiveness', 'improves economic performance', 'gains in productivity', 'boost productivity', 'improve productivity', 'productivity increase']</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4206,6 +4711,11 @@
           <t>C080302</t>
         </is>
       </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>['job creation', 'creates quality jobs', 'entrepreneurship', 'support entrepreneurs', 'support productive activities', 'non‑agriculture employment', 'increase employment', 'new jobs', 'finance for enterprises', 'jobs and growth', 'creation job', 'encourage enterprises to be innovative', 'support for small and medium-sized enterprises', 'helping SMEs', 'help small and medium-sized enterprises', 'support to SMEs', 'creative jobs', 'sustainable jobs', 'emerging industry jobs', 'jobs in innovative sectors', 'access jobs', ' job-rich recovery', 'workers living in extreme poverty', 'stimulate business environment', 'stimulate investment climate', 'stimulate business climate', 'Ease of Doing Business Index', 'economic freedom', 'support to Micro, Small and Medium Enterprises', 'support to MSME', 'private sectors organizations promotion', 'private sector development', 'supporting private SMEs', 'private sector advocacy', 'capital markets', 'regulatory framework for SMEs development', 'help entrepreneurs', 'create business climate', 'create business environment', 'create investment climate', 'support innovation of SMEs', 'support innovation of enterprise', 'support innovation of Small and medium sized ']</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4243,6 +4753,11 @@
           <t>C200202</t>
         </is>
       </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>['decouple economic growth', 'improve resource efficiency', 'material footprint', 'material consumption', 'resource productivity', 'green growth', 'climate-resilient growth', 'economic growth decoupled from resource use', 'resource efficiency in consumption and production']</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4280,6 +4795,11 @@
           <t>C200203</t>
         </is>
       </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>['decouple economic growth', 'improve resource efficiency', 'material footprint', 'material consumption', 'resource productivity', 'green growth', 'climate-resilient growth', 'economic growth decoupled from resource use', 'resource efficiency in consumption and production']</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4317,6 +4837,11 @@
           <t>C080501</t>
         </is>
       </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>['full employment', 'productive employment', 'decent work', 'unemployment', 'inclusive employment', 'equal pay', 'high-skilled employment', 'help most vulnerable to return to the labour', 'quality employment', 'minimum wage', 'fair working conditions', 'gender pay gap', 'gender balanced labour market', 'decent job', 'inclusive job', 'quality job', 'job creation for the most vulnerable', 'creation of job opportunities', 'decent labour', 'protecting jobs', 'women participation in the labour force', 'informal employment', 'underutilized women in the labour force', 'help women make steady incomes', 'vocational rehabilitation', 'employment of people with disabilities', 'recruitment of persons with disabilities', 'Decent employment', 'access to employment', 'unpaid work', 'underutilised women in the labour force', 'poor job search skills']</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4354,6 +4879,11 @@
           <t>C080502</t>
         </is>
       </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>['full employment', 'productive employment', 'decent work', 'unemployment', 'inclusive employment', 'equal pay', 'high-skilled employment', 'help most vulnerable to return to the labour', 'quality employment', 'minimum wage', 'fair working conditions', 'gender pay gap', 'gender balanced labour market', 'decent job', 'inclusive job', 'quality job', 'job creation for the most vulnerable', 'creation of job opportunities', 'decent labour', 'protecting jobs', 'women participation in the labour force', 'informal employment', 'underutilized women in the labour force', 'help women make steady incomes', 'vocational rehabilitation', 'employment of people with disabilities', 'recruitment of persons with disabilities', 'Decent employment', 'access to employment', 'unpaid work', 'underutilised women in the labour force', 'poor job search skills']</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4391,6 +4921,11 @@
           <t>C080601</t>
         </is>
       </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>['unemployment among youth', 'youth employment', 'youth unemployment', 'youth training', 'youth work', 'jobs for youth', 'young people employed', 'young people unemployed', 'help young people get into work', 'young people aged 15 to 29 not in employment, education or training', 'education for insertion into the labour market', 'NEET', 'helped 3.5 million young people a year to get in training, education or work', 'help young people to get in training, education or work', 'young people not in employment, education or training']</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4428,6 +4963,11 @@
           <t>C080701</t>
         </is>
       </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>['forced labour', 'child labour', 'forced slavery', 'human trafficking', 'child soldier', ' child domestic workers', 'protection of children affected by armed conflict', 'prevention of recruitment of minors', 'recruitment of youth by extremists groups']</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4465,6 +5005,11 @@
           <t>C080801</t>
         </is>
       </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>['labour right', 'safe working', 'secure working', 'precarious employment', 'occupational injuries', 'occupational accidents', 'accidents at work', 'collective bargaining', 'labour union', 'employee rights', 'health and safety requirements', 'health and safety of workers', 'health protection of workers', 'health and safety resulting from workplace', 'health surveillance of workers', "protection of workers' health", 'protection of workers against risks to their health', 'health requirements for work', ' health relating to workstation', 'workers’ safety and health', 'health of workers', 'safety and health of workers', 'occupational health', 'health and safety requirements regarding the exposure of workers to the risks', 'exposure of workers to the risks', 'workers’ health', 'health of exposed workers', 'protection for all workers', 'health at work', 'Health Protection at Work', 'health and safety conditions of the work', 'protection of the health and safety of workers', 'safety requirements at the workplace', 'protection of labour', 'labour standard', 'improving the labour conditions', 'workers’ rights']</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4502,6 +5047,11 @@
           <t>C080802</t>
         </is>
       </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>['labour right', 'safe working', 'secure working', 'precarious employment', 'occupational injuries', 'occupational accidents', 'accidents at work', 'collective bargaining', 'labour union', 'employee rights', 'health and safety requirements', 'health and safety of workers', 'health protection of workers', 'health and safety resulting from workplace', 'health surveillance of workers', "protection of workers' health", 'protection of workers against risks to their health', 'health requirements for work', ' health relating to workstation', 'workers’ safety and health', 'health of workers', 'safety and health of workers', 'occupational health', 'health and safety requirements regarding the exposure of workers to the risks', 'exposure of workers to the risks', 'workers’ health', 'health of exposed workers', 'protection for all workers', 'health at work', 'Health Protection at Work', 'health and safety conditions of the work', 'protection of the health and safety of workers', 'safety requirements at the workplace', 'protection of labour', 'labour standard', 'improving the labour conditions', 'workers’ rights']</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4539,6 +5089,11 @@
           <t>C080901</t>
         </is>
       </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>['impact of sustainable tourism', 'monitoring sustainable tourism', 'evaluate sustainable tourism', 'sustainable tourism evaluation', 'sustainable tourism monitoring', 'plan for sustainable tourism', 'eco-tourism', 'culture linked to tourism', 'agri-tourism', 'green tourism', 'inclusive tourism', 'responsible tourism', 'responsible ecotourism', 'promote local culture', 'promote local products']</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4576,6 +5131,11 @@
           <t>C081001</t>
         </is>
       </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>['access to banking', 'access to financial service', 'access to insurance', 'commercial bank branches', 'number of atm', 'automated teller machines', 'mobile money service', 'bank account', 'financial inclusion', 'access to credit and financial services', 'financial service providers', 'microfinance', 'micro-credit']</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4613,6 +5173,11 @@
           <t>C081002</t>
         </is>
       </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>['access to banking', 'access to financial service', 'access to insurance', 'commercial bank branches', 'number of atm', 'automated teller machines', 'mobile money service', 'bank account', 'financial inclusion', 'access to credit and financial services', 'financial service providers', 'microfinance', 'micro-credit']</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4650,6 +5215,11 @@
           <t>C080a01</t>
         </is>
       </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>['aid for trade', 'aid for disbursement', 'trade-related technical assistance', 'trade-related assistance', 'trade-related direct foreign investment', 'FDI for trade', 'trade policy development support']</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4687,6 +5257,11 @@
           <t>C080b01</t>
         </is>
       </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>['strategy for youth employment', 'policy for youth employment', 'global jobs pact', 'youth employment strategy', 'increase professional abilities of the youth', 'increase the employability of the youth', 'youth unemployment rise', 'opportunities for youth to enter the labour market', 'enabling youth entrepreneurship', 'enhancing youth entrepreneurship', 'empowering youth', 'reinforcing youth participation', 'reinforcing youth leadership', 'opportunities for youth employment', 'enhancing youth employability', 'creating opportunities for youth', 'creating incentives for entrepreneurship for youth', 'creating incentives for innovation for youth', 'employment opportunities for the youth', 'instrument to fight youth unemployment', 'youth employment policy']</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4724,6 +5299,11 @@
           <t>C090101</t>
         </is>
       </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>['quality infrastructure', 'resilient infrastructure', 'sustainable infrastructure', 'reliable infrastructure', 'all-season road', 'transborder infrastructure', 'regional infrastructure', 'inland waterways', 'passenger transport', 'freight transport', 'transport infrastructure', 'infrastructure providing basic services', 'enhancement of basic infrastructure', 'infrastructure gaps', 'chronic infrastructure deficit', 'transport system and infrastructure']</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4761,6 +5341,11 @@
           <t>C090102</t>
         </is>
       </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>['quality infrastructure', 'resilient infrastructure', 'sustainable infrastructure', 'reliable infrastructure', 'all-season road', 'transborder infrastructure', 'regional infrastructure', 'inland waterways', 'passenger transport', 'freight transport', 'transport infrastructure', 'infrastructure providing basic services', 'enhancement of basic infrastructure', 'infrastructure gaps', 'chronic infrastructure deficit', 'transport system and infrastructure']</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4798,6 +5383,11 @@
           <t>C090201</t>
         </is>
       </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>['inclusive industrialisation', 'sustainable industrialization', 'manufacturing value', 'high technology employment', 'medium technology employment', 'employment in high technology', 'employment in medium technology', 'manufacturing industry', 'industrial modernization', 'industrial modernisation', 'manufacturing employment', 'construction of industrial parks', 'solar industry', 'clean industry', 'cultural industries', 'creative industries', 'sustainable industrialisation', 'inclusive industrialization']</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -4835,6 +5425,11 @@
           <t>C090202</t>
         </is>
       </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>['inclusive industrialisation', 'sustainable industrialization', 'manufacturing value', 'high technology employment', 'medium technology employment', 'employment in high technology', 'employment in medium technology', 'manufacturing industry', 'industrial modernization', 'industrial modernisation', 'manufacturing employment', 'construction of industrial parks', 'solar industry', 'clean industry', 'cultural industries', 'creative industries', 'sustainable industrialisation', 'inclusive industrialization']</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4872,6 +5467,11 @@
           <t>C090301</t>
         </is>
       </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>['small scale industry', 'small enterprises and financial services', 'access to finance small scale industry', 'access to finance industry', 'industry access to finance', 'credit small scale indsutry', 'small scale industry access to credit', 'small scale industry credit', 'financial instrument supporting Union enterprises', 'financial instrument to support enterprises', 'financial instrument for enterprises', 'financial instrument for SME', 'loans to expansion and growth-stage enterprises', 'loans for enterprises', 'loans for SME', 'credit for enterprises', 'credit for SME', 'access to finance for rural Micro-Enterprises', 'access to finance for SME', 'SME finance', 'SME credit', 'financial support SME', 'promote SME', 'SME access', 'SME internationalisation', 'funding SME', 'promote transational participation SME', 'provide capacity building to micro and small enterprises', 'provide advice to micro and small enterprises', 'small producers', 'small private businesses', 'small production', 'small cooperatives', 'micro small medium enterprises', 'micro, small and medium-sized enterprises', 'small-scale farmers', 'small business', 'finance market for the innovative companies', 'finance market for SMEs', 'access to finance for MSMEs']</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -4909,6 +5509,11 @@
           <t>C090302</t>
         </is>
       </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>['small scale industry', 'small enterprises and financial services', 'access to finance small scale industry', 'access to finance industry', 'industry access to finance', 'credit small scale indsutry', 'small scale industry access to credit', 'small scale industry credit', 'financial instrument supporting Union enterprises', 'financial instrument to support enterprises', 'financial instrument for enterprises', 'financial instrument for SME', 'loans to expansion and growth-stage enterprises', 'loans for enterprises', 'loans for SME', 'credit for enterprises', 'credit for SME', 'access to finance for rural Micro-Enterprises', 'access to finance for SME', 'SME finance', 'SME credit', 'financial support SME', 'promote SME', 'SME access', 'SME internationalisation', 'funding SME', 'promote transational participation SME', 'provide capacity building to micro and small enterprises', 'provide advice to micro and small enterprises', 'small producers', 'small private businesses', 'small production', 'small cooperatives', 'micro small medium enterprises', 'micro, small and medium-sized enterprises', 'small-scale farmers', 'small business', 'finance market for the innovative companies', 'finance market for SMEs', 'access to finance for MSMEs']</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -4946,6 +5551,11 @@
           <t>C090401</t>
         </is>
       </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>['upgrade infrastructure', 'sustainable industrial process', 'retrofitting', 'retrofit', 'resource-use efficiency', 'upgrade existing infrastructure', 'clean technologies', 'low-emission technologies', 'industry transition to sustainable']</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -4983,6 +5593,11 @@
           <t>C090501</t>
         </is>
       </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>['innovative infrastructure', 'innovative industry', 'industrial innovation', 'industry technology', 'research and development', 'R&amp;D', 'innovative technology', 'green technology', 'Expenditure in Research', 'Expenditure in Innovation', 'personnel employed in RD&amp;I', 'foster innovation', 'Investing in digital infrastructure', 'research and innovation', 'innovation and research', 'Horizon Europe', 'Eurostars', 'EUREKA', 'establish research cells', 'foster research and partnerships', 'set up research partnerships', 'networks for research', 'facilitate innovation', 'foster technological progress', 'foster research cooperation', 'facilitate research cooperation', 'improve research cooperation', 'strengthen research cooperation', 'scientific research', 'science technology and innovation', 'STI', 'Science Technology Research and Innovation']</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5020,6 +5635,11 @@
           <t>C090502</t>
         </is>
       </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>['innovative infrastructure', 'innovative industry', 'industrial innovation', 'industry technology', 'research and development', 'R&amp;D', 'innovative technology', 'green technology', 'Expenditure in Research', 'Expenditure in Innovation', 'personnel employed in RD&amp;I', 'foster innovation', 'Investing in digital infrastructure', 'research and innovation', 'innovation and research', 'Horizon Europe', 'Eurostars', 'EUREKA', 'establish research cells', 'foster research and partnerships', 'set up research partnerships', 'networks for research', 'facilitate innovation', 'foster technological progress', 'foster research cooperation', 'facilitate research cooperation', 'improve research cooperation', 'strengthen research cooperation', 'scientific research', 'science technology and innovation', 'STI', 'Science Technology Research and Innovation']</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5057,6 +5677,11 @@
           <t>C090a01</t>
         </is>
       </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>['international support to infrastructure', 'development assistance to infrastructure', 'infrastructure in developing countries', 'infrastructure development in developing countries', 'developing countries infrastructure', 'oda for rural infrastructure development', 'official development assistance for rural infrastructure']</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5094,6 +5719,11 @@
           <t>C090b01</t>
         </is>
       </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>['research in developing countries', 'innovation in developing countries', 'technology development in developing countries', 'technologies in developing countries', 'industry in developing countries', 'industrial diversification in developing countries', 'research and development developing countries', 'developing countries research and development', 'developing countries technology', 'developing countries innovation', 'R&amp;D in developing countries']</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5131,6 +5761,11 @@
           <t>C090c01</t>
         </is>
       </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>['internet access', 'access to free internet', 'access to information technology', 'access to ICT', 'access to communication technology', 'network coverage', 'access internet', 'ict access', 'information technology access', 'fibre-optic internet', 'internet connectivity', 'internet networks', 'provide free internet', 'affordable internet package', 'making ICT more accessible', 'intercontinental hub for ICT', 'ICT Policy', 'provide ICT classes', 'ICT literacy', 'improvements of the ICT systems', 'ICT in partnership', 'improve communications infrastructure', 'area covered by a mobile network', 'digitalization of businesses and services', 'bridge the digital divide', 'people who remain offline', 'people unable to access online', 'potential of digital technologies', 'reach of a mobile-cellular signal', '3G network in developing countries', 'higher-quality network', 'equal access to information and knowledge', 'optic fibre in ldc', 'broadband in ldc', '4G network in ldc', '5G network in ldc', 'optic fibre in least developed countries', 'broadband in least developed countries', 'optic fibre in developing countries', 'broadband in developing countries', '3G network in least developed countries', '3G network in ldc']</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5168,6 +5803,11 @@
           <t>C100101</t>
         </is>
       </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>['economic equality', 'economic inequalities', 'equitable income growth', 'equitable distribution of income', 'equal payment', 'income equality', 'income inequality', 'equal income', 'payment inequality', 'payment equality', 'Inequalities based on income', 'Gini index', 'income disparities', 'distribution of real income']</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -5205,6 +5845,11 @@
           <t>C100201</t>
         </is>
       </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>['political inclusion', 'social inclusion', 'economic inclusion', 'social inequalities', 'political inequalities', 'Inequalities based on age', 'Inequalities based on disability', 'Inequalities based on sexual orientation', 'Inequalities based on race', 'Inequalities based on class', 'Inequalities based on ethnicity', 'Inequalities based on religion', 'race inequalities', 'class inequalities', 'ethnicity inequalities', 'religion inequalities', 'empower lower income earners', 'people living below 50 percent of median income', 'inclusion in society', 'inclusion of people with disabilities', 'support for people with disabilities', 'inclusion for all', 'inclusion of persons with disabilities', 'promote inclusion', 'participation of persons with disabilities', 'participation of people with disabilities', 'involvement of persons with disabilities']</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -5242,6 +5887,11 @@
           <t>C200204</t>
         </is>
       </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>['inequalities of outcome', 'discriminatory law', 'equal opportunity', 'discrimination', 'discriminatory practices', 'equality act', 'equality of outcome', 'equal treatment', 'inequalities of opportunity', 'disparities of opportunity', 'be discriminated', 'racism', 'homophobia', 'transphobia', 'religious intolerance', 'discriminatory policies', 'same opportunities for all', 'anti-discrimination legislation', 'accessibility non-discrimination', 'social cohesion']</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -5279,6 +5929,11 @@
           <t>C100401</t>
         </is>
       </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>['social protection policy', 'fiscal equality', 'social protection transfer', 'equality and social policy', 'social equality', 'wage equality', 'progress equality', 'advance equality', 'increase equality', 'improve equality', 'enhance equality', 'Redistributive impact of fiscal policy']</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -5316,6 +5971,11 @@
           <t>C100402</t>
         </is>
       </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>['social protection policy', 'fiscal equality', 'social protection transfer', 'equality and social policy', 'social equality', 'wage equality', 'progress equality', 'advance equality', 'increase equality', 'improve equality', 'enhance equality', 'Redistributive impact of fiscal policy']</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -5353,6 +6013,11 @@
           <t>C100501</t>
         </is>
       </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>['regulation of financial market', 'monitoring of financial market', 'regulation of financial institution', 'monitoring of financial institution', 'financial soundness', 'financial health', 'improve the regulation on income']</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -5390,6 +6055,11 @@
           <t>C200205</t>
         </is>
       </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>['decision power of developing countries', 'voting rights of developing countries', 'participation of developing countries', 'voice of developing countries', 'decision-making in developing countries', 'developing countries are better represented in decision-making', 'developing countries represented in decision-making', 'developing countries representation in decision-making', 'equal representation in international organizations']</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5427,6 +6097,11 @@
           <t>C100701</t>
         </is>
       </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>['safe migration', 'responsible migration', 'orderly migration', 'migration policies', 'manage migration', 'policies for migration', 'safe mobility of people', 'people who died or disappeared in the process of migration', 'died in migration', 'deaths in migration', 'deaths of migrants', 'irregular departures', 'migrant status', 'refugees', 'forced displacement', 'internally displaced people', 'migration partnerships', 'internally displaced persons', 'irregular migration', 'return and readmission', 'Regularised status', 'voluntary returns', 'border management', 'migration routes', 'resettlement', 'migration governance', 'migration management', 'asylum', 'assisted voluntary return', 'legal mobility', 'sustainable reintegration', 'border control', 'smuggling of migrants', 'migrant smuggling', 'host communities', 'diaspora']</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -5464,6 +6139,11 @@
           <t>C100702</t>
         </is>
       </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>['safe migration', 'responsible migration', 'orderly migration', 'migration policies', 'manage migration', 'policies for migration', 'safe mobility of people', 'people who died or disappeared in the process of migration', 'died in migration', 'deaths in migration', 'deaths of migrants', 'irregular departures', 'migrant status', 'refugees', 'forced displacement', 'internally displaced people', 'migration partnerships', 'internally displaced persons', 'irregular migration', 'return and readmission', 'Regularised status', 'voluntary returns', 'border management', 'migration routes', 'resettlement', 'migration governance', 'migration management', 'asylum', 'assisted voluntary return', 'legal mobility', 'sustainable reintegration', 'border control', 'smuggling of migrants', 'migrant smuggling', 'host communities', 'diaspora']</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -5501,6 +6181,11 @@
           <t>C100703</t>
         </is>
       </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>['safe migration', 'responsible migration', 'orderly migration', 'migration policies', 'manage migration', 'policies for migration', 'safe mobility of people', 'people who died or disappeared in the process of migration', 'died in migration', 'deaths in migration', 'deaths of migrants', 'irregular departures', 'migrant status', 'refugees', 'forced displacement', 'internally displaced people', 'migration partnerships', 'internally displaced persons', 'irregular migration', 'return and readmission', 'Regularised status', 'voluntary returns', 'border management', 'migration routes', 'resettlement', 'migration governance', 'migration management', 'asylum', 'assisted voluntary return', 'legal mobility', 'sustainable reintegration', 'border control', 'smuggling of migrants', 'migrant smuggling', 'host communities', 'diaspora']</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5538,6 +6223,11 @@
           <t>C100704</t>
         </is>
       </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>['safe migration', 'responsible migration', 'orderly migration', 'migration policies', 'manage migration', 'policies for migration', 'safe mobility of people', 'people who died or disappeared in the process of migration', 'died in migration', 'deaths in migration', 'deaths of migrants', 'irregular departures', 'migrant status', 'refugees', 'forced displacement', 'internally displaced people', 'migration partnerships', 'internally displaced persons', 'irregular migration', 'return and readmission', 'Regularised status', 'voluntary returns', 'border management', 'migration routes', 'resettlement', 'migration governance', 'migration management', 'asylum', 'assisted voluntary return', 'legal mobility', 'sustainable reintegration', 'border control', 'smuggling of migrants', 'migrant smuggling', 'host communities', 'diaspora']</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5575,6 +6265,11 @@
           <t>C100a01</t>
         </is>
       </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>['special treatment of developing countries', 'developing countries treated special', 'differential treatment for developing countries', 'developing countries special rights', 'special rights for developing countries', 'differential treatment provision', 'Tariff line for developing countries', 'Tariff line for least developed countries', 'Tariff line for LDCs', 'differential treatment for least developed countries', 'differential treatment for LDCs', 'tariff rates on goods coming from developing countries', 'tariff rates on goods from developing countries', 'tariff rates for developing countries', 'tariff rates for least developed countries', 'tariff rates for LDCs']</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5612,6 +6307,11 @@
           <t>C100b01</t>
         </is>
       </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>['development aid to neediest countries', 'aid to ldc', 'aid to developing', 'aid least developed', 'aid small island', 'assistance ldc', 'assistance small island', 'assistance least developed', 'direct investment developing countries', 'direct investment ldc', 'direct investment small island', 'direct investment least developed', 'fdi developing countries', 'fdi least developed', 'fdi ldc', 'fdi small island', 'resource flows for development', 'resource flows to developing countries', 'resource flows to least developed countries', 'resource flows to LDCs', 'development assistance', 'direct investment to regions where the need is greatest', 'official development assistance', 'ODA']</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5649,6 +6349,11 @@
           <t>C100c01</t>
         </is>
       </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>['remittance cost', 'remittance corridors', 'remittance transfer cost', 'remittance transaction cost', 'migrant remittances', 'remittances from migrants']</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -5686,6 +6391,11 @@
           <t>C110101</t>
         </is>
       </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>['access to housing', 'safe housing', 'adequate housing', 'affordable housing', 'inadequate housing', 'slum', 'informal settlements', 'live in informal area', 'right to housing', 'urban renewal', 'demand for housing', 'capacity building of the communal services', 'overburdened services', 'social housing']</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -5723,6 +6433,11 @@
           <t>C110201</t>
         </is>
       </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>['affordable transport', 'safe transport', 'accessible transport', 'public transport', 'sustainable transport', 'transport system', 'clean transport', 'clean mobility', 'clean urban mobility', 'electric transport', 'reshaping of the transport sector', 'rail transport network', 'climate resilient transportation infrastructure', 'efficient technologies for transportation', 'sustainable urban mobility', 'sustainable mobility', 'sustainable and smart mobility', 'multimodal mobility']</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -5760,6 +6475,11 @@
           <t>C110301</t>
         </is>
       </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>['inclusive urbanization', 'sustainable urbanization', 'urban planning', 'urban management', 'sustainable human settlement', 'urban development', 'city planning', 'sustainable cities', 'urban sustainability', 'participation in urban', 'participation and urban planning', 'citizen participation', 'urban social participation', 'urban participation', 'inclusion and civil society', 'inclusive cities', 'inclusive communities', 'sustainable communities', 'design of urban settlements', 'disadvantaged urban areas', 'new urban agenda', 'urban growth', 'urban transition', 'urban wellbeing', 'urban environment', 'better urban governance', 'urban centres as economic poles', 'sustainable urban expansion', 'urban spaces management', 'mega-cities pressure', 'local authorities planning', 'inclusive human settlement', 'safe human settlement', 'inclusive urbanisation', 'sustainable urbanisation']</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -5797,6 +6517,11 @@
           <t>C110302</t>
         </is>
       </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>['inclusive urbanization', 'sustainable urbanization', 'urban planning', 'urban management', 'sustainable human settlement', 'urban development', 'city planning', 'sustainable cities', 'urban sustainability', 'participation in urban', 'participation and urban planning', 'citizen participation', 'urban social participation', 'urban participation', 'inclusion and civil society', 'inclusive cities', 'inclusive communities', 'sustainable communities', 'design of urban settlements', 'disadvantaged urban areas', 'new urban agenda', 'urban growth', 'urban transition', 'urban wellbeing', 'urban environment', 'better urban governance', 'urban centres as economic poles', 'sustainable urban expansion', 'urban spaces management', 'mega-cities pressure', 'local authorities planning', 'inclusive human settlement', 'safe human settlement', 'inclusive urbanisation', 'sustainable urbanisation']</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -5834,6 +6559,11 @@
           <t>C110401</t>
         </is>
       </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>['cultural heritage', 'natural heritage', 'unesco world heritage', 'heritage protection', 'heritage conservation', 'heritage park']</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -5871,6 +6601,11 @@
           <t>C200303</t>
         </is>
       </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>['disaster related deaths', 'disaster related cost', 'flood victim', 'flood related cost', 'damage due to flooding', 'disaster resilience', 'disaster vulnerability', 'disaster damage', 'direct economic loss disaster', 'economic loss climate-related', 'economic loss natural disaster', 'disaster risk management', 'disaster risk reduction', 'disaster management', 'disaster preparedness', 'disaster mitigation', 'post-disaster response', 'disaster emergency action', 'DRR', ' Sendai Framework', 'economic cost of disasters']</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -5908,6 +6643,11 @@
           <t>C200211</t>
         </is>
       </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>['disaster related deaths', 'disaster related cost', 'flood victim', 'flood related cost', 'damage due to flooding', 'disaster resilience', 'disaster vulnerability', 'disaster damage', 'direct economic loss disaster', 'economic loss climate-related', 'economic loss natural disaster', 'disaster risk management', 'disaster risk reduction', 'disaster management', 'disaster preparedness', 'disaster mitigation', 'post-disaster response', 'disaster emergency action', 'DRR', ' Sendai Framework', 'economic cost of disasters']</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -5945,6 +6685,11 @@
           <t>C110503</t>
         </is>
       </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>['disaster related deaths', 'disaster related cost', 'flood victim', 'flood related cost', 'damage due to flooding', 'disaster resilience', 'disaster vulnerability', 'disaster damage', 'direct economic loss disaster', 'economic loss climate-related', 'economic loss natural disaster', 'disaster risk management', 'disaster risk reduction', 'disaster management', 'disaster preparedness', 'disaster mitigation', 'post-disaster response', 'disaster emergency action', 'DRR', ' Sendai Framework', 'economic cost of disasters']</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -5982,6 +6727,11 @@
           <t>C110603</t>
         </is>
       </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>['urban solid waste', 'urban waste', 'air pollution in cities', 'urban air pollution', 'air pollution in urban', 'particulate matter in cities', 'particulate matter in urban', 'smart waste management', 'improvements to air quality', 'waste management and recycling schemes', 'urban waste reduction', 'urban waste pickers', 'urban waste recycling', 'urbanization pressure', 'urban hazardous waste', 'municipal waste generation and management', 'municipal waste management', 'quality of the air we breathe', 'reduce air, water and noise pollution', 'zero-emission mobility', 'reduce congestion and pollution especially in urban areas']</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -6019,6 +6769,11 @@
           <t>C110602</t>
         </is>
       </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>['urban solid waste', 'urban waste', 'air pollution in cities', 'urban air pollution', 'air pollution in urban', 'particulate matter in cities', 'particulate matter in urban', 'smart waste management', 'improvements to air quality', 'waste management and recycling schemes', 'urban waste reduction', 'urban waste pickers', 'urban waste recycling', 'urbanization pressure', 'urban hazardous waste', 'municipal waste generation and management', 'municipal waste management', 'quality of the air we breathe', 'reduce air, water and noise pollution', 'zero-emission mobility', 'reduce congestion and pollution especially in urban areas']</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -6056,6 +6811,11 @@
           <t>C110701</t>
         </is>
       </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>['green space', 'inclusive public space', 'safe public space', 'open space in cities', 'urban parks', 'green urban development', 'green urban transition', 'Green urban spaces', 'Urban Greening Plans', 'accessible urban forests', 'accessible urban gardens', 'Greening urban']</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -6093,6 +6853,11 @@
           <t>C110702</t>
         </is>
       </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>['green space', 'inclusive public space', 'safe public space', 'open space in cities', 'urban parks', 'green urban development', 'green urban transition', 'Green urban spaces', 'Urban Greening Plans', 'accessible urban forests', 'accessible urban gardens', 'Greening urban']</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -6130,6 +6895,11 @@
           <t>C110a02</t>
         </is>
       </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>['regional planning', 'regional development plan', ' regional development strategy', 'urban development plan', ' urban development strategy', 'peri-urban area', 'sub urban area', 'urban rural interface', 'rural urban interface', 'regional programmes', 'improve regional management', 'regional network', 'regional development projects', 'regional integration', 'regional driving force', 'urban development at regional level', 'innovation at regional level', 'regional strategy', 'initiatives of regional importance', 'regional socioeconomic integration', 'regional and triangular cooperation potential', 'regional initiatives', 'community-driven solutions', 'global, regional and country-level action']</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -6167,6 +6937,11 @@
           <t>C200304</t>
         </is>
       </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>['urban disaster risk', 'disaster risk management in urban', 'disaster risk reduction in urban', 'disaster risk reduction strategy', 'urban inclusion', 'climate change adaptation urban', 'climate change adaptation plan urban', 'urban climate change adaptation', 'urban climate change mitigation', 'climate change mitigation urban', 'climate change mitigation plan urban', 'local disaster risk', 'disaster risk reducation plan', 'urban disaster resilience', 'foster inclusion in cities', 'fight inequalities in cities', 'facilitate inclusion in cities', 'tackle inequalities in cities']</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -6202,6 +6977,11 @@
       <c r="G156" t="inlineStr">
         <is>
           <t>C200305</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>['urban disaster risk', 'disaster risk management in urban', 'disaster risk reduction in urban', 'disaster risk reduction strategy', 'urban inclusion', 'climate change adaptation urban', 'climate change adaptation plan urban', 'urban climate change adaptation', 'urban climate change mitigation', 'climate change mitigation urban', 'climate change mitigation plan urban', 'local disaster risk', 'disaster risk reducation plan', 'urban disaster resilience', 'foster inclusion in cities', 'fight inequalities in cities', 'facilitate inclusion in cities', 'tackle inequalities in cities']</t>
         </is>
       </c>
     </row>
@@ -6233,6 +7013,11 @@
       <c r="G157" t="n">
         <v>0</v>
       </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>['support LDC in utilizing local building materials for sustainable buildings', 'support LDC in utilising local building materials for sustainable buildings', 'support ldc in sustainable building', 'support least developed countries in sustainable building', 'support developing countries in sustainable building', 'support ldc in resilient building', 'support least developed countries in resilient building', 'support developing countries in resilient building', 'support ldc in building sustainable', 'support least developed countries in building sustainable', 'support developing countries in building sustainable ', 'support ldc in building resilient', 'support least developed countries in building resilient', 'support developing countries in building resilient']</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -6270,6 +7055,11 @@
           <t>C120101</t>
         </is>
       </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>['SCP national action', 'SCP national plan', 'SCP national programme', 'Programmes on Sustainable Consumption and Production', 'sustainable consumption and production action plan', 'sustainable consumption and production in national plan', 'sustainable consumption and production in national policies', 'sustainable consumption action plan', 'sustainable consumption in national plan', 'sustainable consumption in national policies', 'sustainable production action plan', 'sustainable production in national plan', 'sustainable production in national policies', 'policy instruments aimed at supporting the shift to sustainable consumption and production', 'policy instruments to support the shift to sustainable consumption and production', 'policy instruments to support sustainable consumption and production', 'policy instruments for sustainable consumption and production', 'policy for sustainable consumption and production', 'policy to promote Sustainable Consumption and Production']</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -6307,6 +7097,11 @@
           <t>C200202</t>
         </is>
       </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>['sustainable resource use', 'sustainable resource management', 'natural resource efficiency', 'resource use efficiency', 'material footprint', 'efficient resource use', 'efficient use of resources', 'material consumption', 'use natural resources sustainably', 'use natural resources unsustainably', 'efficient management of natural resources', 'sustainable natural resource use', 'use resources sustainably', 'improve the resource efficiency', 'sustainable raw materials']</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -6344,6 +7139,11 @@
           <t>C200203</t>
         </is>
       </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>['sustainable resource use', 'sustainable resource management', 'natural resource efficiency', 'resource use efficiency', 'material footprint', 'efficient resource use', 'efficient use of resources', 'material consumption', 'use natural resources sustainably', 'use natural resources unsustainably', 'efficient management of natural resources', 'sustainable natural resource use', 'use resources sustainably', 'improve the resource efficiency', 'sustainable raw materials']</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -6381,6 +7181,11 @@
           <t>C120301</t>
         </is>
       </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>['food waste', 'food loss', 'post harvest loss', 'waste food', 'food lost in supply chains', 'reduce the environmental impact of the food processing']</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -6418,6 +7223,11 @@
           <t>C120401</t>
         </is>
       </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>['waste management', 'chemical waste', 'hazardous waste', 'hazardous chemical', 'waste treatment', 'management of chemicals', 'management of wastes', 'chemical release', 'chemicals pollution', 'waste pollution', 'hazardous pesticides', 'Persistent Organic Pollutants', 'toxic waste', 'solid waste', 'waste processing', 'waste collection']</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -6455,6 +7265,11 @@
           <t>C120402</t>
         </is>
       </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>['waste management', 'chemical waste', 'hazardous waste', 'hazardous chemical', 'waste treatment', 'management of chemicals', 'management of wastes', 'chemical release', 'chemicals pollution', 'waste pollution', 'hazardous pesticides', 'Persistent Organic Pollutants', 'toxic waste', 'solid waste', 'waste processing', 'waste collection']</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -6492,6 +7307,11 @@
           <t>C120501</t>
         </is>
       </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>['waste reduction', 'reduce waste', 'recycling', 'upcycling', 'reuse of resources', 'circular economy', 'waste-to-energy', 'resource reuse']</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -6529,6 +7349,11 @@
           <t>C120601</t>
         </is>
       </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>['sustainability reporting', 'company sustainability', 'sustainable business strategy', 'sustainability information', 'sustainability in companies']</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -6566,6 +7391,11 @@
           <t>C120702</t>
         </is>
       </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>['sustainable public procurement', 'green public procurement', 'sustainable procurement', 'green procurement', 'climate-friendly public procurement', 'climate-friendly procurement', 'GPP']</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -6603,6 +7433,11 @@
           <t>C200306</t>
         </is>
       </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>['education for sustainable development', 'climate change education', 'awareness for sustainable development', 'sustainability education', 'awareness sustainability', 'sustainability awareness', 'sustainability campaign', 'encourage sustainability', 'Ensure consumer information', 'adequate consumer information', 'sustainable lifestyle', 'sustainable way of life', 'sustainability in every day life', 'sustainable behaviour', 'lifestyles in harmony with nature', 'lifestyles in harmony with environment', 'lifestyles respect nature', 'lifestyles respect environment', 'sustainable consumer choices', 'adopt sustainable practices', 'empower consumers to make informed choices', 'enabling buyers to make sustainable decisions', 'give consumers better \ninformation', 'informed consumer choices']</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -6640,6 +7475,11 @@
           <t>C200208</t>
         </is>
       </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>['support developing countries sustainable', 'promote sustainability in developing countries', 'promote sustainable lifestyle in developing countries', 'sustainable consumption in developing countries', 'developing countries sustainable lifestyle', 'developing countries sustainable consumption', 'sustainable production developing countries', 'developing countries sustainable production']</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -6677,6 +7517,11 @@
           <t>C120b02</t>
         </is>
       </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>['sustainable tourism', 'tourism that promotes local culture', 'tourism that promotes local products', 'monitor the economic and environmental aspects of tourism', 'monitor the environmental impact of tourism', 'tourism policies', 'tourism sustainable']</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -6714,6 +7559,11 @@
           <t>C120c01</t>
         </is>
       </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>['fossil-fuel subsidies', 'carbon taxation', 'carbon tax', 'subsidies to fossil fuels', 'environmental cost of fossil fuel', 'fossil fuel tax']</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -6751,6 +7601,11 @@
           <t>C200303</t>
         </is>
       </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>['disaster risk reduction', 'climate resilience', 'climate-related hazards', 'climate vulnerability', 'vulnerability to climate change', 'cope with climate change', 'coping strategies climate change', 'climate change cope', 'climate change resilience', 'resilient climate change', 'climate change adaptation', 'climate change mitigation', 'climate governance', 'prevent the effects of climate change', 'addressing climate impact', 'climate mitigation', 'mitigate natural disasters', 'reduce the impact of natural disasters', 'adaptation to \nclimate change', 'climate adaptation', 'hydrogeological disasters', ' extreme weather', 'mitigate impacts of climate change', 'resilience to climate']</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -6788,6 +7643,11 @@
           <t>C200304</t>
         </is>
       </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>['disaster risk reduction', 'climate resilience', 'climate-related hazards', 'climate vulnerability', 'vulnerability to climate change', 'cope with climate change', 'coping strategies climate change', 'climate change cope', 'climate change resilience', 'resilient climate change', 'climate change adaptation', 'climate change mitigation', 'climate governance', 'prevent the effects of climate change', 'addressing climate impact', 'climate mitigation', 'mitigate natural disasters', 'reduce the impact of natural disasters', 'adaptation to \nclimate change', 'climate adaptation', 'hydrogeological disasters', ' extreme weather', 'mitigate impacts of climate change', 'resilience to climate']</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -6825,6 +7685,11 @@
           <t>C200305</t>
         </is>
       </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>['disaster risk reduction', 'climate resilience', 'climate-related hazards', 'climate vulnerability', 'vulnerability to climate change', 'cope with climate change', 'coping strategies climate change', 'climate change cope', 'climate change resilience', 'resilient climate change', 'climate change adaptation', 'climate change mitigation', 'climate governance', 'prevent the effects of climate change', 'addressing climate impact', 'climate mitigation', 'mitigate natural disasters', 'reduce the impact of natural disasters', 'adaptation to \nclimate change', 'climate adaptation', 'hydrogeological disasters', ' extreme weather', 'mitigate impacts of climate change', 'resilience to climate']</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -6862,6 +7727,11 @@
           <t>C130203</t>
         </is>
       </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>['climate change measures', 'national climate change adaptation', 'planning for climate change adaptation', 'climate change adaptation strategy', 'climate adaptation plan', 'climate adaptation strategy', 'nationally determined contribution', 'national adaptation plans', 'climate plan', 'climate action plan', 'climate change strategy', 'necp', 'Governance of the Energy Union and Climate Action', 'climate change policy', 'meet the goals of the Paris Agreement', 'climate related planning', 'addressing climate policy issues', 'plan for climate neutrality', 'strategy on climate action', 'national adaptation plans for responding to climate change', 'climate action to meet the goals of the Paris Climate Change Agreement', 'reducing greenhouse gas emissions', 'reduce GHG', 'Climate law', 'emissions reduction', 'Climate Pact', 'reduce emissions', 'climate-related policy', 'climate legislation', 'integrate climate change into risk management practices', 'climate objectives', 'net zero emissions', 'greenhouse gas emission reductions', 'policies contribute to climate', 'reduce carbon emissions', 'NDC', 'Emission Trading', 'MRV', 'mitigation strategies']</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -6899,6 +7769,11 @@
           <t>C130202</t>
         </is>
       </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>['climate change measures', 'national climate change adaptation', 'planning for climate change adaptation', 'climate change adaptation strategy', 'climate adaptation plan', 'climate adaptation strategy', 'nationally determined contribution', 'national adaptation plans', 'climate plan', 'climate action plan', 'climate change strategy', 'necp', 'Governance of the Energy Union and Climate Action', 'climate change policy', 'meet the goals of the Paris Agreement', 'climate related planning', 'addressing climate policy issues', 'plan for climate neutrality', 'strategy on climate action', 'national adaptation plans for responding to climate change', 'climate action to meet the goals of the Paris Climate Change Agreement', 'reducing greenhouse gas emissions', 'reduce GHG', 'Climate law', 'emissions reduction', 'Climate Pact', 'reduce emissions', 'climate-related policy', 'climate legislation', 'integrate climate change into risk management practices', 'climate objectives', 'net zero emissions', 'greenhouse gas emission reductions', 'policies contribute to climate', 'reduce carbon emissions', 'NDC', 'Emission Trading', 'MRV', 'mitigation strategies']</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -6936,6 +7811,11 @@
           <t>C200306</t>
         </is>
       </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>['climate change knowledge', 'climate change awareness', 'human capacity climate change', 'institutional capacity climate change', 'climate change mitigation capacity', 'climate change through education', 'improvement in climate change knowledge', 'climate change learning', 'learning climate change', 'education climate change', 'awareness climate change', 'awareness raising climate change', 'climate change curricula', 'research and innovation in climate', 'climate-related research', 'knowledge and understanding of climate change', ' knowledge of climate change', 'understanding of climate change', 'promote public awareness to address the effects of climate change', 'promote awareness to address climate change', 'climate change forum', 'better understand the risks posed by climate change', 'skills and attitudes on climate change']</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -6973,6 +7853,11 @@
           <t>C130a02</t>
         </is>
       </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>['green climate fund', 'climate related expending', 'funding climate change', 'financing climate change', 'development assistance to climate change', 'helping developing countries cut emissions', 'helping developing countries cope with climate impacts', 'green climate fund capitalization', 'address the needs of developing countries in the face of climate change', 'enable the climate finance', 'climate finance', 'Climate Change Fund', 'climate related investment', 'finance for climate action', 'investments on climate resilient', 'additional climate finance', 'green climate fund capitalisation']</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -7010,6 +7895,11 @@
           <t>C130b02</t>
         </is>
       </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>['climate change related planning in least developed', 'climate change related planning small island', 'raise capacity for effective climate change-related planning', ' raise capacity for effective climate change-related management', 'address the needs of developing countries to adapt to climate change', 'support developing countries in climate change', 'support small island developing states in climate change']</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -7047,6 +7937,11 @@
           <t>C140101</t>
         </is>
       </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>['marine pollution', 'nutrient pollution', 'marine debris', 'coastal eutrophication', 'plastic debris', 'deterioration of coastal waters', 'coastal waters pollution', 'coastal water eutrophication', 'plastic litter', 'threaten marine environment', 'threaten marine life', 'marine litter', 'Clean Oceans', 'plastic waste ocean', 'ocean plastic waste', 'plastic ocean', 'plastic discharges ocean', 'oil spills ocean', 'oil spills sea']</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -7084,6 +7979,11 @@
           <t>C140201</t>
         </is>
       </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>['healthy ocean', 'productive ocean', 'marine ecosystem', 'coastal ecosystem', 'marine biodiversity', 'sustainable management of oceanic and coastal fisheries', 'protect lives and livelihoods in coastal areas', 'integrated costal management', 'water management in the sea basin', 'sustainable marine environments', 'sustainable maritime transport', 'coastal biodiversity', 'loss of coastal habitats', 'marine key biodiversity areas', 'oceans must be conserved', 'sustainable development of water ecosystems', 'protection of water and marine resources', 'conserve seas', 'conserve marine resources', 'protect oceans', 'protect seas', 'protect marine resources', 'protecting coastal wetlands', 'sustainably managing marine areas', 'sustainably managing coastal areas', ' maritime ecosystems']</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -7121,6 +8021,11 @@
           <t>C140301</t>
         </is>
       </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>['ocean acidification', 'marine acidity', 'ocean acidity', 'marine acidification', 'acidification ocean', 'acidification marine', 'acidity marine', 'acidity ocean', 'ph of the ocean', 'ph of the earths ocean', 'oceans ph', 'ocean chemistry', 'ocean pollution', 'ocean warming', 'ocean heat', 'marine heatwaves']</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -7158,6 +8063,11 @@
           <t>C140401</t>
         </is>
       </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>['overfishing', 'fish stock', 'sustainable fishing', 'destructive fishing', 'unregulated fishing', 'unreported fishing', 'illegal fishing', 'poor fisheries management', 'overexploited fish stocks', 'depleted fisheries', 'reduce the adverse impacts of fishing', 'Fisheries Agreement', 'fish industry', 'sustainable fisheries', 'SFPA']</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -7195,6 +8105,11 @@
           <t>C140501</t>
         </is>
       </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>['marine protected area', 'marine protected sites', 'marine area conservation', 'conserve marine area', 'protect marine area', 'marine area protection', 'conserve coastal area', 'coastal area protection', 'protect coastal area', 'marine environment', 'international ocean policy', 'protect sea areas']</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -7232,6 +8147,11 @@
           <t>C140601</t>
         </is>
       </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>['fisheries subsidies', 'regulated fishing', 'subsidies fishing', 'fisheries law', 'fisheries management', 'add value locally to fisheries resources', 'sustainable ocean economy']</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -7269,6 +8189,11 @@
           <t>C140701</t>
         </is>
       </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>['small island developing States marine resource', 'small island developing States sustainable use of marine resource', 'sustainable fisheries in small island', 'marine resource management small island developing', 'marine resources small island developing', 'marine resource use small island developing', 'sustainable aquaculture small island developing', 'small islands sustainable management of marine resources']</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -7306,6 +8231,11 @@
           <t>C140a01</t>
         </is>
       </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>['ocean technology', 'research in marine technology', 'funds for marine technology', 'research and development in marine technology']</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -7343,6 +8273,11 @@
           <t>C140b01</t>
         </is>
       </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>['small scale fisher', 'artisanal fisher', 'small scale fisheries', 'small scale fishing', 'family based fishery', 'small scale coastal fishermen', 'small fisheries', ' small-medium fisheries']</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -7380,6 +8315,11 @@
           <t>C140c01</t>
         </is>
       </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>['ocean conservation', 'sustainable use of ocean', 'law of the sea', 'ocean related instrument', 'ocean related legislation', 'conservation of ocean', 'management of marine resource', 'ocean-related instruments for conservation and sustainable use', 'health of the ocean', 'ocean health', 'UNCLOS']</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -7417,6 +8357,11 @@
           <t>C150101</t>
         </is>
       </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>['conserve terrestrial', 'restoration of terrestrial', 'restore inland freshwater', 'conserve inland freshwater', 'protect terrestrial', ' inland freshwater ecosystem', 'terrestrial ecosystem', 'terrestrial biodiversity', 'freshwater biodiversity', 'protect tundra', 'protect taiga', 'protect temperate deciduous forest', ' protect tropical rainforest', 'protect grassland', 'forests in protected areas', 'Well-managed protected areas', 'management of protected areas', 'land protected', 'restore ecosystem', 'land areas protected', 'protect land area', 'ecosystems protected', 'ecosystem restoration', 'maintain ecosystem', 'enhance ecosystem', 'restore degraded ecosystems', 'health of ecosystems', 'grassland protection', 'enhance healthy ecosystems', 'Effectively manage all protected areas', 'ensure all use of ecosystems is sustainable', 'sustainable use of ecosystem', 'achieve good condition of ecosystems', 'protection of natural ecosystems', 'natural ecosystems protection', 'restore natural ecosystems', 'natural ecosystems restoration', 'preserving ecosystems', 'maintaining biodiversity', 'enhancing biodiversity', 'conservation landscapes', 'landscape approach', 'conserve savanna', 'Landscape protection', 'Landscape restoration', 'Sustainable landscape management', 'Sustainable landscape use', 'Landscape ecology', 'sustainable use of terrestrial ecosystems', 'protect savanna']</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -7454,6 +8399,11 @@
           <t>C150102</t>
         </is>
       </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>['conserve terrestrial', 'restoration of terrestrial', 'restore inland freshwater', 'conserve inland freshwater', 'protect terrestrial', ' inland freshwater ecosystem', 'terrestrial ecosystem', 'terrestrial biodiversity', 'freshwater biodiversity', 'protect tundra', 'protect taiga', 'protect temperate deciduous forest', ' protect tropical rainforest', 'protect grassland', 'forests in protected areas', 'Well-managed protected areas', 'management of protected areas', 'land protected', 'restore ecosystem', 'land areas protected', 'protect land area', 'ecosystems protected', 'ecosystem restoration', 'maintain ecosystem', 'enhance ecosystem', 'restore degraded ecosystems', 'health of ecosystems', 'grassland protection', 'enhance healthy ecosystems', 'Effectively manage all protected areas', 'ensure all use of ecosystems is sustainable', 'sustainable use of ecosystem', 'achieve good condition of ecosystems', 'protection of natural ecosystems', 'natural ecosystems protection', 'restore natural ecosystems', 'natural ecosystems restoration', 'preserving ecosystems', 'maintaining biodiversity', 'enhancing biodiversity', 'conservation landscapes', 'landscape approach', 'conserve savanna', 'Landscape protection', 'Landscape restoration', 'Sustainable landscape management', 'Sustainable landscape use', 'Landscape ecology', 'sustainable use of terrestrial ecosystems', 'protect savanna']</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -7491,6 +8441,11 @@
           <t>C150201</t>
         </is>
       </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>['deforestation', 'deforested area', 'illegal logging', 'reforestation', 'afforestation', 'sustainable forest', 'forest management', 'management of forest', 'clearing forest', 'forest clearing', 'sustainable use of forest', 'conserve forest', 'protect forest', 'loss of forests', 'forest loss', 'forest lost', 'forests under long-term management plans', 'forests management plans', 'forest policy', 'forest planning', 'forests conserved', 'forests restored', 'restore forests', 'forest protection', 'mantain forests', 'maintenance of forest', 'Increase the quantity of forests', 'forest areas covered by management plans', 'protect forest ecosystems', 'restore forest ecosystems', 'protect world’s forests', 'restore world’s forests', 'forest preservation', 'forestry', ' forest resources', 'forest cover', 'forest reserves', 'forest degradation', 'forestry sector', 'agroforestry', 'forest partnership', 'sustainable development of forests', 'FLEGT', "forest value chains'", 'Muraille Verte', 'great green wall', 'GGWSSI']</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -7528,6 +8483,11 @@
           <t>C150301</t>
         </is>
       </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>['degraded soil', 'degraded land', 'soil degradation', 'environmental degradation', 'land erosion', 'soil erosion', 'degraded area', 'erosive area', 'desertification', 'address the high fire risk', 'land affected by drought', 'land affected by floods', 'land restoration', 'degradation of drylands', 'restore land', 'reducing flood damage', 'restore soil ecosystems', 'land degradation', 'restore soil health', 'remediation of contaminated soil', 'organic soil', 'soil fertility', 'arable land', 'land use change']</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -7565,6 +8525,11 @@
           <t>C150401</t>
         </is>
       </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>['mountain ecosystem', 'conserve mountain area', 'mountain biodiversity', 'biodiversity mountain', 'mountain green cover index', 'montane ecosystem', 'mountain conservation', 'mountain area conservation', 'conservation mountain', 'mountain protected area', 'protect mountain', 'mgci']</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -7602,6 +8567,11 @@
           <t>C150402</t>
         </is>
       </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>['mountain ecosystem', 'conserve mountain area', 'mountain biodiversity', 'biodiversity mountain', 'mountain green cover index', 'montane ecosystem', 'mountain conservation', 'mountain area conservation', 'conservation mountain', 'mountain protected area', 'protect mountain', 'mgci']</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -7639,6 +8609,11 @@
           <t>C150501</t>
         </is>
       </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>['biodiversity loss', 'biodiversity degradation', 'red list index', 'natural habitat loss', 'natural habitat degradation', 'preserve natural habitat', 'natural habitat conservation', 'protect natural habitat', 'conserve natural habitat', 'restore biodiversity', 'protected species', 'species extinction', 'threatened species', 'species threatened with extinction', 'biodiversity at risk', 'loss of natural habitats', 'maintenance of biological diversity', 'biodiversity conservation', 'conserve biodiversity', 'extinction risk', 'risk of extinction', 'conservation of biological diversity', 'sustainable use of biological diversity', 'conserve wildlife habitats', 'restore wildlife habitats', 'conservation and sustainable use of biological diversity', 'biodiversity protection', 'biodiversity and nature protection', 'restore habitats and species', 'safeguard biodiversity', 'protect habitats and species', 'preserve biodiversity', 'sustain biodiversity', 'biodiversity-friendly', 'Red List species', 'high ecological value', 'Areas protected', 'protected areas', 'national parks', 'biological corridors', 'flagship species', 'iconic fauna', 'iconic species', 'IUCN red list', 'international union for conservation of nature', 'endangered species']</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -7676,6 +8651,11 @@
           <t>C150601</t>
         </is>
       </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>['fair and equitable sharing of genetic resources', 'access to genetic resources', 'utilize genetic resources', 'Genetic Resources and the Fair and Equitable Sharing of Benefits Arising from their Utilization', 'fair and equitable sharing of the benefits arising from the utilisation of genetic resource', 'Genetic resources preservation', 'preserve genetic resources', 'access and benefit-sharing of genetic resources', 'sustainably use genetic resources', 'safeguard genetic resources', 'nagoya protocol', 'utilise genetic resources']</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -7713,6 +8693,11 @@
           <t>C200206</t>
         </is>
       </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>['poaching', 'wildlife trafficking', 'traded wildlife', 'trafficking of protected species', 'illegal wildlife', 'poachers', 'animals illegally traded', 'plants illegally traded']</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -7750,6 +8735,11 @@
           <t>C150801</t>
         </is>
       </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>['invasive alien species', 'invasive species', 'invasive alien plant', 'invasive plant']</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -7787,6 +8777,11 @@
           <t>C150902</t>
         </is>
       </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>['ecosystem and biodiversity values integration', 'ecosystem service', 'ecosystem valuation', 'biodiversity valuation', 'value ecosystem', 'value biodiversity', 'biodiversity in local planning', 'biodiversity in local plans', 'biodiversity in national planning', 'biodiversity in national plans', 'biodiversity in development strategies', 'Plan for Biodiversity', 'strategy for biodiversity', "biodiversity's intrinsic value", 'integrate biodiversity into the development and implementation of policies', 'integrate biodiversity into policies', 'biodiversity restoration plans', 'Environmental capital']</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -7824,6 +8819,11 @@
           <t>C200210</t>
         </is>
       </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>['biodiversity funding', 'financing conservation', 'financing protected area', 'financing biodiversity', 'official development assistance to conservation of nature', 'ecosystem benefits', 'benefits ecosystem', 'biodiversity benefits', 'benefits biodiversity', 'financial resources to conserve biodiversity', 'financial resources to conserve ecosystems', 'financial resources for biodiversity', 'financial resources for ecosystems', 'financial mobilization for ecosystems', 'financial mobilisation for ecosystems', 'public expenditure on conservation of biodiversity', 'public expenditure on conservation of ecosystems', 'public expenditure for biodiversity', 'public expenditure for ecosystems', 'Official development assistance for biodiversity', 'finance mobilized from biodiversity', 'ODA for biodiversity', 'resources to developing countries for biodiversity', 'resources for global biodiversity', 'resources to support biodiversity', 'resources to support ecosystem', 'funds for biodiversity', 'financial flows to developing countries for biodiversity', 'financial flows for biodiversity']</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -7861,6 +8861,11 @@
           <t>C200210</t>
         </is>
       </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>['finance forest', 'funding forest', 'sustainable forest management funding', 'funding sustainable forest', 'funding forest conservation', 'funding conservation forest', 'redd+', 'finance conservation forest', 'forest management in developing countries', 'finance sustainable forest management', 'finance forest management']</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -7898,6 +8903,11 @@
           <t>C200206</t>
         </is>
       </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>['global wildlife', 'wildlife crime prevention', 'protect wildlife', 'support against poaching and trafficking of protected species', 'global support for efforts to combat poaching', 'global support for efforts to combat trafficking of protected species', 'global support to combat poaching', 'global support to combat trafficking of protected species', 'global support to protected species']</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -7935,6 +8945,11 @@
           <t>C160101</t>
         </is>
       </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>['homicide', 'conflict related death', 'physical violence', 'sexual violence', 'psychological violence', 'reduce violence', 'armed conflict', 'fleeing war', 'fleeing persecution', 'fleeing conflict', 'enforced disappearances', 'conflict and violence', 'reduce all forms of violence', 'end conflict', 'forcibly displaced', 'persecution', 'physical punishment', 'psychological aggression', 'victims of violence', 'local conflicts', 'religious conflict', 'violent extremism', 'violent groups']</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -7972,6 +8987,11 @@
           <t>C160102</t>
         </is>
       </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>['homicide', 'conflict related death', 'physical violence', 'sexual violence', 'psychological violence', 'reduce violence', 'armed conflict', 'fleeing war', 'fleeing persecution', 'fleeing conflict', 'enforced disappearances', 'conflict and violence', 'reduce all forms of violence', 'end conflict', 'forcibly displaced', 'persecution', 'physical punishment', 'psychological aggression', 'victims of violence', 'local conflicts', 'religious conflict', 'violent extremism', 'violent groups']</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -8009,6 +9029,11 @@
           <t>C160103</t>
         </is>
       </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>['homicide', 'conflict related death', 'physical violence', 'sexual violence', 'psychological violence', 'reduce violence', 'armed conflict', 'fleeing war', 'fleeing persecution', 'fleeing conflict', 'enforced disappearances', 'conflict and violence', 'reduce all forms of violence', 'end conflict', 'forcibly displaced', 'persecution', 'physical punishment', 'psychological aggression', 'victims of violence', 'local conflicts', 'religious conflict', 'violent extremism', 'violent groups']</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -8046,6 +9071,11 @@
           <t>C160105</t>
         </is>
       </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>['homicide', 'conflict related death', 'physical violence', 'sexual violence', 'psychological violence', 'reduce violence', 'armed conflict', 'fleeing war', 'fleeing persecution', 'fleeing conflict', 'enforced disappearances', 'conflict and violence', 'reduce all forms of violence', 'end conflict', 'forcibly displaced', 'persecution', 'physical punishment', 'psychological aggression', 'victims of violence', 'local conflicts', 'religious conflict', 'violent extremism', 'violent groups']</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -8083,6 +9113,11 @@
           <t>C160201</t>
         </is>
       </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>['children violence', 'abuse children', 'children abuse', 'children torture', 'child sexual abuse', 'sexual violence against children', 'sexual abuse of children', 'trafficking of children', 'child trafficking', 'torture of children', " children's rights", 'risk of the minor being a victim of human trafficking', 'trafficking of minors', "minor's trafficking", 'violence by caregivers', 'aggression by caregivers', 'violence by parents', 'aggression by parents', 'violence by mother', 'violence by father', 'calling a child offensive names', 'shaking the child', 'shaking the children', 'slapping child', 'slapping children', 'hitting child', 'hitting children', 'spanking child', 'spanking children', 'beating child', 'beating children', 'violence against children', 'violence against child', 'children in commercial sexual exploitation', 'sexual exploitation of children', 'child in commercial sexual exploitation', 'child in sexual exploitation', 'sexual exploitation of child', 'Child prostitution', 'child sexual slavery', 'children sexual exploitation', 'Children prostitution', 'children sexual slavery', 'violence in childhood']</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -8120,6 +9155,11 @@
           <t>C160202</t>
         </is>
       </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>['children violence', 'abuse children', 'children abuse', 'children torture', 'child sexual abuse', 'sexual violence against children', 'sexual abuse of children', 'trafficking of children', 'child trafficking', 'torture of children', " children's rights", 'risk of the minor being a victim of human trafficking', 'trafficking of minors', "minor's trafficking", 'violence by caregivers', 'aggression by caregivers', 'violence by parents', 'aggression by parents', 'violence by mother', 'violence by father', 'calling a child offensive names', 'shaking the child', 'shaking the children', 'slapping child', 'slapping children', 'hitting child', 'hitting children', 'spanking child', 'spanking children', 'beating child', 'beating children', 'violence against children', 'violence against child', 'children in commercial sexual exploitation', 'sexual exploitation of children', 'child in commercial sexual exploitation', 'child in sexual exploitation', 'sexual exploitation of child', 'Child prostitution', 'child sexual slavery', 'children sexual exploitation', 'Children prostitution', 'children sexual slavery', 'violence in childhood']</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -8157,6 +9197,11 @@
           <t>C160203</t>
         </is>
       </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>['children violence', 'abuse children', 'children abuse', 'children torture', 'child sexual abuse', 'sexual violence against children', 'sexual abuse of children', 'trafficking of children', 'child trafficking', 'torture of children', " children's rights", 'risk of the minor being a victim of human trafficking', 'trafficking of minors', "minor's trafficking", 'violence by caregivers', 'aggression by caregivers', 'violence by parents', 'aggression by parents', 'violence by mother', 'violence by father', 'calling a child offensive names', 'shaking the child', 'shaking the children', 'slapping child', 'slapping children', 'hitting child', 'hitting children', 'spanking child', 'spanking children', 'beating child', 'beating children', 'violence against children', 'violence against child', 'children in commercial sexual exploitation', 'sexual exploitation of children', 'child in commercial sexual exploitation', 'child in sexual exploitation', 'sexual exploitation of child', 'Child prostitution', 'child sexual slavery', 'children sexual exploitation', 'Children prostitution', 'children sexual slavery', 'violence in childhood']</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -8194,6 +9239,11 @@
           <t>C160301</t>
         </is>
       </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>['conflict resolution mechanism', 'unsentenced detainees', 'rule of law', 'access to justice', 'justice for all', 'equality of citizens', 'right to justice', 'law enforcement', 'reinforcing the law', 'ensure that international law is respected', 'assure justice', 'ensure justice', 'deliver justice', 'dispute resolution mechanism', 'respect for international law', 'judicial independence', 'improving justice', 'justice reform', 'impunity']</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -8231,6 +9281,11 @@
           <t>C160302</t>
         </is>
       </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>['conflict resolution mechanism', 'unsentenced detainees', 'rule of law', 'access to justice', 'justice for all', 'equality of citizens', 'right to justice', 'law enforcement', 'reinforcing the law', 'ensure that international law is respected', 'assure justice', 'ensure justice', 'deliver justice', 'dispute resolution mechanism', 'respect for international law', 'judicial independence', 'improving justice', 'justice reform', 'impunity']</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -8268,6 +9323,11 @@
           <t>C160303</t>
         </is>
       </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>['conflict resolution mechanism', 'unsentenced detainees', 'rule of law', 'access to justice', 'justice for all', 'equality of citizens', 'right to justice', 'law enforcement', 'reinforcing the law', 'ensure that international law is respected', 'assure justice', 'ensure justice', 'deliver justice', 'dispute resolution mechanism', 'respect for international law', 'judicial independence', 'improving justice', 'justice reform', 'impunity']</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -8305,6 +9365,11 @@
           <t>C160401</t>
         </is>
       </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>['illicit flow', 'illicit financial', 'illicit arm', 'stolen asset', 'organized crime', 'seized arms', 'surrendered arms', 'financial illicit', 'inward illicit', 'outward illicit', 'illicit origin', 'illegal arm', 'illegal weapons', 'transfer of firearms', 'organised crime', 'funding armed groups', 'Combating the Financing of Terrorism', 'money laundering', 'KYC/AML/CFT', 'illicit drugs', 'anti-fraud', 'fraud', 'measures against illegal activities', 'arms trafficking', 'trafficking of arms', 'drug trafficking', 'trafficking of drugs', 'anti-money laundering', 'countering the financing of terrorism']</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -8342,6 +9407,11 @@
           <t>C160402</t>
         </is>
       </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>['illicit flow', 'illicit financial', 'illicit arm', 'stolen asset', 'organized crime', 'seized arms', 'surrendered arms', 'financial illicit', 'inward illicit', 'outward illicit', 'illicit origin', 'illegal arm', 'illegal weapons', 'transfer of firearms', 'organised crime', 'funding armed groups', 'Combating the Financing of Terrorism', 'money laundering', 'KYC/AML/CFT', 'illicit drugs', 'anti-fraud', 'fraud', 'measures against illegal activities', 'arms trafficking', 'trafficking of arms', 'drug trafficking', 'trafficking of drugs', 'anti-money laundering', 'countering the financing of terrorism']</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -8379,6 +9449,11 @@
           <t>C160501</t>
         </is>
       </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>['corruption', 'bribery', 'bribe', 'anti-corruption', 'anticorruption']</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -8416,6 +9491,11 @@
           <t>C160502</t>
         </is>
       </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>['corruption', 'bribery', 'bribe', 'anti-corruption', 'anticorruption']</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -8453,6 +9533,11 @@
           <t>C160601</t>
         </is>
       </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>['transparent institutions', 'accountable public service', 'transparent public service', 'effective public services', 'quality public service', 'transparent public institutions', 'accountable public institutions', 'quality public institution', 'effective institutions', 'institutional capacity', 'public service quality', 'institutional transparency', 'institutional accountability', 'transparency in political process', 'transparency of political', 'enforce institutions', 'strong institutions', 'quality public administrations', 'effective governance', 'accountable institutions', 'inclusive institutions', 'institution more agile and flexible, as well as more transparent', 'greater transparency and democratic legitimacy', 'good governance', 'weak governance', 'governance review', 'Institutional Strengthening', 'strengthening public institutions', 'governance in public institutions', 'Public Sector Strengthening', 'strong governance', 'resilient governance', 'inclusive governance', 'transparent governance']</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -8490,6 +9575,11 @@
           <t>C160602</t>
         </is>
       </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>['transparent institutions', 'accountable public service', 'transparent public service', 'effective public services', 'quality public service', 'transparent public institutions', 'accountable public institutions', 'quality public institution', 'effective institutions', 'institutional capacity', 'public service quality', 'institutional transparency', 'institutional accountability', 'transparency in political process', 'transparency of political', 'enforce institutions', 'strong institutions', 'quality public administrations', 'effective governance', 'accountable institutions', 'inclusive institutions', 'institution more agile and flexible, as well as more transparent', 'greater transparency and democratic legitimacy', 'good governance', 'weak governance', 'governance review', 'Institutional Strengthening', 'strengthening public institutions', 'governance in public institutions', 'Public Sector Strengthening', 'strong governance', 'resilient governance', 'inclusive governance', 'transparent governance']</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -8527,6 +9617,11 @@
           <t>C160701</t>
         </is>
       </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>['inclusive decision', 'responsive decision making', 'participatory decision', 'representative decision making', 'social equality in decision making', 'inclusive public service', 'public service inclusion', 'participation public service', 'public service participation', 'integrity of the electoral process', 'fair elections', 'electoral infrastructure', 'integrity of elections', 'threats to election', 'representation of workers', 'participation in democratic life', 'inclusive participation', 'stronger role to the voice of the people', 'inclusive approach with participation of all stakeholders', 'effective participation', 'enabling environment for CSOs', 'enabling environment for civil society organisations', 'multi-party dialogue', 'intra-community dialogue', 'inter-community dialogue', 'intercultural dialogue', 'inter-faith dialogue', 'civic space', 'structured dialogue CSO', 'Civil Society Strengthening', 'election monitoring', 'election observation', 'monitoring of elections', 'observation of elections', 'progress in institutionalising electoral democracy', 'structured dialogue civil society organisations']</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -8564,6 +9659,11 @@
           <t>C160702</t>
         </is>
       </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>['inclusive decision', 'responsive decision making', 'participatory decision', 'representative decision making', 'social equality in decision making', 'inclusive public service', 'public service inclusion', 'participation public service', 'public service participation', 'integrity of the electoral process', 'fair elections', 'electoral infrastructure', 'integrity of elections', 'threats to election', 'representation of workers', 'participation in democratic life', 'inclusive participation', 'stronger role to the voice of the people', 'inclusive approach with participation of all stakeholders', 'effective participation', 'enabling environment for CSOs', 'enabling environment for civil society organisations', 'multi-party dialogue', 'intra-community dialogue', 'inter-community dialogue', 'intercultural dialogue', 'inter-faith dialogue', 'civic space', 'structured dialogue CSO', 'Civil Society Strengthening', 'election monitoring', 'election observation', 'monitoring of elections', 'observation of elections', 'progress in institutionalising electoral democracy', 'structured dialogue civil society organisations']</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -8601,6 +9701,11 @@
           <t>C200205</t>
         </is>
       </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>['participation developing countries', 'developing countries participating', 'global governance developing countries', 'developing countries in international organizations', 'inclusion developing countries', 'developing countries inclusion', 'developing countries in global governance']</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -8638,6 +9743,11 @@
           <t>C160901</t>
         </is>
       </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>['birth certificate', 'legal identity', 'legal registration and documentation of a person', 'undocumented people', 'birth registration', 'registered births', 'civil registration', 'children officially recorded', 'stateless', 'denied nationality', 'legally invisible', 'births were never registered', 'births not registered', 'Registration of birth', 'identity documentation', 'national identity cards', 'registration of civil status', 'civil registry', 'death registration']</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -8675,6 +9785,11 @@
           <t>C161001</t>
         </is>
       </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>['public access to information', 'information access', 'free media', 'free press', 'threaten journalist', 'torture journalist', 'kidnapping journalist', 'killing journalist', 'journalists under risk', 'human right advocate', 'disappearences of human rights defenders', 'disappearances of journalists', 'disappearances of trade unionists', 'human rights defenders death', 'journalists death', 'trade unionists death', 'torture of human rights defenders', 'torture of trade unionists', 'Freedom to express views', 'Freedom to express opinion', 'freedom of information', 'right to information', 'journalist freedom', 'rights based approach', 'fundamental freedom', 'protect individual freedom', 'disappearances of human rights activist', 'disappearances of human rights advocates', 'disappearances of activists', 'disappearances of whistleblowers']</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -8712,6 +9827,11 @@
           <t>C161002</t>
         </is>
       </c>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>['public access to information', 'information access', 'free media', 'free press', 'threaten journalist', 'torture journalist', 'kidnapping journalist', 'killing journalist', 'journalists under risk', 'human right advocate', 'disappearences of human rights defenders', 'disappearances of journalists', 'disappearances of trade unionists', 'human rights defenders death', 'journalists death', 'trade unionists death', 'torture of human rights defenders', 'torture of trade unionists', 'Freedom to express views', 'Freedom to express opinion', 'freedom of information', 'right to information', 'journalist freedom', 'rights based approach', 'fundamental freedom', 'protect individual freedom', 'disappearances of human rights activist', 'disappearances of human rights advocates', 'disappearances of activists', 'disappearances of whistleblowers']</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -8749,6 +9869,11 @@
           <t>C160a01</t>
         </is>
       </c>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>['Paris Principles', 'prevent violence', 'combat terrorism', 'combat crime', 'prevent crime', 'fight terrorism', 'counter terrorism', 'tackle terrorism', 'prosecute terrorism', 'address the threat of terrorist offences', 'terrorist offences and serious crime', 'prosecute terrorist offences', 'human rights institutions', 'institutions for human rights', 'NHRI', 'national human rights institutions', 'conflict management', 'security sector reforms', 'SSR', 'conflict sensitivity', 'Ministry of Defence', 'state and resilience building', 'European Peace Facility']</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -8786,6 +9911,11 @@
           <t>C200204</t>
         </is>
       </c>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>['non-discriminatory law', 'sustainable development policies', 'non discriminatory policies', 'human rights law', 'human rights politics', 'human rights policy', 'human rights council', 'discriminatory policies', 'discriminatory law', 'law against discrimination', 'Charter of Fundamental Rights', 'policy for human rights', 'law for human rights', 'policies without discrimination']</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -8823,6 +9953,11 @@
           <t>C170101</t>
         </is>
       </c>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>['domestic resource mobilization', 'domestic capacity', 'domestic tax', 'international support to developing countries', 'domestic budget', 'improve tax collection', 'increase tax collection', 'raise tax revenue', 'increase tax revenue', 'improve tax revenue', 'reform tax systems', 'domestic revenue resources', 'tax systems reform', 'financial flows to developing countries', 'revenue mobilisation', 'domestic revenue', 'Public Finance Management', 'PFM', 'Public Expenditure and Financial Accountability', 'PEFA', 'Tax Administration', 'tax transparency', 'tax collection', 'taxpayers', 'tax evasion', 'budget transparency', 'resources mobilization for sustainable development', 'resources mobilisation for sustainable development', 'domestic resource mobilisation', 'tax avoidance']</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -8860,6 +9995,11 @@
           <t>C170102</t>
         </is>
       </c>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>['domestic resource mobilization', 'domestic capacity', 'domestic tax', 'international support to developing countries', 'domestic budget', 'improve tax collection', 'increase tax collection', 'raise tax revenue', 'increase tax revenue', 'improve tax revenue', 'reform tax systems', 'domestic revenue resources', 'tax systems reform', 'financial flows to developing countries', 'revenue mobilisation', 'domestic revenue', 'Public Finance Management', 'PFM', 'Public Expenditure and Financial Accountability', 'PEFA', 'Tax Administration', 'tax transparency', 'tax collection', 'taxpayers', 'tax evasion', 'budget transparency', 'resources mobilization for sustainable development', 'resources mobilisation for sustainable development', 'domestic resource mobilisation', 'tax avoidance']</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -8897,6 +10037,11 @@
           <t>C170201</t>
         </is>
       </c>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>['official development assistance', 'oda', 'financial assistance over GNI', 'assistance for developing countries', 'international development cooperation', 'support developing countries', 'developing countries support']</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -8934,6 +10079,11 @@
           <t>C170304</t>
         </is>
       </c>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>['financial support to developing countries', 'finance developing countries', 'financial resources to developing countries', 'foreign direct investments to developing countries', 'remittances to developing countries', 'FDI do developing countries', 'developing countries remittances', 'developing countries financial support', 'developing countries receive financial support']</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -8971,6 +10121,11 @@
           <t>C170302</t>
         </is>
       </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>['financial support to developing countries', 'finance developing countries', 'financial resources to developing countries', 'foreign direct investments to developing countries', 'remittances to developing countries', 'FDI do developing countries', 'developing countries remittances', 'developing countries financial support', 'developing countries receive financial support']</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -9008,6 +10163,11 @@
           <t>C170401</t>
         </is>
       </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>['restructure debt in developing countries', 'reduce debt in developing countries', 'restructure debt in Africa', 'support developing countries with debt', 'help developing countries with debt', 'unsustainable debt levels developing countries', 'debt burden least developed countries', 'debt level reduction developing countries', 'debt relief for developing countries', 'debt moratorium developing countries', 'debt moratorium least deveveloped countries', 'debt burden on developing countries', 'help developing countries manage their debt', 'debt of developing countries', 'reduce debt distress in developing countries']</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -9045,6 +10205,11 @@
           <t>C170502</t>
         </is>
       </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>['investment promotion regime', 'foreign direct investment in the least developing countries', 'increased foreign direct investment flows', 'finance investment in developing countries', 'finance investment in last developing countries', 'address barriers to private investment in developing countries', 'supporting investment projects', 'foster investments in developing countries', 'public loans least developed countries', 'public loans developing countries', 'mobilisation of public and private investment developing countries', 'mitigate investment risks developing countries', 'promotion of private investments', 'investment climate in developing countries', 'foreign investors']</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -9082,6 +10247,11 @@
           <t>C170602</t>
         </is>
       </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>['technology cooperation agreement', 'global technology facilitation mechanism', 'Joint Technology Initiatives', 'Partnering in Research and Innovation', 'cooperation on technology', 'cooperation on science', 'cooperation on innovation', 'partnership in innovation', 'share innovation', 'share technology', 'knowledge-sharing', ' technology facilitation', ' technology cooperation', ' technology agreement', ' science cooperation', 'technology transfer', 'knowledege transfer', 'cooperation instruments and actions', 'GPEDC', 'Global Partnership for Effective Development Co-operation', 'collaboration on technology', 'collaboration on science', 'collaboration on innovation', 'partnerships in research', 'cooperation in research']</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -9119,6 +10289,11 @@
           <t>C170701</t>
         </is>
       </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>['technology in developing countries', 'technology dissemination in developing countries', 'technology diffusion in developing countries', 'developing countries technology', 'technology transfer in developing countries']</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -9156,6 +10331,11 @@
           <t>C170801</t>
         </is>
       </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>['technology in least developed countries', 'internet in least developed countries', 'ict in least developed countries', 'innovation in least developed countries', 'science capacity-building', 'technology capacity-building', 'innovation capacity-building', 'capacity-building in innovation', 'capacity-building in technology', 'capacity-building in science', 'international collaboration on technology', 'cooperation on information and communications technology', 'cooperation in ICT', 'collaboration information and communications technology', 'collaboration ICT', 'ICT cooperation', 'international information and communications technology', 'ICT capacity in least developed countries']</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -9193,6 +10373,11 @@
           <t>C170901</t>
         </is>
       </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t>['financial assistance to developing', 'technical assistance to developing', 'north south cooperation', 'south south cooperation', 'triangular cooperation', 'support capacity-building in developing countries', 'capacity building in least developed countries', 'national plans to implement the Sustainable Development Goals', 'national plans to implement the SDGs', 'national plans to implement Sustainable Development', 'cooperation on sustainable development', 'European Fund for Sustainable Development', 'capacity building assistance to improve the investment', 'EFSD', 'capacity building support in developing countries', 'support capacity building in developing countries']</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -9230,6 +10415,11 @@
           <t>C171001</t>
         </is>
       </c>
+      <c r="H238" t="inlineStr">
+        <is>
+          <t>['trade agreements for sustainable development', 'trade partnerships', 'trade relations around the world', 'progressive and modern trade rules', 'promote sustainable growth by expanding trade', 'rules for global trade', 'responsible trade', 'fair trade', 'transparent trade', 'ethical trade', 'sustainable trade', 'sustainable development in trade policies', 'rules with the global trade system', 'trade agenda to promote sustainable development', 'trade policy to sustainable development', 'trade to promote sustainable development', 'trade policy to promote the social and environmental pillars of sustainable development', 'trade and sustainable development', 'trade policy in support of sustainable development', 'Reinforced international regulatory cooperation helps to facilitate trade', 'Reinforce international regulatory cooperation for trade', 'regulatory trade cooperation', 'trade regulations', 'against unfair trade practices', 'responsible and fair trade', 'elimination of trade barriers', 'enforcing the rules of global trade', 'reinvigorate the WTO', 'rules governing global trade within the WTO', 'multilateral trading system', 'rules to govern global trade', 'open trading system', 'WTO-compatible trade agreements', 'promoting free trade', 'African Continental Free Trade Area', 'AfCFTA', 'fair and open trading system', 'trade barriers', 'EU’s trade interests', 'trade policy', 'trade facilitation', 'regional economic integration', 'Free Trade Area', 'trade facilitation in international regulatory cooperation', 'Economic Partnership Agreement']</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -9267,6 +10457,11 @@
           <t>C171101</t>
         </is>
       </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>['global export developing countries', 'global exports least developed countries', 'global exports share in developing countries', 'increase the exports of developing countries', 'increase the exports of least developed countries', 'increase the exports of Africa', 'increase the exports to improve the trade balance of developing countries', 'Export Strategy']</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -9304,6 +10499,11 @@
           <t>C171201</t>
         </is>
       </c>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>['tariffs faced by developing countries', 'tariffs faced by least developed countries', 'tariffs faced by small island developing countries', 'market access developing countries', 'market access least developed', 'market access small island', 'duty-free market access for least developed countries', 'quota-free market access for least developed countries', 'trade agreements with developing coutries', 'Aid for Trade Strategy', 'transparent trade rules', 'tariffs rules for developing countries', 'GSP+', 'everything but arms']</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -9341,6 +10541,11 @@
           <t>C171301</t>
         </is>
       </c>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>['macroeconomic dashboard', 'macroeconomic stability', 'policy coordination', 'economy with low vulnerability to external shocks', 'macroeconomic instability', 'macroeconomic policy coherence', 'macroeconomic coordination', 'macroeconomic situation', 'macro-economic stability']</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -9378,6 +10583,11 @@
           <t>C171401</t>
         </is>
       </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>['policy coherence for sustainable development', 'systematic promotion of mutually reinforcing policy actions', 'minimise contradictions and building synergies between different policies', 'coherent integration of policies', 'take account of development objectives in policies', 'PCD', 'PCSD', 'policy coherence for development']</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -9415,6 +10625,11 @@
           <t>C171501</t>
         </is>
       </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>['poverty eradication policies', 'sustainable development policies', 'respect sovereignty', 'promote ownership by countries', 'country-led policies for poverty eradication', 'country-led policies for sustainable development', 'policies tackle poverty', 'policies reduce poverty', 'policies foster sustainable development', 'policies focus on sustainable development', 'policies focus on poverty reduction']</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -9452,6 +10667,11 @@
           <t>C171601</t>
         </is>
       </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>['multi stakeholder partnership', 'multi stakeholder development', 'partnership for sustainable development', 'partnership for SDGs', 'multi-stakeholder alliances', 'platform for a multi-stakeholder dialogue on sustainable', 'multi-stakeholder dialogue platform', 'multi stakeholder platform']</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -9489,6 +10709,11 @@
           <t>C171702</t>
         </is>
       </c>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>['public private partnership', 'civil society partnership', 'public partnership', 'partnership with private sector', 'cooperation with private sector', 'public and private cooperation', 'cooperation with SME', 'partnership with SME', 'SME cooperation across developing countries', 'private sector for sustainable development', 'integrate private sector development objectives in support strategies', 'Engaging the private sector in sustainable', 'private sector engagement for development', 'engagement of European companies in developing countries', 'private sector development support', 'PRIVATE SECTOR PARTNER IN DEVELOPMENT COOPERATION', 'partnership and cooperation agreement between private and public', 'working in partnership with the EU in the field of private sector development', 'foster business innovation partnerships between private and public sector', 'exploring possible partnerships with the private sector', 'boosting horizontal partnerships', 'partnership public private', 'partnership private and public', 'tap into private investment', 'Public-Private Dialogue', 'Roadmap for Civil Society']</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -9526,6 +10751,11 @@
           <t>C171804</t>
         </is>
       </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>['availability of disaggregated data', 'fundamental principles of official statistics', 'sustainable development indicators', 'national statistical legislation', 'availability of reliable data', 'data availability in developing countries', 'data accountability developing countries', ' availability of data in developing countries', 'availability of data disaggregated', 'data at national level', ' statistics on sustainable development', 'national statistical plan', 'partnerships in data collection', 'data collection in development countries', ' collect data in development countries', ' collect information in development countries', 'Information gathering in development countries', 'indicators for sustainable development', 'official statistics in developing countries', 'weak statistical systems and mechanisms ', 'advocate for more and better data in developing countries']</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -9563,6 +10793,11 @@
           <t>C171802</t>
         </is>
       </c>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>['availability of disaggregated data', 'fundamental principles of official statistics', 'sustainable development indicators', 'national statistical legislation', 'availability of reliable data', 'data availability in developing countries', 'data accountability developing countries', ' availability of data in developing countries', 'availability of data disaggregated', 'data at national level', ' statistics on sustainable development', 'national statistical plan', 'partnerships in data collection', 'data collection in development countries', ' collect data in development countries', ' collect information in development countries', 'Information gathering in development countries', 'indicators for sustainable development', 'official statistics in developing countries', 'weak statistical systems and mechanisms ', 'advocate for more and better data in developing countries']</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -9600,6 +10835,11 @@
           <t>C171803</t>
         </is>
       </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>['availability of disaggregated data', 'fundamental principles of official statistics', 'sustainable development indicators', 'national statistical legislation', 'availability of reliable data', 'data availability in developing countries', 'data accountability developing countries', ' availability of data in developing countries', 'availability of data disaggregated', 'data at national level', ' statistics on sustainable development', 'national statistical plan', 'partnerships in data collection', 'data collection in development countries', ' collect data in development countries', ' collect information in development countries', 'Information gathering in development countries', 'indicators for sustainable development', 'official statistics in developing countries', 'weak statistical systems and mechanisms ', 'advocate for more and better data in developing countries']</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -9637,6 +10877,11 @@
           <t>C171901</t>
         </is>
       </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>['statistical capacity in developing countries', 'birth registration', 'death registration', 'population census', 'income census', 'measure progress SDG', 'sdg progress measure', 'statistical capacity in least developed countries', 'statistical capacity in small island', 'measurement of progress on sustainable development', 'statistical capacity-building', 'statistical capacity development', 'statistical capacity building', 'statistical capacity indicator', 'data on statistical capacity', 'data on sustainable development', 'data that complement gross domestic product', 'data that complement GDP', 'Beyond GDP', 'indicators to complement GDP', 'measure sustainable development', 'international cooperation on data collection', 'Monitoring sustainable development', 'evaluating sustainable development', 'assess sustainable development', 'statistical capacity development at the national level for developing countries', 'national statistical systems of developing countries', 'international funding for data and statistics', 'strengthening of the statistical system', 'monitoring of SDGs', 'reporting on SDGs', 'SDG monitoring', 'SDG reporting']</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -9672,6 +10917,11 @@
       <c r="G250" t="inlineStr">
         <is>
           <t>C171902</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>['statistical capacity in developing countries', 'birth registration', 'death registration', 'population census', 'income census', 'measure progress SDG', 'sdg progress measure', 'statistical capacity in least developed countries', 'statistical capacity in small island', 'measurement of progress on sustainable development', 'statistical capacity-building', 'statistical capacity development', 'statistical capacity building', 'statistical capacity indicator', 'data on statistical capacity', 'data on sustainable development', 'data that complement gross domestic product', 'data that complement GDP', 'Beyond GDP', 'indicators to complement GDP', 'measure sustainable development', 'international cooperation on data collection', 'Monitoring sustainable development', 'evaluating sustainable development', 'assess sustainable development', 'statistical capacity development at the national level for developing countries', 'national statistical systems of developing countries', 'international funding for data and statistics', 'strengthening of the statistical system', 'monitoring of SDGs', 'reporting on SDGs', 'SDG monitoring', 'SDG reporting']</t>
         </is>
       </c>
     </row>

</xml_diff>